<commit_message>
update including web scraping
</commit_message>
<xml_diff>
--- a/PositionInfo/full_Port.xlsx
+++ b/PositionInfo/full_Port.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="24000" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="24000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Id" sheetId="33" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="421">
   <si>
     <t>Name</t>
   </si>
@@ -1226,9 +1226,6 @@
   </si>
   <si>
     <t>VaR_bootstrap</t>
-  </si>
-  <si>
-    <t>VaR_Share</t>
   </si>
   <si>
     <t>component_VaR</t>
@@ -1697,7 +1694,7 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="104">
+  <dxfs count="103">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1963,25 +1960,6 @@
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0000%"/>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="169" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -21307,123 +21285,122 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="RiskTab22" displayName="RiskTab22" ref="A1:N78" totalsRowShown="0" headerRowDxfId="103" dataDxfId="101" headerRowBorderDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="RiskTab22" displayName="RiskTab22" ref="A1:N78" totalsRowShown="0" headerRowDxfId="102" dataDxfId="100" headerRowBorderDxfId="101">
   <tableColumns count="14">
-    <tableColumn id="1" name="Nr." dataDxfId="100" totalsRowDxfId="99"/>
-    <tableColumn id="12" name="Category" totalsRowDxfId="98"/>
-    <tableColumn id="9" name="ShortName" totalsRowDxfId="97"/>
-    <tableColumn id="24" name="Name" dataDxfId="96" totalsRowDxfId="95"/>
-    <tableColumn id="32" name="AlphaVantage" dataDxfId="94" totalsRowDxfId="93"/>
-    <tableColumn id="6" name="AV.length" dataDxfId="92" totalsRowDxfId="91"/>
-    <tableColumn id="10" name="AV.time" dataDxfId="90" totalsRowDxfId="89"/>
-    <tableColumn id="11" name="AV.down" dataDxfId="88" totalsRowDxfId="87"/>
-    <tableColumn id="5" name="barchart" dataDxfId="86" totalsRowDxfId="85"/>
-    <tableColumn id="7" name="barchart.length" dataDxfId="84" totalsRowDxfId="83"/>
-    <tableColumn id="2" name="Bloomberg" dataDxfId="82" totalsRowDxfId="81"/>
-    <tableColumn id="8" name="bloomberg.length" dataDxfId="80" totalsRowDxfId="79"/>
-    <tableColumn id="3" name="ISIN" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="4" name="WKN" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="1" name="Nr." dataDxfId="99" totalsRowDxfId="98"/>
+    <tableColumn id="12" name="Category" totalsRowDxfId="97"/>
+    <tableColumn id="9" name="ShortName" totalsRowDxfId="96"/>
+    <tableColumn id="24" name="Name" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="32" name="AlphaVantage" dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="6" name="AV.length" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="10" name="AV.time" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="11" name="AV.down" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="5" name="barchart" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="7" name="barchart.length" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="2" name="Bloomberg" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="8" name="bloomberg.length" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="3" name="ISIN" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="4" name="WKN" dataDxfId="75" totalsRowDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2" displayName="Table2" ref="A1:R78" totalsRowShown="0" headerRowDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2" displayName="Table2" ref="A1:R78" totalsRowShown="0" headerRowDxfId="73">
   <autoFilter ref="A1:R78"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="Nr." dataDxfId="73">
+    <tableColumn id="1" name="Nr." dataDxfId="72">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Nr.]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Category" dataDxfId="72">
+    <tableColumn id="16" name="Category" dataDxfId="71">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Category]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="71">
+    <tableColumn id="2" name="Name" dataDxfId="70">
       <calculatedColumnFormula>RiskTab22[[#This Row],[ShortName]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="AlphaVantage" dataDxfId="70">
+    <tableColumn id="13" name="AlphaVantage" dataDxfId="69">
       <calculatedColumnFormula>RiskTab22[[#This Row],[AlphaVantage]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Volume" dataDxfId="69">
+    <tableColumn id="3" name="Volume" dataDxfId="68">
       <calculatedColumnFormula>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="ClosePrice" dataDxfId="68"/>
-    <tableColumn id="14" name="CloseDate" dataDxfId="67"/>
-    <tableColumn id="5" name="Value" dataDxfId="66"/>
-    <tableColumn id="6" name="SharePortfolio" dataDxfId="65"/>
-    <tableColumn id="7" name="1D.logReturn" dataDxfId="64"/>
-    <tableColumn id="15" name="1D.logRetorn.on.portfolio" dataDxfId="63">
+    <tableColumn id="4" name="ClosePrice" dataDxfId="67"/>
+    <tableColumn id="14" name="CloseDate" dataDxfId="66"/>
+    <tableColumn id="5" name="Value" dataDxfId="65"/>
+    <tableColumn id="6" name="SharePortfolio" dataDxfId="64"/>
+    <tableColumn id="7" name="1D.logReturn" dataDxfId="63"/>
+    <tableColumn id="15" name="1D.logRetorn.on.portfolio" dataDxfId="62">
       <calculatedColumnFormula>Table2[[#This Row],[1D.logReturn]]*Table2[[#This Row],[Value]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="1D.return" dataDxfId="62"/>
-    <tableColumn id="9" name="5D.logReturn" dataDxfId="61"/>
-    <tableColumn id="10" name="23D.logReturn" dataDxfId="60"/>
-    <tableColumn id="11" name="125D.logReturn" dataDxfId="59"/>
-    <tableColumn id="12" name="250D.logReturn" dataDxfId="58"/>
-    <tableColumn id="17" name="curr.1D.logReturn" dataDxfId="57"/>
-    <tableColumn id="18" name="curr.Date" dataDxfId="56"/>
+    <tableColumn id="8" name="1D.return" dataDxfId="61"/>
+    <tableColumn id="9" name="5D.logReturn" dataDxfId="60"/>
+    <tableColumn id="10" name="23D.logReturn" dataDxfId="59"/>
+    <tableColumn id="11" name="125D.logReturn" dataDxfId="58"/>
+    <tableColumn id="12" name="250D.logReturn" dataDxfId="57"/>
+    <tableColumn id="17" name="curr.1D.logReturn" dataDxfId="56"/>
+    <tableColumn id="18" name="curr.Date" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table22" displayName="Table22" ref="A1:AO78" totalsRowShown="0" headerRowDxfId="55">
-  <autoFilter ref="A1:AO78"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table22" displayName="Table22" ref="A1:AN78" totalsRowShown="0" headerRowDxfId="54">
+  <autoFilter ref="A1:AN78"/>
   <sortState ref="A2:Y82">
     <sortCondition descending="1" ref="J1:J75"/>
   </sortState>
-  <tableColumns count="41">
-    <tableColumn id="1" name="Nr." dataDxfId="54">
+  <tableColumns count="40">
+    <tableColumn id="1" name="Nr." dataDxfId="53">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Nr.]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" name="Category" dataDxfId="53">
+    <tableColumn id="41" name="Category" dataDxfId="52">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Category]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="52">
+    <tableColumn id="2" name="Name" dataDxfId="51">
       <calculatedColumnFormula>RiskTab22[[#This Row],[ShortName]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="AlphaVantage" dataDxfId="51">
+    <tableColumn id="13" name="AlphaVantage" dataDxfId="50">
       <calculatedColumnFormula>RiskTab22[[#This Row],[AlphaVantage]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Value" dataDxfId="50">
+    <tableColumn id="21" name="Value" dataDxfId="49">
       <calculatedColumnFormula>Table2[[#This Row],[Volume]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="SharePortfolio" dataDxfId="49"/>
-    <tableColumn id="14" name="CloseDate" dataDxfId="48"/>
-    <tableColumn id="3" name="Beta1Y" dataDxfId="47"/>
-    <tableColumn id="18" name="Beta" dataDxfId="46"/>
-    <tableColumn id="19" name="250D.logReturn" dataDxfId="45">
+    <tableColumn id="24" name="SharePortfolio" dataDxfId="48"/>
+    <tableColumn id="14" name="CloseDate" dataDxfId="47"/>
+    <tableColumn id="3" name="Beta1Y" dataDxfId="46"/>
+    <tableColumn id="18" name="Beta" dataDxfId="45"/>
+    <tableColumn id="19" name="250D.logReturn" dataDxfId="44">
       <calculatedColumnFormula>Table2[[#This Row],[250D.logReturn]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="250D.CAPM.Return" dataDxfId="44"/>
-    <tableColumn id="22" name="Jensen.Alpha" dataDxfId="43">
+    <tableColumn id="20" name="250D.CAPM.Return" dataDxfId="43"/>
+    <tableColumn id="22" name="Jensen.Alpha" dataDxfId="42">
       <calculatedColumnFormula>Table22[[#This Row],[250D.logReturn]]-Table22[[#This Row],[std_log_returns_1Y]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="std_log_returns_1Y" dataDxfId="42"/>
-    <tableColumn id="5" name="std_log_returns" dataDxfId="41"/>
-    <tableColumn id="37" name="VolaN1_MSGARCH" dataDxfId="40"/>
-    <tableColumn id="6" name="VaR Normal std1Y" dataDxfId="39"/>
-    <tableColumn id="7" name="VaR Normal" dataDxfId="38"/>
-    <tableColumn id="8" name="VaR HS 1Y" dataDxfId="37"/>
-    <tableColumn id="9" name="individual VaR Bootstrap" dataDxfId="36"/>
-    <tableColumn id="10" name="marginal VaR in €" dataDxfId="35"/>
-    <tableColumn id="11" name="incremental VaR" dataDxfId="34"/>
-    <tableColumn id="23" name="incremental VaR to Port VaR (share Portfolio VaR)" dataDxfId="33"/>
-    <tableColumn id="12" name="incremental VaR per Value" dataDxfId="32"/>
-    <tableColumn id="15" name="share Portfolio VaR / share portfolio" dataDxfId="31"/>
-    <tableColumn id="26" name="VaR bootstrap 05Quantile" dataDxfId="30"/>
-    <tableColumn id="25" name="VaR bootstrap 95Quantile" dataDxfId="29"/>
-    <tableColumn id="34" name="VaR_bootstrap" dataDxfId="28"/>
-    <tableColumn id="39" name="ind_VaR_MSGARCH" dataDxfId="27"/>
-    <tableColumn id="33" name="incVaR bootstrap 05Quantile" dataDxfId="26"/>
-    <tableColumn id="32" name="incVaR bootstrap 95Quantile" dataDxfId="25"/>
-    <tableColumn id="31" name="incVaR bootstrap" dataDxfId="24"/>
-    <tableColumn id="30" name="mVaR bootstrap 05Quantile" dataDxfId="23"/>
-    <tableColumn id="29" name="mVaR bootstrap 95Quantile" dataDxfId="22"/>
-    <tableColumn id="16" name="mVaR bootstrap" dataDxfId="21"/>
-    <tableColumn id="27" name="component_VaR" dataDxfId="20"/>
-    <tableColumn id="36" name="VaR_Share" dataDxfId="19"/>
+    <tableColumn id="4" name="std_log_returns_1Y" dataDxfId="41"/>
+    <tableColumn id="5" name="std_log_returns" dataDxfId="40"/>
+    <tableColumn id="37" name="VolaN1_MSGARCH" dataDxfId="39"/>
+    <tableColumn id="6" name="VaR Normal std1Y" dataDxfId="38"/>
+    <tableColumn id="7" name="VaR Normal" dataDxfId="37"/>
+    <tableColumn id="8" name="VaR HS 1Y" dataDxfId="36"/>
+    <tableColumn id="9" name="individual VaR Bootstrap" dataDxfId="35"/>
+    <tableColumn id="10" name="marginal VaR in €" dataDxfId="34"/>
+    <tableColumn id="11" name="incremental VaR" dataDxfId="33"/>
+    <tableColumn id="23" name="incremental VaR to Port VaR (share Portfolio VaR)" dataDxfId="32"/>
+    <tableColumn id="12" name="incremental VaR per Value" dataDxfId="31"/>
+    <tableColumn id="15" name="share Portfolio VaR / share portfolio" dataDxfId="30"/>
+    <tableColumn id="26" name="VaR bootstrap 05Quantile" dataDxfId="29"/>
+    <tableColumn id="25" name="VaR bootstrap 95Quantile" dataDxfId="28"/>
+    <tableColumn id="34" name="VaR_bootstrap" dataDxfId="27"/>
+    <tableColumn id="39" name="ind_VaR_MSGARCH" dataDxfId="26"/>
+    <tableColumn id="33" name="incVaR bootstrap 05Quantile" dataDxfId="25"/>
+    <tableColumn id="32" name="incVaR bootstrap 95Quantile" dataDxfId="24"/>
+    <tableColumn id="31" name="incVaR bootstrap" dataDxfId="23"/>
+    <tableColumn id="30" name="mVaR bootstrap 05Quantile" dataDxfId="22"/>
+    <tableColumn id="29" name="mVaR bootstrap 95Quantile" dataDxfId="21"/>
+    <tableColumn id="16" name="mVaR bootstrap" dataDxfId="20"/>
+    <tableColumn id="27" name="component_VaR" dataDxfId="19"/>
     <tableColumn id="38" name="MSGARCH_prob" dataDxfId="18"/>
     <tableColumn id="40" name="ES_MSGARCH" dataDxfId="17"/>
     <tableColumn id="17" name="ES bootstrap 05Quantile" dataDxfId="16"/>
@@ -21765,7 +21742,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>29</v>
@@ -21809,7 +21786,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C2" t="s">
         <v>193</v>
@@ -21841,7 +21818,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C3" t="s">
         <v>196</v>
@@ -21873,16 +21850,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C4" t="s">
+        <v>410</v>
+      </c>
+      <c r="D4" s="49" t="s">
         <v>409</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" s="1" t="s">
         <v>411</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>410</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>412</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="8"/>
@@ -21899,7 +21876,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C5" t="s">
         <v>199</v>
@@ -21908,7 +21885,7 @@
         <v>200</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F5" s="9">
         <v>443</v>
@@ -21937,7 +21914,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C6" t="s">
         <v>203</v>
@@ -21971,16 +21948,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="8"/>
@@ -21997,7 +21974,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C8" t="s">
         <v>206</v>
@@ -22031,10 +22008,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>209</v>
@@ -22065,7 +22042,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C10" t="s">
         <v>211</v>
@@ -22103,7 +22080,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C11" t="s">
         <v>216</v>
@@ -22135,16 +22112,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C12" t="s">
+        <v>388</v>
+      </c>
+      <c r="D12" s="49" t="s">
         <v>389</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="E12" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="8"/>
@@ -22161,7 +22138,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C13" t="s">
         <v>219</v>
@@ -22193,7 +22170,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C14" t="s">
         <v>222</v>
@@ -22225,7 +22202,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C15" t="s">
         <v>225</v>
@@ -22263,7 +22240,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C16" t="s">
         <v>230</v>
@@ -22301,7 +22278,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C17" t="s">
         <v>235</v>
@@ -22335,7 +22312,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C18" t="s">
         <v>238</v>
@@ -22369,16 +22346,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C19" t="s">
+        <v>391</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>391</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="D19" s="49" t="s">
-        <v>392</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>393</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="8"/>
@@ -22395,16 +22372,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C20" t="s">
+        <v>413</v>
+      </c>
+      <c r="D20" s="49" t="s">
+        <v>412</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="D20" s="49" t="s">
-        <v>413</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>415</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="8"/>
@@ -22421,7 +22398,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C21" t="s">
         <v>241</v>
@@ -22459,7 +22436,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C22" t="s">
         <v>246</v>
@@ -22497,7 +22474,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C23" t="s">
         <v>251</v>
@@ -22537,7 +22514,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C24" t="s">
         <v>257</v>
@@ -22575,10 +22552,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C25" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>262</v>
@@ -22607,7 +22584,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C26" t="s">
         <v>264</v>
@@ -22645,7 +22622,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C27" t="s">
         <v>269</v>
@@ -22677,10 +22654,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C28" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>272</v>
@@ -22709,7 +22686,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C29" t="s">
         <v>274</v>
@@ -22745,7 +22722,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C30" t="s">
         <v>279</v>
@@ -22783,7 +22760,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C31" t="s">
         <v>284</v>
@@ -22821,7 +22798,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C32" t="s">
         <v>289</v>
@@ -22859,7 +22836,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C33" t="s">
         <v>294</v>
@@ -22893,7 +22870,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C34" t="s">
         <v>297</v>
@@ -22931,7 +22908,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C35" t="s">
         <v>302</v>
@@ -22969,7 +22946,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C36" t="s">
         <v>307</v>
@@ -23007,7 +22984,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C37" t="s">
         <v>312</v>
@@ -23045,7 +23022,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C38" t="s">
         <v>317</v>
@@ -23083,7 +23060,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C39" t="s">
         <v>322</v>
@@ -23121,7 +23098,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C40" t="s">
         <v>327</v>
@@ -23155,7 +23132,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C41" t="s">
         <v>330</v>
@@ -23193,7 +23170,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C42" t="s">
         <v>335</v>
@@ -23231,7 +23208,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C43" t="s">
         <v>340</v>
@@ -23269,7 +23246,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C44" t="s">
         <v>345</v>
@@ -23307,7 +23284,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C45" t="s">
         <v>348</v>
@@ -23341,7 +23318,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C46" t="s">
         <v>351</v>
@@ -23375,7 +23352,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C47" t="s">
         <v>354</v>
@@ -23409,7 +23386,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C48" t="s">
         <v>357</v>
@@ -23441,7 +23418,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C49" t="s">
         <v>360</v>
@@ -23473,7 +23450,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C50" t="s">
         <v>363</v>
@@ -23505,7 +23482,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C51" t="s">
         <v>366</v>
@@ -23537,7 +23514,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C52" t="s">
         <v>369</v>
@@ -23569,10 +23546,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C53" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D53" t="s">
         <v>372</v>
@@ -23601,7 +23578,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C54" t="s">
         <v>374</v>
@@ -23633,7 +23610,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C55" t="s">
         <v>377</v>
@@ -23665,7 +23642,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C56" t="s">
         <v>380</v>
@@ -23701,7 +23678,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C57" t="s">
         <v>120</v>
@@ -23733,7 +23710,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C58" t="s">
         <v>123</v>
@@ -23769,7 +23746,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C59" t="s">
         <v>128</v>
@@ -23801,7 +23778,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C60" t="s">
         <v>131</v>
@@ -23833,7 +23810,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C61" t="s">
         <v>134</v>
@@ -23865,7 +23842,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C62" t="s">
         <v>137</v>
@@ -23897,7 +23874,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C63" t="s">
         <v>140</v>
@@ -23929,7 +23906,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C64" t="s">
         <v>143</v>
@@ -23961,7 +23938,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C65" t="s">
         <v>146</v>
@@ -23993,7 +23970,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C66" t="s">
         <v>149</v>
@@ -24025,7 +24002,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C67" t="s">
         <v>152</v>
@@ -24057,7 +24034,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C68" t="s">
         <v>155</v>
@@ -24089,7 +24066,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C69" t="s">
         <v>158</v>
@@ -24121,7 +24098,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C70" t="s">
         <v>161</v>
@@ -24153,7 +24130,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C71" t="s">
         <v>164</v>
@@ -24185,7 +24162,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C72" t="s">
         <v>167</v>
@@ -24217,7 +24194,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C73" t="s">
         <v>170</v>
@@ -24249,7 +24226,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C74" t="s">
         <v>173</v>
@@ -24281,7 +24258,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C75" t="s">
         <v>176</v>
@@ -24313,7 +24290,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C76" t="s">
         <v>179</v>
@@ -24345,7 +24322,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>182</v>
@@ -24377,7 +24354,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>185</v>
@@ -24484,7 +24461,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
@@ -24529,10 +24506,10 @@
         <v>59</v>
       </c>
       <c r="Q1" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="R1" s="14" t="s">
         <v>419</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -28742,13 +28719,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP81"/>
+  <dimension ref="A1:AO81"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A76" sqref="A76:XFD76"/>
+      <selection pane="bottomRight" activeCell="AG11" sqref="AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -28773,18 +28750,18 @@
     <col min="21" max="21" width="10.6640625" customWidth="1"/>
     <col min="22" max="23" width="14.83203125" customWidth="1"/>
     <col min="24" max="33" width="11.33203125" customWidth="1"/>
-    <col min="37" max="37" width="17.1640625" customWidth="1"/>
-    <col min="38" max="38" width="12" customWidth="1"/>
-    <col min="39" max="40" width="10.6640625" customWidth="1"/>
-    <col min="41" max="41" width="10" customWidth="1"/>
+    <col min="36" max="36" width="17.1640625" customWidth="1"/>
+    <col min="37" max="37" width="12" customWidth="1"/>
+    <col min="38" max="39" width="10.6640625" customWidth="1"/>
+    <col min="40" max="40" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="56" customHeight="1">
+    <row r="1" spans="1:40" ht="56" customHeight="1">
       <c r="A1" s="27" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>0</v>
@@ -28883,28 +28860,25 @@
         <v>102</v>
       </c>
       <c r="AI1" s="33" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AJ1" s="33" t="s">
-        <v>387</v>
+        <v>189</v>
       </c>
       <c r="AK1" s="33" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="AL1" s="33" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="AM1" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="AN1" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="AO1" s="27" t="s">
+      <c r="AN1" s="27" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:40">
       <c r="A2" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>1</v>
@@ -29006,18 +28980,17 @@
       <c r="AI2" s="36"/>
       <c r="AJ2" s="36"/>
       <c r="AK2" s="36"/>
-      <c r="AL2" s="36"/>
+      <c r="AL2" s="26">
+        <v>-3.3445307652912898E-2</v>
+      </c>
       <c r="AM2" s="26">
-        <v>-3.3445307652912898E-2</v>
-      </c>
-      <c r="AN2" s="26">
         <v>-2.74546666918043E-2</v>
       </c>
-      <c r="AO2" s="34" t="e">
+      <c r="AN2" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:40">
       <c r="A3" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>2</v>
@@ -29119,18 +29092,17 @@
       <c r="AI3" s="36"/>
       <c r="AJ3" s="36"/>
       <c r="AK3" s="36"/>
-      <c r="AL3" s="36"/>
+      <c r="AL3" s="26">
+        <v>-3.8295470076922897E-2</v>
+      </c>
       <c r="AM3" s="26">
-        <v>-3.8295470076922897E-2</v>
-      </c>
-      <c r="AN3" s="26">
         <v>-2.5605384434687298E-2</v>
       </c>
-      <c r="AO3" s="34" t="e">
+      <c r="AN3" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:40">
       <c r="A4" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>3</v>
@@ -29236,22 +29208,19 @@
       <c r="AI4" s="36">
         <v>-0.67620327269263103</v>
       </c>
-      <c r="AJ4" s="36">
-        <v>13.5740311504732</v>
-      </c>
+      <c r="AJ4" s="36"/>
       <c r="AK4" s="36"/>
-      <c r="AL4" s="36"/>
+      <c r="AL4" s="26">
+        <v>-0.169520823184417</v>
+      </c>
       <c r="AM4" s="26">
-        <v>-0.169520823184417</v>
-      </c>
-      <c r="AN4" s="26">
         <v>-9.56060450005361E-2</v>
       </c>
-      <c r="AO4" s="34" t="e">
+      <c r="AN4" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:40">
       <c r="A5" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>4</v>
@@ -29357,22 +29326,19 @@
       <c r="AI5" s="36">
         <v>-0.63524417358112095</v>
       </c>
-      <c r="AJ5" s="36">
-        <v>12.751822637608401</v>
-      </c>
+      <c r="AJ5" s="36"/>
       <c r="AK5" s="36"/>
-      <c r="AL5" s="36"/>
+      <c r="AL5" s="26">
+        <v>-0.22064195134047301</v>
+      </c>
       <c r="AM5" s="26">
-        <v>-0.22064195134047301</v>
-      </c>
-      <c r="AN5" s="26">
         <v>-0.112085512265169</v>
       </c>
-      <c r="AO5" s="34" t="e">
+      <c r="AN5" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:40">
       <c r="A6" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>5</v>
@@ -29478,22 +29444,19 @@
       <c r="AI6" s="36">
         <v>-1.35938080211032</v>
       </c>
-      <c r="AJ6" s="36">
-        <v>27.288062773970498</v>
-      </c>
+      <c r="AJ6" s="36"/>
       <c r="AK6" s="36"/>
-      <c r="AL6" s="36"/>
+      <c r="AL6" s="26">
+        <v>-0.431270563233983</v>
+      </c>
       <c r="AM6" s="26">
-        <v>-0.431270563233983</v>
-      </c>
-      <c r="AN6" s="26">
         <v>-0.215453839393101</v>
       </c>
-      <c r="AO6" s="34">
+      <c r="AN6" s="34">
         <v>-0.32815825258604098</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:40">
       <c r="A7" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>6</v>
@@ -29599,22 +29562,19 @@
       <c r="AI7" s="36">
         <v>-0.58079912522844201</v>
       </c>
-      <c r="AJ7" s="36">
-        <v>11.658898642453099</v>
-      </c>
+      <c r="AJ7" s="36"/>
       <c r="AK7" s="36"/>
-      <c r="AL7" s="36"/>
+      <c r="AL7" s="26">
+        <v>-0.24539098137818499</v>
+      </c>
       <c r="AM7" s="26">
-        <v>-0.24539098137818499</v>
-      </c>
-      <c r="AN7" s="26">
         <v>-0.15174022257737499</v>
       </c>
-      <c r="AO7" s="34" t="e">
+      <c r="AN7" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:40">
       <c r="A8" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>7</v>
@@ -29720,22 +29680,19 @@
       <c r="AI8" s="36">
         <v>0</v>
       </c>
-      <c r="AJ8" s="36">
-        <v>0</v>
-      </c>
+      <c r="AJ8" s="36"/>
       <c r="AK8" s="36"/>
-      <c r="AL8" s="36"/>
+      <c r="AL8" s="26">
+        <v>-4.1471210608181999E-2</v>
+      </c>
       <c r="AM8" s="26">
-        <v>-4.1471210608181999E-2</v>
-      </c>
-      <c r="AN8" s="26">
         <v>-3.0146777960181899E-2</v>
       </c>
-      <c r="AO8" s="34" t="e">
+      <c r="AN8" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:40">
       <c r="A9" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>8</v>
@@ -29829,12 +29786,11 @@
       <c r="AI9" s="36"/>
       <c r="AJ9" s="36"/>
       <c r="AK9" s="36"/>
-      <c r="AL9" s="36"/>
+      <c r="AL9" s="26"/>
       <c r="AM9" s="26"/>
-      <c r="AN9" s="26"/>
-      <c r="AO9" s="34"/>
+      <c r="AN9" s="34"/>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:40">
       <c r="A10" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>9</v>
@@ -29936,18 +29892,17 @@
       <c r="AI10" s="36"/>
       <c r="AJ10" s="36"/>
       <c r="AK10" s="36"/>
-      <c r="AL10" s="36"/>
+      <c r="AL10" s="26">
+        <v>-0.23945482531110401</v>
+      </c>
       <c r="AM10" s="26">
-        <v>-0.23945482531110401</v>
-      </c>
-      <c r="AN10" s="26">
         <v>-0.15782218283768401</v>
       </c>
-      <c r="AO10" s="34" t="e">
+      <c r="AN10" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:40">
       <c r="A11" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>10</v>
@@ -30049,18 +30004,17 @@
       <c r="AI11" s="36"/>
       <c r="AJ11" s="36"/>
       <c r="AK11" s="36"/>
-      <c r="AL11" s="36"/>
+      <c r="AL11" s="26">
+        <v>-7.7015962552748493E-2</v>
+      </c>
       <c r="AM11" s="26">
-        <v>-7.7015962552748493E-2</v>
-      </c>
-      <c r="AN11" s="26">
         <v>-6.0967257622191497E-2</v>
       </c>
-      <c r="AO11" s="34" t="e">
+      <c r="AN11" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:40">
       <c r="A12" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>11</v>
@@ -30166,22 +30120,19 @@
       <c r="AI12" s="36">
         <v>-2.1951561152431E-3</v>
       </c>
-      <c r="AJ12" s="36">
-        <v>4.4065325755981599E-2</v>
-      </c>
+      <c r="AJ12" s="36"/>
       <c r="AK12" s="36"/>
-      <c r="AL12" s="36"/>
+      <c r="AL12" s="26">
+        <v>-6.3677626629120396E-2</v>
+      </c>
       <c r="AM12" s="26">
-        <v>-6.3677626629120396E-2</v>
-      </c>
-      <c r="AN12" s="26">
         <v>-2.28284418247044E-2</v>
       </c>
-      <c r="AO12" s="34" t="e">
+      <c r="AN12" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:40">
       <c r="A13" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>12</v>
@@ -30287,22 +30238,19 @@
       <c r="AI13" s="36">
         <v>-2.2064811413883501E-2</v>
       </c>
-      <c r="AJ13" s="36">
-        <v>0.442926631024327</v>
-      </c>
+      <c r="AJ13" s="36"/>
       <c r="AK13" s="36"/>
-      <c r="AL13" s="36"/>
+      <c r="AL13" s="26">
+        <v>-3.6744605348128602E-2</v>
+      </c>
       <c r="AM13" s="26">
-        <v>-3.6744605348128602E-2</v>
-      </c>
-      <c r="AN13" s="26">
         <v>-2.5176660724515802E-2</v>
       </c>
-      <c r="AO13" s="34" t="e">
+      <c r="AN13" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:40">
       <c r="A14" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>13</v>
@@ -30408,22 +30356,19 @@
       <c r="AI14" s="36">
         <v>-1.6370482769372599E-2</v>
       </c>
-      <c r="AJ14" s="36">
-        <v>0.32861929545963098</v>
-      </c>
+      <c r="AJ14" s="36"/>
       <c r="AK14" s="36"/>
-      <c r="AL14" s="36"/>
+      <c r="AL14" s="26">
+        <v>-5.8926472002704101E-2</v>
+      </c>
       <c r="AM14" s="26">
-        <v>-5.8926472002704101E-2</v>
-      </c>
-      <c r="AN14" s="26">
         <v>-3.3845985568591197E-2</v>
       </c>
-      <c r="AO14" s="34" t="e">
+      <c r="AN14" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:40">
       <c r="A15" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>14</v>
@@ -30529,22 +30474,19 @@
       <c r="AI15" s="36">
         <v>-0.10967945268870199</v>
       </c>
-      <c r="AJ15" s="36">
-        <v>2.2016934367012801</v>
-      </c>
+      <c r="AJ15" s="36"/>
       <c r="AK15" s="36"/>
-      <c r="AL15" s="36"/>
+      <c r="AL15" s="26">
+        <v>-9.0625473538779006E-2</v>
+      </c>
       <c r="AM15" s="26">
-        <v>-9.0625473538779006E-2</v>
-      </c>
-      <c r="AN15" s="26">
         <v>-5.7292099574339499E-2</v>
       </c>
-      <c r="AO15" s="34" t="e">
+      <c r="AN15" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:40">
       <c r="A16" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>15</v>
@@ -30650,22 +30592,19 @@
       <c r="AI16" s="36">
         <v>-5.5024576824640901E-3</v>
       </c>
-      <c r="AJ16" s="36">
-        <v>0.110455738684185</v>
-      </c>
+      <c r="AJ16" s="36"/>
       <c r="AK16" s="36"/>
-      <c r="AL16" s="36"/>
+      <c r="AL16" s="26">
+        <v>-6.5259532103828705E-2</v>
+      </c>
       <c r="AM16" s="26">
-        <v>-6.5259532103828705E-2</v>
-      </c>
-      <c r="AN16" s="26">
         <v>-2.8492201548946799E-2</v>
       </c>
-      <c r="AO16" s="34" t="e">
+      <c r="AN16" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="17" spans="1:41">
+    <row r="17" spans="1:40">
       <c r="A17" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>16</v>
@@ -30765,16 +30704,13 @@
       <c r="AI17" s="36">
         <v>-8.3946059276953002E-3</v>
       </c>
-      <c r="AJ17" s="36">
-        <v>0.16851240885709001</v>
-      </c>
+      <c r="AJ17" s="36"/>
       <c r="AK17" s="36"/>
-      <c r="AL17" s="36"/>
+      <c r="AL17" s="26"/>
       <c r="AM17" s="26"/>
-      <c r="AN17" s="26"/>
-      <c r="AO17" s="34"/>
+      <c r="AN17" s="34"/>
     </row>
-    <row r="18" spans="1:41">
+    <row r="18" spans="1:40">
       <c r="A18" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>17</v>
@@ -30880,22 +30816,19 @@
       <c r="AI18" s="36">
         <v>-6.18529559380782E-2</v>
       </c>
-      <c r="AJ18" s="36">
-        <v>1.2416295285130301</v>
-      </c>
+      <c r="AJ18" s="36"/>
       <c r="AK18" s="36"/>
-      <c r="AL18" s="36"/>
+      <c r="AL18" s="26">
+        <v>-0.11710361474940099</v>
+      </c>
       <c r="AM18" s="26">
-        <v>-0.11710361474940099</v>
-      </c>
-      <c r="AN18" s="26">
         <v>-5.56518648997434E-2</v>
       </c>
-      <c r="AO18" s="34" t="e">
+      <c r="AN18" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="19" spans="1:41">
+    <row r="19" spans="1:40">
       <c r="A19" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>18</v>
@@ -30995,12 +30928,11 @@
       <c r="AI19" s="36"/>
       <c r="AJ19" s="36"/>
       <c r="AK19" s="36"/>
-      <c r="AL19" s="36"/>
+      <c r="AL19" s="26"/>
       <c r="AM19" s="26"/>
-      <c r="AN19" s="26"/>
-      <c r="AO19" s="34"/>
+      <c r="AN19" s="34"/>
     </row>
-    <row r="20" spans="1:41">
+    <row r="20" spans="1:40">
       <c r="A20" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>19</v>
@@ -31106,22 +31038,19 @@
       <c r="AI20" s="36">
         <v>-3.28661080532721E-3</v>
       </c>
-      <c r="AJ20" s="36">
-        <v>6.5975068818207402E-2</v>
-      </c>
+      <c r="AJ20" s="36"/>
       <c r="AK20" s="36"/>
-      <c r="AL20" s="36"/>
+      <c r="AL20" s="26">
+        <v>-0.13754944846997999</v>
+      </c>
       <c r="AM20" s="26">
-        <v>-0.13754944846997999</v>
-      </c>
-      <c r="AN20" s="26">
         <v>-6.0227556741026297E-2</v>
       </c>
-      <c r="AO20" s="34" t="e">
+      <c r="AN20" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="21" spans="1:41">
+    <row r="21" spans="1:40">
       <c r="A21" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>20</v>
@@ -31223,18 +31152,17 @@
       <c r="AI21" s="36"/>
       <c r="AJ21" s="36"/>
       <c r="AK21" s="36"/>
-      <c r="AL21" s="36"/>
+      <c r="AL21" s="26">
+        <v>-4.6187839587458902E-2</v>
+      </c>
       <c r="AM21" s="26">
-        <v>-4.6187839587458902E-2</v>
-      </c>
-      <c r="AN21" s="26">
         <v>-3.9125372970037001E-2</v>
       </c>
-      <c r="AO21" s="34" t="e">
+      <c r="AN21" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="22" spans="1:41">
+    <row r="22" spans="1:40">
       <c r="A22" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>21</v>
@@ -31340,22 +31268,19 @@
       <c r="AI22" s="36">
         <v>-1.9375784650011E-2</v>
       </c>
-      <c r="AJ22" s="36">
-        <v>0.38894739943629397</v>
-      </c>
+      <c r="AJ22" s="36"/>
       <c r="AK22" s="36"/>
-      <c r="AL22" s="36"/>
+      <c r="AL22" s="26">
+        <v>-6.8532786585286901E-2</v>
+      </c>
       <c r="AM22" s="26">
-        <v>-6.8532786585286901E-2</v>
-      </c>
-      <c r="AN22" s="26">
         <v>-3.2074820504600803E-2</v>
       </c>
-      <c r="AO22" s="34" t="e">
+      <c r="AN22" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="23" spans="1:41">
+    <row r="23" spans="1:40">
       <c r="A23" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>22</v>
@@ -31457,18 +31382,17 @@
       <c r="AI23" s="36"/>
       <c r="AJ23" s="36"/>
       <c r="AK23" s="36"/>
-      <c r="AL23" s="36"/>
+      <c r="AL23" s="26">
+        <v>-0.187998717326439</v>
+      </c>
       <c r="AM23" s="26">
-        <v>-0.187998717326439</v>
-      </c>
-      <c r="AN23" s="26">
         <v>-0.12992133520837201</v>
       </c>
-      <c r="AO23" s="34" t="e">
+      <c r="AN23" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="24" spans="1:41">
+    <row r="24" spans="1:40">
       <c r="A24" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>23</v>
@@ -31570,18 +31494,17 @@
       <c r="AI24" s="36"/>
       <c r="AJ24" s="36"/>
       <c r="AK24" s="36"/>
-      <c r="AL24" s="36"/>
+      <c r="AL24" s="26">
+        <v>-0.156188950747221</v>
+      </c>
       <c r="AM24" s="26">
-        <v>-0.156188950747221</v>
-      </c>
-      <c r="AN24" s="26">
         <v>-0.12557904748429899</v>
       </c>
-      <c r="AO24" s="34" t="e">
+      <c r="AN24" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="25" spans="1:41">
+    <row r="25" spans="1:40">
       <c r="A25" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>24</v>
@@ -31681,16 +31604,15 @@
       <c r="AI25" s="36"/>
       <c r="AJ25" s="36"/>
       <c r="AK25" s="36"/>
-      <c r="AL25" s="36"/>
+      <c r="AL25" s="26">
+        <v>-0.156188950747221</v>
+      </c>
       <c r="AM25" s="26">
-        <v>-0.156188950747221</v>
-      </c>
-      <c r="AN25" s="26">
         <v>-0.12948869087735601</v>
       </c>
-      <c r="AO25" s="34"/>
+      <c r="AN25" s="34"/>
     </row>
-    <row r="26" spans="1:41">
+    <row r="26" spans="1:40">
       <c r="A26" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>25</v>
@@ -31796,22 +31718,19 @@
       <c r="AI26" s="36">
         <v>-0.159261202047628</v>
       </c>
-      <c r="AJ26" s="36">
-        <v>3.1969920953620798</v>
-      </c>
+      <c r="AJ26" s="36"/>
       <c r="AK26" s="36"/>
-      <c r="AL26" s="36"/>
+      <c r="AL26" s="26">
+        <v>-0.19366577676014499</v>
+      </c>
       <c r="AM26" s="26">
-        <v>-0.19366577676014499</v>
-      </c>
-      <c r="AN26" s="26">
         <v>-0.111296434131563</v>
       </c>
-      <c r="AO26" s="34" t="e">
+      <c r="AN26" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="27" spans="1:41">
+    <row r="27" spans="1:40">
       <c r="A27" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>26</v>
@@ -31917,22 +31836,19 @@
       <c r="AI27" s="36">
         <v>-1.3400484159600001E-2</v>
       </c>
-      <c r="AJ27" s="36">
-        <v>0.26899986551309601</v>
-      </c>
+      <c r="AJ27" s="36"/>
       <c r="AK27" s="36"/>
-      <c r="AL27" s="36"/>
+      <c r="AL27" s="26">
+        <v>-0.15968366140405199</v>
+      </c>
       <c r="AM27" s="26">
-        <v>-0.15968366140405199</v>
-      </c>
-      <c r="AN27" s="26">
         <v>-7.0303252446051304E-2</v>
       </c>
-      <c r="AO27" s="34" t="e">
+      <c r="AN27" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="28" spans="1:41">
+    <row r="28" spans="1:40">
       <c r="A28" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>27</v>
@@ -32038,22 +31954,19 @@
       <c r="AI28" s="36">
         <v>-7.1682651098618697E-2</v>
       </c>
-      <c r="AJ28" s="36">
-        <v>1.4389497629708199</v>
-      </c>
+      <c r="AJ28" s="36"/>
       <c r="AK28" s="36"/>
-      <c r="AL28" s="36"/>
+      <c r="AL28" s="26">
+        <v>-0.36500688102871498</v>
+      </c>
       <c r="AM28" s="26">
-        <v>-0.36500688102871498</v>
-      </c>
-      <c r="AN28" s="26">
         <v>-0.120658265839372</v>
       </c>
-      <c r="AO28" s="34" t="e">
+      <c r="AN28" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="29" spans="1:41">
+    <row r="29" spans="1:40">
       <c r="A29" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>28</v>
@@ -32159,22 +32072,19 @@
       <c r="AI29" s="36">
         <v>-0.55336000051026202</v>
       </c>
-      <c r="AJ29" s="36">
-        <v>11.108088629092499</v>
-      </c>
+      <c r="AJ29" s="36"/>
       <c r="AK29" s="36"/>
-      <c r="AL29" s="36"/>
+      <c r="AL29" s="26">
+        <v>-0.34308001137970701</v>
+      </c>
       <c r="AM29" s="26">
-        <v>-0.34308001137970701</v>
-      </c>
-      <c r="AN29" s="26">
         <v>-0.13212516473283201</v>
       </c>
-      <c r="AO29" s="34" t="e">
+      <c r="AN29" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="30" spans="1:41">
+    <row r="30" spans="1:40">
       <c r="A30" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>29</v>
@@ -32280,22 +32190,19 @@
       <c r="AI30" s="36">
         <v>0</v>
       </c>
-      <c r="AJ30" s="36">
-        <v>0</v>
-      </c>
+      <c r="AJ30" s="36"/>
       <c r="AK30" s="36"/>
-      <c r="AL30" s="36"/>
+      <c r="AL30" s="26">
+        <v>-4.54794841442894E-2</v>
+      </c>
       <c r="AM30" s="26">
-        <v>-4.54794841442894E-2</v>
-      </c>
-      <c r="AN30" s="26">
         <v>-2.9350078444288701E-2</v>
       </c>
-      <c r="AO30" s="34" t="e">
+      <c r="AN30" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="31" spans="1:41">
+    <row r="31" spans="1:40">
       <c r="A31" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>30</v>
@@ -32401,22 +32308,19 @@
       <c r="AI31" s="36">
         <v>-6.1297791466874398E-2</v>
       </c>
-      <c r="AJ31" s="36">
-        <v>1.2304852171349601</v>
-      </c>
+      <c r="AJ31" s="36"/>
       <c r="AK31" s="36"/>
-      <c r="AL31" s="36"/>
+      <c r="AL31" s="26">
+        <v>-3.8995898452835097E-2</v>
+      </c>
       <c r="AM31" s="26">
-        <v>-3.8995898452835097E-2</v>
-      </c>
-      <c r="AN31" s="26">
         <v>-3.5414163202009498E-2</v>
       </c>
-      <c r="AO31" s="34" t="e">
+      <c r="AN31" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="32" spans="1:41">
+    <row r="32" spans="1:40">
       <c r="A32" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>31</v>
@@ -32522,22 +32426,19 @@
       <c r="AI32" s="36">
         <v>0</v>
       </c>
-      <c r="AJ32" s="36">
-        <v>0</v>
-      </c>
+      <c r="AJ32" s="36"/>
       <c r="AK32" s="36"/>
-      <c r="AL32" s="36"/>
+      <c r="AL32" s="26">
+        <v>-3.31984933410059E-2</v>
+      </c>
       <c r="AM32" s="26">
-        <v>-3.31984933410059E-2</v>
-      </c>
-      <c r="AN32" s="26">
         <v>-2.3048302942091599E-2</v>
       </c>
-      <c r="AO32" s="34" t="e">
+      <c r="AN32" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="33" spans="1:41">
+    <row r="33" spans="1:40">
       <c r="A33" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>32</v>
@@ -32643,22 +32544,19 @@
       <c r="AI33" s="36">
         <v>0</v>
       </c>
-      <c r="AJ33" s="36">
-        <v>0</v>
-      </c>
+      <c r="AJ33" s="36"/>
       <c r="AK33" s="36"/>
-      <c r="AL33" s="36"/>
+      <c r="AL33" s="26">
+        <v>-0.13203805659683801</v>
+      </c>
       <c r="AM33" s="26">
-        <v>-0.13203805659683801</v>
-      </c>
-      <c r="AN33" s="26">
         <v>-6.4818415811091906E-2</v>
       </c>
-      <c r="AO33" s="34" t="e">
+      <c r="AN33" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="34" spans="1:41">
+    <row r="34" spans="1:40">
       <c r="A34" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>33</v>
@@ -32764,22 +32662,19 @@
       <c r="AI34" s="36">
         <v>-8.9130081854499901E-2</v>
       </c>
-      <c r="AJ34" s="36">
-        <v>1.7891875954986001</v>
-      </c>
+      <c r="AJ34" s="36"/>
       <c r="AK34" s="36"/>
-      <c r="AL34" s="36"/>
+      <c r="AL34" s="26">
+        <v>-3.9128127281761398E-2</v>
+      </c>
       <c r="AM34" s="26">
-        <v>-3.9128127281761398E-2</v>
-      </c>
-      <c r="AN34" s="26">
         <v>-3.1598346199546601E-2</v>
       </c>
-      <c r="AO34" s="34" t="e">
+      <c r="AN34" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="35" spans="1:41">
+    <row r="35" spans="1:40">
       <c r="A35" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>34</v>
@@ -32885,22 +32780,19 @@
       <c r="AI35" s="36">
         <v>-7.3298161471949203E-2</v>
       </c>
-      <c r="AJ35" s="36">
-        <v>1.4713793429759301</v>
-      </c>
+      <c r="AJ35" s="36"/>
       <c r="AK35" s="36"/>
-      <c r="AL35" s="36"/>
+      <c r="AL35" s="26">
+        <v>-6.4420511553588994E-2</v>
+      </c>
       <c r="AM35" s="26">
-        <v>-6.4420511553588994E-2</v>
-      </c>
-      <c r="AN35" s="26">
         <v>-4.0532932078243503E-2</v>
       </c>
-      <c r="AO35" s="34" t="e">
+      <c r="AN35" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="36" spans="1:41">
+    <row r="36" spans="1:40">
       <c r="A36" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>35</v>
@@ -33006,22 +32898,19 @@
       <c r="AI36" s="36">
         <v>-0.22924206302699299</v>
       </c>
-      <c r="AJ36" s="36">
-        <v>4.6017803080666102</v>
-      </c>
+      <c r="AJ36" s="36"/>
       <c r="AK36" s="36"/>
-      <c r="AL36" s="36"/>
+      <c r="AL36" s="26">
+        <v>-0.14876702932064001</v>
+      </c>
       <c r="AM36" s="26">
-        <v>-0.14876702932064001</v>
-      </c>
-      <c r="AN36" s="26">
         <v>-0.100383097283019</v>
       </c>
-      <c r="AO36" s="34" t="e">
+      <c r="AN36" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="37" spans="1:41">
+    <row r="37" spans="1:40">
       <c r="A37" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>36</v>
@@ -33127,22 +33016,19 @@
       <c r="AI37" s="36">
         <v>-0.28690790479068501</v>
       </c>
-      <c r="AJ37" s="36">
-        <v>5.7593581608056201</v>
-      </c>
+      <c r="AJ37" s="36"/>
       <c r="AK37" s="36"/>
-      <c r="AL37" s="36"/>
+      <c r="AL37" s="26">
+        <v>-0.23878183658594301</v>
+      </c>
       <c r="AM37" s="26">
-        <v>-0.23878183658594301</v>
-      </c>
-      <c r="AN37" s="26">
         <v>-0.17003889475825101</v>
       </c>
-      <c r="AO37" s="34" t="e">
+      <c r="AN37" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="38" spans="1:41">
+    <row r="38" spans="1:40">
       <c r="A38" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>37</v>
@@ -33248,22 +33134,19 @@
       <c r="AI38" s="36">
         <v>0</v>
       </c>
-      <c r="AJ38" s="36">
-        <v>0</v>
-      </c>
+      <c r="AJ38" s="36"/>
       <c r="AK38" s="36"/>
-      <c r="AL38" s="36"/>
+      <c r="AL38" s="26">
+        <v>-0.21146168435950499</v>
+      </c>
       <c r="AM38" s="26">
-        <v>-0.21146168435950499</v>
-      </c>
-      <c r="AN38" s="26">
         <v>-0.10518986979452299</v>
       </c>
-      <c r="AO38" s="34" t="e">
+      <c r="AN38" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="39" spans="1:41">
+    <row r="39" spans="1:40">
       <c r="A39" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>38</v>
@@ -33369,22 +33252,19 @@
       <c r="AI39" s="36">
         <v>-1.0950218990405399E-2</v>
       </c>
-      <c r="AJ39" s="36">
-        <v>0.219813508278937</v>
-      </c>
+      <c r="AJ39" s="36"/>
       <c r="AK39" s="36"/>
-      <c r="AL39" s="36"/>
+      <c r="AL39" s="26">
+        <v>-5.1307705102197503E-2</v>
+      </c>
       <c r="AM39" s="26">
-        <v>-5.1307705102197503E-2</v>
-      </c>
-      <c r="AN39" s="26">
         <v>-3.6031922370022597E-2</v>
       </c>
-      <c r="AO39" s="34" t="e">
+      <c r="AN39" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="40" spans="1:41">
+    <row r="40" spans="1:40">
       <c r="A40" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>39</v>
@@ -33490,22 +33370,19 @@
       <c r="AI40" s="36">
         <v>-4.5223936136194097E-2</v>
       </c>
-      <c r="AJ40" s="36">
-        <v>0.90782038870543302</v>
-      </c>
+      <c r="AJ40" s="36"/>
       <c r="AK40" s="36"/>
-      <c r="AL40" s="36"/>
+      <c r="AL40" s="26">
+        <v>-0.125058345094303</v>
+      </c>
       <c r="AM40" s="26">
-        <v>-0.125058345094303</v>
-      </c>
-      <c r="AN40" s="26">
         <v>-6.0087738622177901E-2</v>
       </c>
-      <c r="AO40" s="34" t="e">
+      <c r="AN40" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="41" spans="1:41">
+    <row r="41" spans="1:40">
       <c r="A41" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>40</v>
@@ -33611,22 +33488,19 @@
       <c r="AI41" s="36">
         <v>-1.54397684082216E-2</v>
       </c>
-      <c r="AJ41" s="36">
-        <v>0.30993623632542899</v>
-      </c>
+      <c r="AJ41" s="36"/>
       <c r="AK41" s="36"/>
-      <c r="AL41" s="36"/>
+      <c r="AL41" s="26">
+        <v>-5.4352491744792203E-2</v>
+      </c>
       <c r="AM41" s="26">
-        <v>-5.4352491744792203E-2</v>
-      </c>
-      <c r="AN41" s="26">
         <v>-3.50111446428579E-2</v>
       </c>
-      <c r="AO41" s="34" t="e">
+      <c r="AN41" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="42" spans="1:41">
+    <row r="42" spans="1:40">
       <c r="A42" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>41</v>
@@ -33732,22 +33606,19 @@
       <c r="AI42" s="36">
         <v>-2.21302431924272E-3</v>
       </c>
-      <c r="AJ42" s="36">
-        <v>4.4424010144964297E-2</v>
-      </c>
+      <c r="AJ42" s="36"/>
       <c r="AK42" s="36"/>
-      <c r="AL42" s="36"/>
+      <c r="AL42" s="26">
+        <v>-3.8857490715942702E-2</v>
+      </c>
       <c r="AM42" s="26">
-        <v>-3.8857490715942702E-2</v>
-      </c>
-      <c r="AN42" s="26">
         <v>-2.58035425334231E-2</v>
       </c>
-      <c r="AO42" s="34" t="e">
+      <c r="AN42" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="43" spans="1:41">
+    <row r="43" spans="1:40">
       <c r="A43" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>42</v>
@@ -33853,22 +33724,19 @@
       <c r="AI43" s="36">
         <v>-3.2327434863326197E-2</v>
       </c>
-      <c r="AJ43" s="36">
-        <v>0.648937420995221</v>
-      </c>
+      <c r="AJ43" s="36"/>
       <c r="AK43" s="36"/>
-      <c r="AL43" s="36"/>
+      <c r="AL43" s="26">
+        <v>-9.7973466758260103E-2</v>
+      </c>
       <c r="AM43" s="26">
-        <v>-9.7973466758260103E-2</v>
-      </c>
-      <c r="AN43" s="26">
         <v>-5.6803259272514998E-2</v>
       </c>
-      <c r="AO43" s="34" t="e">
+      <c r="AN43" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="44" spans="1:41">
+    <row r="44" spans="1:40">
       <c r="A44" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>43</v>
@@ -33968,12 +33836,11 @@
       <c r="AI44" s="36"/>
       <c r="AJ44" s="36"/>
       <c r="AK44" s="36"/>
-      <c r="AL44" s="36"/>
+      <c r="AL44" s="26"/>
       <c r="AM44" s="26"/>
-      <c r="AN44" s="26"/>
-      <c r="AO44" s="34"/>
+      <c r="AN44" s="34"/>
     </row>
-    <row r="45" spans="1:41">
+    <row r="45" spans="1:40">
       <c r="A45" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>44</v>
@@ -34075,18 +33942,17 @@
       <c r="AI45" s="36"/>
       <c r="AJ45" s="36"/>
       <c r="AK45" s="36"/>
-      <c r="AL45" s="36"/>
+      <c r="AL45" s="26">
+        <v>-9.6896103169485895E-2</v>
+      </c>
       <c r="AM45" s="26">
-        <v>-9.6896103169485895E-2</v>
-      </c>
-      <c r="AN45" s="26">
         <v>-5.7959095243286102E-2</v>
       </c>
-      <c r="AO45" s="34" t="e">
+      <c r="AN45" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="46" spans="1:41">
+    <row r="46" spans="1:40">
       <c r="A46" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>45</v>
@@ -34188,18 +34054,17 @@
       <c r="AI46" s="36"/>
       <c r="AJ46" s="36"/>
       <c r="AK46" s="36"/>
-      <c r="AL46" s="36"/>
+      <c r="AL46" s="26">
+        <v>-0.12179386036301799</v>
+      </c>
       <c r="AM46" s="26">
-        <v>-0.12179386036301799</v>
-      </c>
-      <c r="AN46" s="26">
         <v>-6.5089802480464906E-2</v>
       </c>
-      <c r="AO46" s="34" t="e">
+      <c r="AN46" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="47" spans="1:41">
+    <row r="47" spans="1:40">
       <c r="A47" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>46</v>
@@ -34301,18 +34166,17 @@
       <c r="AI47" s="36"/>
       <c r="AJ47" s="36"/>
       <c r="AK47" s="36"/>
-      <c r="AL47" s="36"/>
+      <c r="AL47" s="26">
+        <v>-0.31677846731360199</v>
+      </c>
       <c r="AM47" s="26">
-        <v>-0.31677846731360199</v>
-      </c>
-      <c r="AN47" s="26">
         <v>-0.203545805030664</v>
       </c>
-      <c r="AO47" s="34" t="e">
+      <c r="AN47" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="48" spans="1:41">
+    <row r="48" spans="1:40">
       <c r="A48" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>47</v>
@@ -34414,18 +34278,17 @@
       <c r="AI48" s="36"/>
       <c r="AJ48" s="36"/>
       <c r="AK48" s="36"/>
-      <c r="AL48" s="36"/>
+      <c r="AL48" s="26">
+        <v>-4.2002628152343999E-2</v>
+      </c>
       <c r="AM48" s="26">
-        <v>-4.2002628152343999E-2</v>
-      </c>
-      <c r="AN48" s="26">
         <v>-2.1024331412601301E-2</v>
       </c>
-      <c r="AO48" s="34" t="e">
+      <c r="AN48" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="49" spans="1:41">
+    <row r="49" spans="1:40">
       <c r="A49" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>48</v>
@@ -34527,18 +34390,17 @@
       <c r="AI49" s="36"/>
       <c r="AJ49" s="36"/>
       <c r="AK49" s="36"/>
-      <c r="AL49" s="36"/>
+      <c r="AL49" s="26">
+        <v>-0.109669817064093</v>
+      </c>
       <c r="AM49" s="26">
-        <v>-0.109669817064093</v>
-      </c>
-      <c r="AN49" s="26">
         <v>-4.4877451540351103E-2</v>
       </c>
-      <c r="AO49" s="34" t="e">
+      <c r="AN49" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="50" spans="1:41">
+    <row r="50" spans="1:40">
       <c r="A50" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>49</v>
@@ -34640,18 +34502,17 @@
       <c r="AI50" s="36"/>
       <c r="AJ50" s="36"/>
       <c r="AK50" s="36"/>
-      <c r="AL50" s="36"/>
+      <c r="AL50" s="26">
+        <v>-0.11623180641436399</v>
+      </c>
       <c r="AM50" s="26">
-        <v>-0.11623180641436399</v>
-      </c>
-      <c r="AN50" s="26">
         <v>-6.1217977698030099E-2</v>
       </c>
-      <c r="AO50" s="34" t="e">
+      <c r="AN50" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="51" spans="1:41">
+    <row r="51" spans="1:40">
       <c r="A51" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>50</v>
@@ -34753,18 +34614,17 @@
       <c r="AI51" s="36"/>
       <c r="AJ51" s="36"/>
       <c r="AK51" s="36"/>
-      <c r="AL51" s="36"/>
+      <c r="AL51" s="26">
+        <v>-4.01175004489902E-2</v>
+      </c>
       <c r="AM51" s="26">
-        <v>-4.01175004489902E-2</v>
-      </c>
-      <c r="AN51" s="26">
         <v>-3.6471990710497101E-2</v>
       </c>
-      <c r="AO51" s="34" t="e">
+      <c r="AN51" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="52" spans="1:41">
+    <row r="52" spans="1:40">
       <c r="A52" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>51</v>
@@ -34866,18 +34726,17 @@
       <c r="AI52" s="36"/>
       <c r="AJ52" s="36"/>
       <c r="AK52" s="36"/>
-      <c r="AL52" s="36"/>
+      <c r="AL52" s="26">
+        <v>-3.9482427560348497E-2</v>
+      </c>
       <c r="AM52" s="26">
-        <v>-3.9482427560348497E-2</v>
-      </c>
-      <c r="AN52" s="26">
         <v>-2.9996689439540598E-2</v>
       </c>
-      <c r="AO52" s="34" t="e">
+      <c r="AN52" s="34" t="e">
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="53" spans="1:41">
+    <row r="53" spans="1:40">
       <c r="A53" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>52</v>
@@ -34981,16 +34840,15 @@
       <c r="AI53" s="36"/>
       <c r="AJ53" s="36"/>
       <c r="AK53" s="36"/>
-      <c r="AL53" s="36"/>
+      <c r="AL53" s="26">
+        <v>-0.14876702932064001</v>
+      </c>
       <c r="AM53" s="26">
-        <v>-0.14876702932064001</v>
-      </c>
-      <c r="AN53" s="26">
         <v>-0.10017487673853601</v>
       </c>
-      <c r="AO53" s="34"/>
+      <c r="AN53" s="34"/>
     </row>
-    <row r="54" spans="1:41">
+    <row r="54" spans="1:40">
       <c r="A54" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>53</v>
@@ -35094,16 +34952,15 @@
       <c r="AI54" s="36"/>
       <c r="AJ54" s="36"/>
       <c r="AK54" s="36"/>
-      <c r="AL54" s="36"/>
+      <c r="AL54" s="26">
+        <v>-0.23878183658594301</v>
+      </c>
       <c r="AM54" s="26">
-        <v>-0.23878183658594301</v>
-      </c>
-      <c r="AN54" s="26">
         <v>-0.17764310019719601</v>
       </c>
-      <c r="AO54" s="34"/>
+      <c r="AN54" s="34"/>
     </row>
-    <row r="55" spans="1:41">
+    <row r="55" spans="1:40">
       <c r="A55" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>54</v>
@@ -35203,12 +35060,11 @@
       <c r="AI55" s="36"/>
       <c r="AJ55" s="36"/>
       <c r="AK55" s="36"/>
-      <c r="AL55" s="36"/>
+      <c r="AL55" s="26"/>
       <c r="AM55" s="26"/>
-      <c r="AN55" s="26"/>
-      <c r="AO55" s="34"/>
+      <c r="AN55" s="34"/>
     </row>
-    <row r="56" spans="1:41">
+    <row r="56" spans="1:40">
       <c r="A56" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>55</v>
@@ -35308,16 +35164,15 @@
       <c r="AI56" s="36"/>
       <c r="AJ56" s="36"/>
       <c r="AK56" s="36"/>
-      <c r="AL56" s="36"/>
+      <c r="AL56" s="26">
+        <v>-0.21146168435950499</v>
+      </c>
       <c r="AM56" s="26">
-        <v>-0.21146168435950499</v>
-      </c>
-      <c r="AN56" s="26">
         <v>-0.11389346930507201</v>
       </c>
-      <c r="AO56" s="34"/>
+      <c r="AN56" s="34"/>
     </row>
-    <row r="57" spans="1:41">
+    <row r="57" spans="1:40">
       <c r="A57" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>56</v>
@@ -35417,12 +35272,11 @@
       <c r="AI57" s="36"/>
       <c r="AJ57" s="36"/>
       <c r="AK57" s="36"/>
-      <c r="AL57" s="36"/>
+      <c r="AL57" s="26"/>
       <c r="AM57" s="26"/>
-      <c r="AN57" s="26"/>
-      <c r="AO57" s="34"/>
+      <c r="AN57" s="34"/>
     </row>
-    <row r="58" spans="1:41">
+    <row r="58" spans="1:40">
       <c r="A58" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>57</v>
@@ -35522,12 +35376,11 @@
       <c r="AI58" s="36"/>
       <c r="AJ58" s="36"/>
       <c r="AK58" s="36"/>
-      <c r="AL58" s="36"/>
+      <c r="AL58" s="26"/>
       <c r="AM58" s="26"/>
-      <c r="AN58" s="26"/>
-      <c r="AO58" s="34"/>
+      <c r="AN58" s="34"/>
     </row>
-    <row r="59" spans="1:41">
+    <row r="59" spans="1:40">
       <c r="A59" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>58</v>
@@ -35627,12 +35480,11 @@
       <c r="AI59" s="36"/>
       <c r="AJ59" s="36"/>
       <c r="AK59" s="36"/>
-      <c r="AL59" s="36"/>
+      <c r="AL59" s="26"/>
       <c r="AM59" s="26"/>
-      <c r="AN59" s="26"/>
-      <c r="AO59" s="34"/>
+      <c r="AN59" s="34"/>
     </row>
-    <row r="60" spans="1:41">
+    <row r="60" spans="1:40">
       <c r="A60" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>59</v>
@@ -35732,12 +35584,11 @@
       <c r="AI60" s="36"/>
       <c r="AJ60" s="36"/>
       <c r="AK60" s="36"/>
-      <c r="AL60" s="36"/>
+      <c r="AL60" s="26"/>
       <c r="AM60" s="26"/>
-      <c r="AN60" s="26"/>
-      <c r="AO60" s="34"/>
+      <c r="AN60" s="34"/>
     </row>
-    <row r="61" spans="1:41">
+    <row r="61" spans="1:40">
       <c r="A61" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>60</v>
@@ -35837,12 +35688,11 @@
       <c r="AI61" s="36"/>
       <c r="AJ61" s="36"/>
       <c r="AK61" s="36"/>
-      <c r="AL61" s="36"/>
+      <c r="AL61" s="26"/>
       <c r="AM61" s="26"/>
-      <c r="AN61" s="26"/>
-      <c r="AO61" s="34"/>
+      <c r="AN61" s="34"/>
     </row>
-    <row r="62" spans="1:41">
+    <row r="62" spans="1:40">
       <c r="A62" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>61</v>
@@ -35942,12 +35792,11 @@
       <c r="AI62" s="36"/>
       <c r="AJ62" s="36"/>
       <c r="AK62" s="36"/>
-      <c r="AL62" s="36"/>
+      <c r="AL62" s="26"/>
       <c r="AM62" s="26"/>
-      <c r="AN62" s="26"/>
-      <c r="AO62" s="34"/>
+      <c r="AN62" s="34"/>
     </row>
-    <row r="63" spans="1:41">
+    <row r="63" spans="1:40">
       <c r="A63" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>62</v>
@@ -36047,12 +35896,11 @@
       <c r="AI63" s="36"/>
       <c r="AJ63" s="36"/>
       <c r="AK63" s="36"/>
-      <c r="AL63" s="36"/>
+      <c r="AL63" s="26"/>
       <c r="AM63" s="26"/>
-      <c r="AN63" s="26"/>
-      <c r="AO63" s="34"/>
+      <c r="AN63" s="34"/>
     </row>
-    <row r="64" spans="1:41">
+    <row r="64" spans="1:40">
       <c r="A64" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>63</v>
@@ -36152,12 +36000,11 @@
       <c r="AI64" s="36"/>
       <c r="AJ64" s="36"/>
       <c r="AK64" s="36"/>
-      <c r="AL64" s="36"/>
+      <c r="AL64" s="26"/>
       <c r="AM64" s="26"/>
-      <c r="AN64" s="26"/>
-      <c r="AO64" s="34"/>
+      <c r="AN64" s="34"/>
     </row>
-    <row r="65" spans="1:42">
+    <row r="65" spans="1:41">
       <c r="A65" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>64</v>
@@ -36257,12 +36104,11 @@
       <c r="AI65" s="36"/>
       <c r="AJ65" s="36"/>
       <c r="AK65" s="36"/>
-      <c r="AL65" s="36"/>
+      <c r="AL65" s="26"/>
       <c r="AM65" s="26"/>
-      <c r="AN65" s="26"/>
-      <c r="AO65" s="34"/>
+      <c r="AN65" s="34"/>
     </row>
-    <row r="66" spans="1:42">
+    <row r="66" spans="1:41">
       <c r="A66" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>65</v>
@@ -36362,12 +36208,11 @@
       <c r="AI66" s="36"/>
       <c r="AJ66" s="36"/>
       <c r="AK66" s="36"/>
-      <c r="AL66" s="36"/>
+      <c r="AL66" s="26"/>
       <c r="AM66" s="26"/>
-      <c r="AN66" s="26"/>
-      <c r="AO66" s="34"/>
+      <c r="AN66" s="34"/>
     </row>
-    <row r="67" spans="1:42">
+    <row r="67" spans="1:41">
       <c r="A67" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>66</v>
@@ -36467,12 +36312,11 @@
       <c r="AI67" s="36"/>
       <c r="AJ67" s="36"/>
       <c r="AK67" s="36"/>
-      <c r="AL67" s="36"/>
+      <c r="AL67" s="26"/>
       <c r="AM67" s="26"/>
-      <c r="AN67" s="26"/>
-      <c r="AO67" s="34"/>
+      <c r="AN67" s="34"/>
     </row>
-    <row r="68" spans="1:42">
+    <row r="68" spans="1:41">
       <c r="A68" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>67</v>
@@ -36572,12 +36416,11 @@
       <c r="AI68" s="36"/>
       <c r="AJ68" s="36"/>
       <c r="AK68" s="36"/>
-      <c r="AL68" s="36"/>
+      <c r="AL68" s="26"/>
       <c r="AM68" s="26"/>
-      <c r="AN68" s="26"/>
-      <c r="AO68" s="34"/>
+      <c r="AN68" s="34"/>
     </row>
-    <row r="69" spans="1:42">
+    <row r="69" spans="1:41">
       <c r="A69" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>68</v>
@@ -36677,12 +36520,11 @@
       <c r="AI69" s="36"/>
       <c r="AJ69" s="36"/>
       <c r="AK69" s="36"/>
-      <c r="AL69" s="36"/>
+      <c r="AL69" s="26"/>
       <c r="AM69" s="26"/>
-      <c r="AN69" s="26"/>
-      <c r="AO69" s="34"/>
+      <c r="AN69" s="34"/>
     </row>
-    <row r="70" spans="1:42">
+    <row r="70" spans="1:41">
       <c r="A70" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>69</v>
@@ -36782,12 +36624,11 @@
       <c r="AI70" s="36"/>
       <c r="AJ70" s="36"/>
       <c r="AK70" s="36"/>
-      <c r="AL70" s="36"/>
+      <c r="AL70" s="26"/>
       <c r="AM70" s="26"/>
-      <c r="AN70" s="26"/>
-      <c r="AO70" s="34"/>
+      <c r="AN70" s="34"/>
     </row>
-    <row r="71" spans="1:42">
+    <row r="71" spans="1:41">
       <c r="A71" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>70</v>
@@ -36887,12 +36728,11 @@
       <c r="AI71" s="36"/>
       <c r="AJ71" s="36"/>
       <c r="AK71" s="36"/>
-      <c r="AL71" s="36"/>
+      <c r="AL71" s="26"/>
       <c r="AM71" s="26"/>
-      <c r="AN71" s="26"/>
-      <c r="AO71" s="34"/>
+      <c r="AN71" s="34"/>
     </row>
-    <row r="72" spans="1:42">
+    <row r="72" spans="1:41">
       <c r="A72" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>71</v>
@@ -36992,12 +36832,11 @@
       <c r="AI72" s="36"/>
       <c r="AJ72" s="36"/>
       <c r="AK72" s="36"/>
-      <c r="AL72" s="36"/>
+      <c r="AL72" s="26"/>
       <c r="AM72" s="26"/>
-      <c r="AN72" s="26"/>
-      <c r="AO72" s="34"/>
+      <c r="AN72" s="34"/>
     </row>
-    <row r="73" spans="1:42">
+    <row r="73" spans="1:41">
       <c r="A73" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>72</v>
@@ -37097,12 +36936,11 @@
       <c r="AI73" s="36"/>
       <c r="AJ73" s="36"/>
       <c r="AK73" s="36"/>
-      <c r="AL73" s="36"/>
+      <c r="AL73" s="26"/>
       <c r="AM73" s="26"/>
-      <c r="AN73" s="26"/>
-      <c r="AO73" s="34"/>
+      <c r="AN73" s="34"/>
     </row>
-    <row r="74" spans="1:42">
+    <row r="74" spans="1:41">
       <c r="A74" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>73</v>
@@ -37161,12 +36999,11 @@
       <c r="AI74" s="36"/>
       <c r="AJ74" s="36"/>
       <c r="AK74" s="36"/>
-      <c r="AL74" s="36"/>
+      <c r="AL74" s="26"/>
       <c r="AM74" s="26"/>
-      <c r="AN74" s="26"/>
-      <c r="AO74" s="34"/>
+      <c r="AN74" s="34"/>
     </row>
-    <row r="75" spans="1:42">
+    <row r="75" spans="1:41">
       <c r="A75" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>74</v>
@@ -37225,12 +37062,11 @@
       <c r="AI75" s="36"/>
       <c r="AJ75" s="36"/>
       <c r="AK75" s="36"/>
-      <c r="AL75" s="36"/>
+      <c r="AL75" s="26"/>
       <c r="AM75" s="26"/>
-      <c r="AN75" s="26"/>
-      <c r="AO75" s="34"/>
+      <c r="AN75" s="34"/>
     </row>
-    <row r="76" spans="1:42">
+    <row r="76" spans="1:41">
       <c r="A76" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>75</v>
@@ -37289,12 +37125,11 @@
       <c r="AI76" s="36"/>
       <c r="AJ76" s="36"/>
       <c r="AK76" s="36"/>
-      <c r="AL76" s="36"/>
+      <c r="AL76" s="26"/>
       <c r="AM76" s="26"/>
-      <c r="AN76" s="26"/>
-      <c r="AO76" s="34"/>
+      <c r="AN76" s="34"/>
     </row>
-    <row r="77" spans="1:42">
+    <row r="77" spans="1:41">
       <c r="A77" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>76</v>
@@ -37353,12 +37188,11 @@
       <c r="AI77" s="36"/>
       <c r="AJ77" s="36"/>
       <c r="AK77" s="36"/>
-      <c r="AL77" s="36"/>
+      <c r="AL77" s="26"/>
       <c r="AM77" s="26"/>
-      <c r="AN77" s="26"/>
-      <c r="AO77" s="34"/>
+      <c r="AN77" s="34"/>
     </row>
-    <row r="78" spans="1:42">
+    <row r="78" spans="1:41">
       <c r="A78" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>77</v>
@@ -37458,12 +37292,11 @@
       <c r="AI78" s="36"/>
       <c r="AJ78" s="36"/>
       <c r="AK78" s="36"/>
-      <c r="AL78" s="36"/>
+      <c r="AL78" s="26"/>
       <c r="AM78" s="26"/>
-      <c r="AN78" s="26"/>
-      <c r="AO78" s="34"/>
+      <c r="AN78" s="34"/>
     </row>
-    <row r="79" spans="1:42">
+    <row r="79" spans="1:41">
       <c r="B79" t="s">
         <v>24</v>
       </c>
@@ -37509,37 +37342,34 @@
       <c r="AI79" s="37"/>
       <c r="AJ79" s="37"/>
       <c r="AK79" s="37"/>
-      <c r="AL79" s="37"/>
+      <c r="AL79" s="35">
+        <v>-6.4514020996561006E-2</v>
+      </c>
       <c r="AM79" s="35">
-        <v>-6.4514020996561006E-2</v>
+        <v>-4.9519025494633398E-2</v>
       </c>
       <c r="AN79" s="35">
-        <v>-4.9519025494633398E-2</v>
-      </c>
-      <c r="AO79" s="35">
         <v>-5.6125117922182097E-2</v>
       </c>
-      <c r="AP79">
+      <c r="AO79">
         <v>-6.2674350059403194E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:42">
+    <row r="80" spans="1:41">
       <c r="AF80" s="37"/>
       <c r="AG80" s="37"/>
       <c r="AH80" s="37"/>
       <c r="AI80" s="37"/>
       <c r="AJ80" s="37"/>
       <c r="AK80" s="37"/>
-      <c r="AL80" s="37"/>
     </row>
-    <row r="81" spans="32:38">
+    <row r="81" spans="32:37">
       <c r="AF81" s="37"/>
       <c r="AG81" s="37"/>
       <c r="AH81" s="37"/>
       <c r="AI81" s="37"/>
       <c r="AJ81" s="37"/>
       <c r="AK81" s="37"/>
-      <c r="AL81" s="37"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="T1:T1048576">
@@ -37552,20 +37382,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{D67F0BD7-0884-5947-AB75-B25881E557C0}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH1:AO1">
-    <cfRule type="dataBar" priority="4">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8182C1BE-9C44-3B4E-9763-3460494E91BE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -37836,6 +37652,20 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AH1:AN1">
+    <cfRule type="dataBar" priority="277">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8182C1BE-9C44-3B4E-9763-3460494E91BE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
@@ -37856,19 +37686,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>T1:T1048576</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8182C1BE-9C44-3B4E-9763-3460494E91BE}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFF555A"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>AH1:AO1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F8DF88AB-CD84-9449-9779-B75363AFFBF5}">
@@ -38048,6 +37865,19 @@
           </x14:cfRule>
           <xm:sqref>AE2:AE78</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8182C1BE-9C44-3B4E-9763-3460494E91BE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AH1:AN1</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -38061,7 +37891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -38099,7 +37929,7 @@
         <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C2" s="41" t="s">
         <v>77</v>
@@ -38185,10 +38015,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="51" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C7" s="41" t="s">
         <v>77</v>
@@ -38205,10 +38035,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="51" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C8" s="54" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
updated aurora and aphira identi.
</commit_message>
<xml_diff>
--- a/PositionInfo/full_Port.xlsx
+++ b/PositionInfo/full_Port.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="24000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="24000"/>
   </bookViews>
   <sheets>
     <sheet name="Id" sheetId="33" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="420">
   <si>
     <t>Name</t>
   </si>
@@ -97,9 +97,6 @@
     <t>barchart</t>
   </si>
   <si>
-    <t>ACBFF</t>
-  </si>
-  <si>
     <t>SPVNF</t>
   </si>
   <si>
@@ -739,9 +736,6 @@
     <t>Aphria Inc</t>
   </si>
   <si>
-    <t>APHQF</t>
-  </si>
-  <si>
     <t>Canopy</t>
   </si>
   <si>
@@ -763,9 +757,6 @@
     <t>Aurora Cannabis Inc</t>
   </si>
   <si>
-    <t>ACBFF</t>
-  </si>
-  <si>
     <t>CA05156X1087</t>
   </si>
   <si>
@@ -1328,6 +1319,12 @@
   </si>
   <si>
     <t>KUSHCO</t>
+  </si>
+  <si>
+    <t>ACB</t>
+  </si>
+  <si>
+    <t>APHA</t>
   </si>
 </sst>
 </file>
@@ -1467,8 +1464,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1647,7 +1648,7 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1670,6 +1671,8 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1692,49 +1695,11 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="103">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1918,6 +1883,26 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3047,6 +3032,26 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
@@ -21285,142 +21290,142 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="RiskTab22" displayName="RiskTab22" ref="A1:N78" totalsRowShown="0" headerRowDxfId="102" dataDxfId="100" headerRowBorderDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="RiskTab22" displayName="RiskTab22" ref="A1:N78" totalsRowShown="0" headerRowDxfId="100" dataDxfId="98" headerRowBorderDxfId="99">
   <tableColumns count="14">
-    <tableColumn id="1" name="Nr." dataDxfId="99" totalsRowDxfId="98"/>
-    <tableColumn id="12" name="Category" totalsRowDxfId="97"/>
-    <tableColumn id="9" name="ShortName" totalsRowDxfId="96"/>
-    <tableColumn id="24" name="Name" dataDxfId="95" totalsRowDxfId="94"/>
-    <tableColumn id="32" name="AlphaVantage" dataDxfId="93" totalsRowDxfId="92"/>
-    <tableColumn id="6" name="AV.length" dataDxfId="91" totalsRowDxfId="90"/>
-    <tableColumn id="10" name="AV.time" dataDxfId="89" totalsRowDxfId="88"/>
-    <tableColumn id="11" name="AV.down" dataDxfId="87" totalsRowDxfId="86"/>
-    <tableColumn id="5" name="barchart" dataDxfId="85" totalsRowDxfId="84"/>
-    <tableColumn id="7" name="barchart.length" dataDxfId="83" totalsRowDxfId="82"/>
-    <tableColumn id="2" name="Bloomberg" dataDxfId="81" totalsRowDxfId="80"/>
-    <tableColumn id="8" name="bloomberg.length" dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="3" name="ISIN" dataDxfId="77" totalsRowDxfId="76"/>
-    <tableColumn id="4" name="WKN" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="1" name="Nr." dataDxfId="97" totalsRowDxfId="96"/>
+    <tableColumn id="12" name="Category" totalsRowDxfId="95"/>
+    <tableColumn id="9" name="ShortName" totalsRowDxfId="94"/>
+    <tableColumn id="24" name="Name" dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="32" name="AlphaVantage" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="6" name="AV.length" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="10" name="AV.time" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="11" name="AV.down" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="5" name="barchart" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="7" name="barchart.length" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="2" name="Bloomberg" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="8" name="bloomberg.length" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="3" name="ISIN" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="4" name="WKN" dataDxfId="73" totalsRowDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2" displayName="Table2" ref="A1:R78" totalsRowShown="0" headerRowDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2" displayName="Table2" ref="A1:R78" totalsRowShown="0" headerRowDxfId="71">
   <autoFilter ref="A1:R78"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="Nr." dataDxfId="72">
+    <tableColumn id="1" name="Nr." dataDxfId="70">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Nr.]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Category" dataDxfId="71">
+    <tableColumn id="16" name="Category" dataDxfId="69">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Category]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="70">
+    <tableColumn id="2" name="Name" dataDxfId="68">
       <calculatedColumnFormula>RiskTab22[[#This Row],[ShortName]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="AlphaVantage" dataDxfId="69">
+    <tableColumn id="13" name="AlphaVantage" dataDxfId="67">
       <calculatedColumnFormula>RiskTab22[[#This Row],[AlphaVantage]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Volume" dataDxfId="68">
+    <tableColumn id="3" name="Volume" dataDxfId="66">
       <calculatedColumnFormula>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="ClosePrice" dataDxfId="67"/>
-    <tableColumn id="14" name="CloseDate" dataDxfId="66"/>
-    <tableColumn id="5" name="Value" dataDxfId="65"/>
-    <tableColumn id="6" name="SharePortfolio" dataDxfId="64"/>
-    <tableColumn id="7" name="1D.logReturn" dataDxfId="63"/>
-    <tableColumn id="15" name="1D.logRetorn.on.portfolio" dataDxfId="62">
+    <tableColumn id="4" name="ClosePrice" dataDxfId="65"/>
+    <tableColumn id="14" name="CloseDate" dataDxfId="64"/>
+    <tableColumn id="5" name="Value" dataDxfId="63"/>
+    <tableColumn id="6" name="SharePortfolio" dataDxfId="62"/>
+    <tableColumn id="7" name="1D.logReturn" dataDxfId="61"/>
+    <tableColumn id="15" name="1D.logRetorn.on.portfolio" dataDxfId="60">
       <calculatedColumnFormula>Table2[[#This Row],[1D.logReturn]]*Table2[[#This Row],[Value]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="1D.return" dataDxfId="61"/>
-    <tableColumn id="9" name="5D.logReturn" dataDxfId="60"/>
-    <tableColumn id="10" name="23D.logReturn" dataDxfId="59"/>
-    <tableColumn id="11" name="125D.logReturn" dataDxfId="58"/>
-    <tableColumn id="12" name="250D.logReturn" dataDxfId="57"/>
-    <tableColumn id="17" name="curr.1D.logReturn" dataDxfId="56"/>
-    <tableColumn id="18" name="curr.Date" dataDxfId="55"/>
+    <tableColumn id="8" name="1D.return" dataDxfId="59"/>
+    <tableColumn id="9" name="5D.logReturn" dataDxfId="58"/>
+    <tableColumn id="10" name="23D.logReturn" dataDxfId="57"/>
+    <tableColumn id="11" name="125D.logReturn" dataDxfId="56"/>
+    <tableColumn id="12" name="250D.logReturn" dataDxfId="55"/>
+    <tableColumn id="17" name="curr.1D.logReturn" dataDxfId="54"/>
+    <tableColumn id="18" name="curr.Date" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table22" displayName="Table22" ref="A1:AN78" totalsRowShown="0" headerRowDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table22" displayName="Table22" ref="A1:AN78" totalsRowShown="0" headerRowDxfId="52">
   <autoFilter ref="A1:AN78"/>
   <sortState ref="A2:Y82">
     <sortCondition descending="1" ref="J1:J75"/>
   </sortState>
   <tableColumns count="40">
-    <tableColumn id="1" name="Nr." dataDxfId="53">
+    <tableColumn id="1" name="Nr." dataDxfId="51">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Nr.]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" name="Category" dataDxfId="52">
+    <tableColumn id="41" name="Category" dataDxfId="50">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Category]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="51">
+    <tableColumn id="2" name="Name" dataDxfId="49">
       <calculatedColumnFormula>RiskTab22[[#This Row],[ShortName]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="AlphaVantage" dataDxfId="50">
+    <tableColumn id="13" name="AlphaVantage" dataDxfId="48">
       <calculatedColumnFormula>RiskTab22[[#This Row],[AlphaVantage]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Value" dataDxfId="49">
+    <tableColumn id="21" name="Value" dataDxfId="47">
       <calculatedColumnFormula>Table2[[#This Row],[Volume]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="SharePortfolio" dataDxfId="48"/>
-    <tableColumn id="14" name="CloseDate" dataDxfId="47"/>
-    <tableColumn id="3" name="Beta1Y" dataDxfId="46"/>
-    <tableColumn id="18" name="Beta" dataDxfId="45"/>
-    <tableColumn id="19" name="250D.logReturn" dataDxfId="44">
+    <tableColumn id="24" name="SharePortfolio" dataDxfId="46"/>
+    <tableColumn id="14" name="CloseDate" dataDxfId="45"/>
+    <tableColumn id="3" name="Beta1Y" dataDxfId="44"/>
+    <tableColumn id="18" name="Beta" dataDxfId="43"/>
+    <tableColumn id="19" name="250D.logReturn" dataDxfId="42">
       <calculatedColumnFormula>Table2[[#This Row],[250D.logReturn]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="250D.CAPM.Return" dataDxfId="43"/>
-    <tableColumn id="22" name="Jensen.Alpha" dataDxfId="42">
+    <tableColumn id="20" name="250D.CAPM.Return" dataDxfId="41"/>
+    <tableColumn id="22" name="Jensen.Alpha" dataDxfId="40">
       <calculatedColumnFormula>Table22[[#This Row],[250D.logReturn]]-Table22[[#This Row],[std_log_returns_1Y]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="std_log_returns_1Y" dataDxfId="41"/>
-    <tableColumn id="5" name="std_log_returns" dataDxfId="40"/>
-    <tableColumn id="37" name="VolaN1_MSGARCH" dataDxfId="39"/>
-    <tableColumn id="6" name="VaR Normal std1Y" dataDxfId="38"/>
-    <tableColumn id="7" name="VaR Normal" dataDxfId="37"/>
-    <tableColumn id="8" name="VaR HS 1Y" dataDxfId="36"/>
-    <tableColumn id="9" name="individual VaR Bootstrap" dataDxfId="35"/>
-    <tableColumn id="10" name="marginal VaR in €" dataDxfId="34"/>
-    <tableColumn id="11" name="incremental VaR" dataDxfId="33"/>
-    <tableColumn id="23" name="incremental VaR to Port VaR (share Portfolio VaR)" dataDxfId="32"/>
-    <tableColumn id="12" name="incremental VaR per Value" dataDxfId="31"/>
-    <tableColumn id="15" name="share Portfolio VaR / share portfolio" dataDxfId="30"/>
-    <tableColumn id="26" name="VaR bootstrap 05Quantile" dataDxfId="29"/>
-    <tableColumn id="25" name="VaR bootstrap 95Quantile" dataDxfId="28"/>
-    <tableColumn id="34" name="VaR_bootstrap" dataDxfId="27"/>
-    <tableColumn id="39" name="ind_VaR_MSGARCH" dataDxfId="26"/>
-    <tableColumn id="33" name="incVaR bootstrap 05Quantile" dataDxfId="25"/>
-    <tableColumn id="32" name="incVaR bootstrap 95Quantile" dataDxfId="24"/>
-    <tableColumn id="31" name="incVaR bootstrap" dataDxfId="23"/>
-    <tableColumn id="30" name="mVaR bootstrap 05Quantile" dataDxfId="22"/>
-    <tableColumn id="29" name="mVaR bootstrap 95Quantile" dataDxfId="21"/>
-    <tableColumn id="16" name="mVaR bootstrap" dataDxfId="20"/>
-    <tableColumn id="27" name="component_VaR" dataDxfId="19"/>
-    <tableColumn id="38" name="MSGARCH_prob" dataDxfId="18"/>
-    <tableColumn id="40" name="ES_MSGARCH" dataDxfId="17"/>
-    <tableColumn id="17" name="ES bootstrap 05Quantile" dataDxfId="16"/>
-    <tableColumn id="35" name="ES bootstrap 95Quantile" dataDxfId="15"/>
-    <tableColumn id="28" name="ES bootstrap" dataDxfId="14"/>
+    <tableColumn id="4" name="std_log_returns_1Y" dataDxfId="39"/>
+    <tableColumn id="5" name="std_log_returns" dataDxfId="38"/>
+    <tableColumn id="37" name="VolaN1_MSGARCH" dataDxfId="37"/>
+    <tableColumn id="6" name="VaR Normal std1Y" dataDxfId="36"/>
+    <tableColumn id="7" name="VaR Normal" dataDxfId="35"/>
+    <tableColumn id="8" name="VaR HS 1Y" dataDxfId="34"/>
+    <tableColumn id="9" name="individual VaR Bootstrap" dataDxfId="33"/>
+    <tableColumn id="10" name="marginal VaR in €" dataDxfId="32"/>
+    <tableColumn id="11" name="incremental VaR" dataDxfId="31"/>
+    <tableColumn id="23" name="incremental VaR to Port VaR (share Portfolio VaR)" dataDxfId="30"/>
+    <tableColumn id="12" name="incremental VaR per Value" dataDxfId="29"/>
+    <tableColumn id="15" name="share Portfolio VaR / share portfolio" dataDxfId="28"/>
+    <tableColumn id="26" name="VaR bootstrap 05Quantile" dataDxfId="27"/>
+    <tableColumn id="25" name="VaR bootstrap 95Quantile" dataDxfId="26"/>
+    <tableColumn id="34" name="VaR_bootstrap" dataDxfId="25"/>
+    <tableColumn id="39" name="ind_VaR_MSGARCH" dataDxfId="24"/>
+    <tableColumn id="33" name="incVaR bootstrap 05Quantile" dataDxfId="23"/>
+    <tableColumn id="32" name="incVaR bootstrap 95Quantile" dataDxfId="22"/>
+    <tableColumn id="31" name="incVaR bootstrap" dataDxfId="21"/>
+    <tableColumn id="30" name="mVaR bootstrap 05Quantile" dataDxfId="20"/>
+    <tableColumn id="29" name="mVaR bootstrap 95Quantile" dataDxfId="19"/>
+    <tableColumn id="16" name="mVaR bootstrap" dataDxfId="18"/>
+    <tableColumn id="27" name="component_VaR" dataDxfId="17"/>
+    <tableColumn id="38" name="MSGARCH_prob" dataDxfId="16"/>
+    <tableColumn id="40" name="ES_MSGARCH" dataDxfId="15"/>
+    <tableColumn id="17" name="ES bootstrap 05Quantile" dataDxfId="14"/>
+    <tableColumn id="35" name="ES bootstrap 95Quantile" dataDxfId="13"/>
+    <tableColumn id="28" name="ES bootstrap" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="DepPositions" displayName="DepPositions" ref="A1:F37" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="DepPositions" displayName="DepPositions" ref="A1:F37" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
   <autoFilter ref="A1:F37"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Name" dataDxfId="9"/>
-    <tableColumn id="2" name="AlphaVantage" dataDxfId="8"/>
-    <tableColumn id="3" name="Deposite" dataDxfId="7"/>
-    <tableColumn id="7" name="Date" dataDxfId="6"/>
-    <tableColumn id="6" name="Price" dataDxfId="5"/>
-    <tableColumn id="4" name="Volume" dataDxfId="4"/>
+    <tableColumn id="1" name="Name" dataDxfId="5"/>
+    <tableColumn id="2" name="AlphaVantage" dataDxfId="4"/>
+    <tableColumn id="3" name="Deposite" dataDxfId="3"/>
+    <tableColumn id="7" name="Date" dataDxfId="2"/>
+    <tableColumn id="6" name="Price" dataDxfId="1"/>
+    <tableColumn id="4" name="Volume" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -21715,11 +21720,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -21742,43 +21747,43 @@
         <v>8</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -21786,16 +21791,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="F2" s="9">
         <v>3884</v>
@@ -21818,16 +21823,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="F3" s="9">
         <v>2637</v>
@@ -21850,16 +21855,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>405</v>
+      </c>
+      <c r="C4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>406</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="C4" t="s">
-        <v>410</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>409</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>411</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="8"/>
@@ -21876,16 +21881,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F5" s="9">
         <v>443</v>
@@ -21903,10 +21908,10 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="N5" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -21914,16 +21919,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="F6" s="9">
         <v>2571</v>
@@ -21948,16 +21953,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C7" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="8"/>
@@ -21974,16 +21979,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="F8" s="9">
         <v>262</v>
@@ -22008,16 +22013,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C9" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="F9" s="9">
         <v>1798</v>
@@ -22042,16 +22047,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="F10" s="9">
         <v>1520</v>
@@ -22069,10 +22074,10 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="N10" s="10" t="s">
         <v>214</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -22080,16 +22085,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C11" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="F11" s="9">
         <v>41</v>
@@ -22112,16 +22117,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C12" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="8"/>
@@ -22138,16 +22143,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="F13" s="9">
         <v>554</v>
@@ -22170,16 +22175,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C14" t="s">
+        <v>221</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>223</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>224</v>
+        <v>419</v>
       </c>
       <c r="F14" s="9">
         <v>882</v>
@@ -22202,16 +22207,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C15" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="F15" s="9">
         <v>1120</v>
@@ -22229,10 +22234,10 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -22240,16 +22245,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>232</v>
+        <v>418</v>
       </c>
       <c r="F16" s="9">
         <v>1054</v>
@@ -22267,10 +22272,10 @@
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -22278,16 +22283,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C17" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F17" s="9">
         <v>2796</v>
@@ -22312,16 +22317,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C18" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F18" s="9">
         <v>1355</v>
@@ -22346,16 +22351,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C19" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="8"/>
@@ -22372,16 +22377,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C20" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="8"/>
@@ -22398,16 +22403,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C21" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F21" s="9">
         <v>1247</v>
@@ -22425,10 +22430,10 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -22436,16 +22441,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C22" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F22" s="9">
         <v>72</v>
@@ -22463,10 +22468,10 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -22474,16 +22479,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C23" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F23" s="9">
         <v>5973</v>
@@ -22499,14 +22504,14 @@
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -22514,16 +22519,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C24" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F24" s="9">
         <v>2459</v>
@@ -22541,10 +22546,10 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -22552,16 +22557,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C25" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F25" s="9">
         <v>2815</v>
@@ -22584,16 +22589,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C26" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F26" s="9">
         <v>2934</v>
@@ -22611,10 +22616,10 @@
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -22622,16 +22627,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C27" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F27" s="9">
         <v>4852</v>
@@ -22654,16 +22659,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C28" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F28" s="9">
         <v>648</v>
@@ -22686,16 +22691,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C29" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F29" s="9">
         <v>425</v>
@@ -22711,10 +22716,10 @@
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="N29" s="10" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -22722,16 +22727,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C30" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F30" s="9">
         <v>923</v>
@@ -22749,10 +22754,10 @@
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
       <c r="M30" s="10" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -22760,16 +22765,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C31" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F31" s="9">
         <v>4053</v>
@@ -22787,10 +22792,10 @@
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
       <c r="M31" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -22798,16 +22803,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C32" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F32" s="9">
         <v>2809</v>
@@ -22825,10 +22830,10 @@
       <c r="K32" s="10"/>
       <c r="L32" s="10"/>
       <c r="M32" s="10" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -22836,16 +22841,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C33" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F33" s="9">
         <v>5654</v>
@@ -22870,16 +22875,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C34" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F34" s="9">
         <v>1898</v>
@@ -22897,10 +22902,10 @@
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="N34" s="10" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -22908,16 +22913,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C35" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D35" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F35" s="9">
         <v>4615</v>
@@ -22935,10 +22940,10 @@
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
       <c r="M35" s="10" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="N35" s="10" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -22946,16 +22951,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C36" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="F36" s="9">
         <v>1172</v>
@@ -22973,10 +22978,10 @@
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
       <c r="M36" s="10" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="N36" s="10" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -22984,16 +22989,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C37" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D37" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F37" s="9">
         <v>2326</v>
@@ -23011,10 +23016,10 @@
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
       <c r="M37" s="10" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="N37" s="10" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -23022,16 +23027,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C38" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D38" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F38" s="9">
         <v>722</v>
@@ -23049,10 +23054,10 @@
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
       <c r="M38" s="10" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="N38" s="10" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -23060,16 +23065,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C39" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D39" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F39" s="9">
         <v>506</v>
@@ -23087,10 +23092,10 @@
       <c r="K39" s="10"/>
       <c r="L39" s="10"/>
       <c r="M39" s="10" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="N39" s="10" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="15" customHeight="1">
@@ -23098,16 +23103,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C40" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F40" s="9">
         <v>506</v>
@@ -23132,16 +23137,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C41" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F41" s="9">
         <v>2052</v>
@@ -23159,10 +23164,10 @@
       <c r="K41" s="10"/>
       <c r="L41" s="10"/>
       <c r="M41" s="10" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="N41" s="10" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1">
@@ -23170,16 +23175,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C42" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F42" s="9">
         <v>1222</v>
@@ -23197,10 +23202,10 @@
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
       <c r="M42" s="10" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="N42" s="10" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15" customHeight="1">
@@ -23208,16 +23213,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C43" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D43" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F43" s="9">
         <v>5653</v>
@@ -23235,10 +23240,10 @@
       <c r="K43" s="10"/>
       <c r="L43" s="10"/>
       <c r="M43" s="10" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="N43" s="10" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -23246,16 +23251,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C44" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F44" s="9">
         <v>1005</v>
@@ -23273,10 +23278,10 @@
       <c r="K44" s="10"/>
       <c r="L44" s="10"/>
       <c r="M44" s="10" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="N44" s="10" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -23284,16 +23289,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C45" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D45" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F45" s="9">
         <v>2484</v>
@@ -23318,16 +23323,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C46" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F46" s="9">
         <v>5969</v>
@@ -23352,16 +23357,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C47" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D47" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F47" s="9">
         <v>1088</v>
@@ -23386,16 +23391,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C48" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F48" s="9">
         <v>443</v>
@@ -23418,16 +23423,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C49" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F49" s="9">
         <v>5973</v>
@@ -23450,16 +23455,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C50" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D50" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F50" s="9">
         <v>5979</v>
@@ -23482,16 +23487,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C51" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D51" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F51" s="9">
         <v>4945</v>
@@ -23514,16 +23519,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C52" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D52" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F52" s="9">
         <v>2691</v>
@@ -23546,16 +23551,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C53" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D53" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F53" s="9">
         <v>5392</v>
@@ -23578,16 +23583,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C54" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D54" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F54" s="9">
         <v>1711</v>
@@ -23610,16 +23615,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C55" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D55" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F55" s="9">
         <v>2835</v>
@@ -23642,16 +23647,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C56" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F56" s="9">
         <v>2178</v>
@@ -23667,10 +23672,10 @@
       <c r="K56" s="10"/>
       <c r="L56" s="10"/>
       <c r="M56" s="10" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="N56" s="10" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="57" spans="1:14">
@@ -23678,16 +23683,16 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C57" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="E57" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="F57" s="9">
         <v>2118</v>
@@ -23710,16 +23715,16 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C58" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" t="s">
         <v>123</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="F58" s="9">
         <v>5654</v>
@@ -23735,10 +23740,10 @@
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
       <c r="M58" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="N58" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="N58" s="10" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -23746,16 +23751,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C59" t="s">
+        <v>127</v>
+      </c>
+      <c r="D59" t="s">
         <v>128</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>130</v>
       </c>
       <c r="F59" s="9">
         <v>5654</v>
@@ -23778,16 +23783,16 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C60" t="s">
+        <v>130</v>
+      </c>
+      <c r="D60" t="s">
         <v>131</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="F60" s="9">
         <v>5654</v>
@@ -23810,16 +23815,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C61" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" t="s">
         <v>134</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="F61" s="9">
         <v>5653</v>
@@ -23842,16 +23847,16 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C62" t="s">
+        <v>136</v>
+      </c>
+      <c r="D62" t="s">
         <v>137</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="F62" s="9">
         <v>5654</v>
@@ -23874,16 +23879,16 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C63" t="s">
+        <v>139</v>
+      </c>
+      <c r="D63" t="s">
         <v>140</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="F63" s="9">
         <v>5654</v>
@@ -23906,16 +23911,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C64" t="s">
+        <v>142</v>
+      </c>
+      <c r="D64" t="s">
         <v>143</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="F64" s="9">
         <v>5654</v>
@@ -23938,16 +23943,16 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C65" t="s">
+        <v>145</v>
+      </c>
+      <c r="D65" t="s">
         <v>146</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="F65" s="9">
         <v>2637</v>
@@ -23970,16 +23975,16 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C66" t="s">
+        <v>148</v>
+      </c>
+      <c r="D66" t="s">
         <v>149</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>151</v>
       </c>
       <c r="F66" s="9">
         <v>5654</v>
@@ -24002,16 +24007,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C67" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" t="s">
         <v>152</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>154</v>
       </c>
       <c r="F67" s="9">
         <v>2103</v>
@@ -24034,16 +24039,16 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C68" t="s">
+        <v>154</v>
+      </c>
+      <c r="D68" t="s">
         <v>155</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="F68" s="9">
         <v>1671</v>
@@ -24066,16 +24071,16 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C69" t="s">
+        <v>157</v>
+      </c>
+      <c r="D69" t="s">
         <v>158</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="F69" s="9">
         <v>1670</v>
@@ -24098,16 +24103,16 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C70" t="s">
+        <v>160</v>
+      </c>
+      <c r="D70" t="s">
         <v>161</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>163</v>
       </c>
       <c r="F70" s="9">
         <v>1672</v>
@@ -24130,16 +24135,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C71" t="s">
+        <v>163</v>
+      </c>
+      <c r="D71" t="s">
         <v>164</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="F71" s="9">
         <v>5654</v>
@@ -24162,16 +24167,16 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C72" t="s">
+        <v>166</v>
+      </c>
+      <c r="D72" t="s">
         <v>167</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>169</v>
       </c>
       <c r="F72" s="9">
         <v>2023</v>
@@ -24194,16 +24199,16 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C73" t="s">
+        <v>169</v>
+      </c>
+      <c r="D73" t="s">
         <v>170</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>172</v>
       </c>
       <c r="F73" s="9">
         <v>5654</v>
@@ -24226,16 +24231,16 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C74" t="s">
+        <v>172</v>
+      </c>
+      <c r="D74" t="s">
         <v>173</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="F74" s="9">
         <v>5654</v>
@@ -24258,16 +24263,16 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C75" t="s">
+        <v>175</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="E75" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="F75" s="9">
         <v>4586</v>
@@ -24290,16 +24295,16 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C76" t="s">
+        <v>178</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="E76" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>181</v>
       </c>
       <c r="F76" s="9">
         <v>3929</v>
@@ -24322,16 +24327,16 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C77" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="E77" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="F77" s="9">
         <v>5969</v>
@@ -24354,16 +24359,16 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C78" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D78" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="E78" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="F78" s="9">
         <v>5969</v>
@@ -24383,12 +24388,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D39:D54 D2:D37">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="102" priority="2">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="101" priority="1">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24461,55 +24466,55 @@
         <v>8</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="P1" s="14" t="s">
-        <v>59</v>
-      </c>
       <c r="Q1" s="14" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="R1" s="14" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -25187,7 +25192,7 @@
       </c>
       <c r="D14" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>APHQF</v>
+        <v>APHA</v>
       </c>
       <c r="E14" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -25299,7 +25304,7 @@
       </c>
       <c r="D16" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>ACBFF</v>
+        <v>ACB</v>
       </c>
       <c r="E16" s="9">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28627,13 +28632,13 @@
     </row>
     <row r="79" spans="1:18">
       <c r="B79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D79" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G79" s="18">
         <v>67886.032783868606</v>
@@ -28721,11 +28726,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG11" sqref="AG11"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -28761,121 +28766,121 @@
         <v>8</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G1" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>64</v>
-      </c>
       <c r="J1" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K1" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="27" t="s">
-        <v>76</v>
-      </c>
       <c r="M1" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="28" t="s">
-        <v>69</v>
-      </c>
       <c r="O1" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="V1" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="W1" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="X1" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y1" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z1" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA1" s="38" t="s">
+        <v>383</v>
+      </c>
+      <c r="AB1" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC1" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD1" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE1" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF1" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG1" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH1" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI1" s="33" t="s">
+        <v>384</v>
+      </c>
+      <c r="AJ1" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="P1" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q1" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="R1" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="S1" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="T1" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="U1" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="V1" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="W1" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="X1" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y1" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z1" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA1" s="38" t="s">
-        <v>386</v>
-      </c>
-      <c r="AB1" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="AC1" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD1" s="27" t="s">
+      <c r="AK1" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="AL1" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM1" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN1" s="27" t="s">
         <v>106</v>
-      </c>
-      <c r="AE1" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="AF1" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="AG1" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="AH1" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI1" s="33" t="s">
-        <v>387</v>
-      </c>
-      <c r="AJ1" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="AK1" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="AL1" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM1" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="AN1" s="27" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:40">
@@ -28900,7 +28905,7 @@
       </c>
       <c r="F2" s="32"/>
       <c r="G2" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H2" s="8">
         <v>1.12368828206889</v>
@@ -29012,7 +29017,7 @@
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -29126,7 +29131,7 @@
         <v>0.109913346657921</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H4" s="8">
         <v>0.87297167555831501</v>
@@ -29244,7 +29249,7 @@
         <v>8.6921534733935393E-2</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H5" s="8">
         <v>1.0174087456408401</v>
@@ -29362,7 +29367,7 @@
         <v>9.9271773636968097E-2</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H6" s="8">
         <v>1.17693038819965</v>
@@ -29480,7 +29485,7 @@
         <v>4.81626540788887E-2</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H7" s="8">
         <v>1.13709000726567</v>
@@ -29598,7 +29603,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H8" s="8">
         <v>2.5273456299036399</v>
@@ -29714,7 +29719,7 @@
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H9" s="8">
         <v>2.2051373821512898</v>
@@ -29812,7 +29817,7 @@
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H10" s="8">
         <v>1.2467095225395199</v>
@@ -29924,7 +29929,7 @@
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H11" s="8">
         <v>0.98314222638481397</v>
@@ -30038,7 +30043,7 @@
         <v>3.3731613845874302E-2</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H12" s="8">
         <v>1.1799630838866699</v>
@@ -30156,7 +30161,7 @@
         <v>2.7541089974481899E-2</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H13" s="8">
         <v>0.972207317430823</v>
@@ -30265,7 +30270,7 @@
       </c>
       <c r="D14" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>APHQF</v>
+        <v>APHA</v>
       </c>
       <c r="E14" s="23">
         <v>2580.2879291251402</v>
@@ -30274,7 +30279,7 @@
         <v>3.8009113558603501E-2</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H14" s="8">
         <v>0.240757381874383</v>
@@ -30392,7 +30397,7 @@
         <v>3.9334475913855901E-2</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H15" s="8">
         <v>0.825346837594228</v>
@@ -30501,7 +30506,7 @@
       </c>
       <c r="D16" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>ACBFF</v>
+        <v>ACB</v>
       </c>
       <c r="E16" s="23">
         <v>334.35556691370601</v>
@@ -30510,7 +30515,7 @@
         <v>4.9252482904429996E-3</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H16" s="8">
         <v>1.49147150508749</v>
@@ -30628,7 +30633,7 @@
         <v>4.2959017577152703E-3</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H17" s="8">
         <v>1.2185902050452899</v>
@@ -30734,7 +30739,7 @@
         <v>2.7312854596122899E-2</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H18" s="8">
         <v>1.2211083293949601</v>
@@ -30850,7 +30855,7 @@
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H19" s="8">
         <v>1.1443476013836</v>
@@ -30956,7 +30961,7 @@
         <v>3.9956625748862702E-3</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="H20" s="8">
         <v>0.89239236712912395</v>
@@ -31072,7 +31077,7 @@
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H21" s="8">
         <v>0.83046656961950804</v>
@@ -31186,7 +31191,7 @@
         <v>1.7480929652102802E-2</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H22" s="8">
         <v>0.93623450006700304</v>
@@ -31302,7 +31307,7 @@
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H23" s="8">
         <v>1.05759506070163</v>
@@ -31414,7 +31419,7 @@
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H24" s="8">
         <v>0.444834654207934</v>
@@ -31526,7 +31531,7 @@
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H25" s="8">
         <v>0.974841869648163</v>
@@ -31636,7 +31641,7 @@
         <v>2.1392141472862499E-2</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H26" s="8">
         <v>0.94417539143017604</v>
@@ -31754,7 +31759,7 @@
         <v>1.35586124944334E-2</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H27" s="8">
         <v>1.2160232560317801</v>
@@ -31872,7 +31877,7 @@
         <v>6.8514281951130704E-3</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H28" s="8">
         <v>1.46228722343879</v>
@@ -31990,7 +31995,7 @@
         <v>6.5820767185414603E-2</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H29" s="8">
         <v>1.56122957897542</v>
@@ -32108,7 +32113,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H30" s="8">
         <v>0.83441990551737599</v>
@@ -32226,7 +32231,7 @@
         <v>4.0885709528287899E-2</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H31" s="8">
         <v>0.85120831730995705</v>
@@ -32344,7 +32349,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H32" s="8">
         <v>0.84868390104259295</v>
@@ -32462,7 +32467,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H33" s="8">
         <v>0.85067922173435295</v>
@@ -32580,7 +32585,7 @@
         <v>9.75832353937615E-2</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H34" s="8">
         <v>0.74948896351660899</v>
@@ -32698,7 +32703,7 @@
         <v>4.34237495772688E-2</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H35" s="8">
         <v>0.72113070519353495</v>
@@ -32816,7 +32821,7 @@
         <v>4.0040449082824899E-2</v>
       </c>
       <c r="G36" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H36" s="8">
         <v>0.99226736652680503</v>
@@ -32934,7 +32939,7 @@
         <v>2.6203073809354001E-2</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H37" s="8">
         <v>1.04787900155383</v>
@@ -33052,7 +33057,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H38" s="8">
         <v>0.891889568527786</v>
@@ -33170,7 +33175,7 @@
         <v>4.0634239526401397E-2</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H39" s="8">
         <v>0.97164603019500595</v>
@@ -33288,7 +33293,7 @@
         <v>1.44609054328393E-2</v>
       </c>
       <c r="G40" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H40" s="8">
         <v>0.99391592339630197</v>
@@ -33406,7 +33411,7 @@
         <v>2.0394417927453199E-2</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H41" s="8">
         <v>1.11950793481483</v>
@@ -33524,7 +33529,7 @@
         <v>1.5556004587761499E-2</v>
       </c>
       <c r="G42" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H42" s="8">
         <v>0.893742288737711</v>
@@ -33642,7 +33647,7 @@
         <v>1.2299066514425199E-2</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H43" s="8">
         <v>1.14576632807677</v>
@@ -33758,7 +33763,7 @@
       </c>
       <c r="F44" s="32"/>
       <c r="G44" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H44" s="8">
         <v>0.745714291714623</v>
@@ -33862,7 +33867,7 @@
       </c>
       <c r="F45" s="32"/>
       <c r="G45" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H45" s="8">
         <v>0.79996196147574405</v>
@@ -33974,7 +33979,7 @@
       </c>
       <c r="F46" s="32"/>
       <c r="G46" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H46" s="8">
         <v>0.89861458008893902</v>
@@ -34086,7 +34091,7 @@
       </c>
       <c r="F47" s="32"/>
       <c r="G47" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H47" s="8">
         <v>0.65930991203202705</v>
@@ -34198,7 +34203,7 @@
       </c>
       <c r="F48" s="32"/>
       <c r="G48" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H48" s="8">
         <v>0.68469966482162203</v>
@@ -34310,7 +34315,7 @@
       </c>
       <c r="F49" s="32"/>
       <c r="G49" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H49" s="8">
         <v>0.54150330634313804</v>
@@ -34422,7 +34427,7 @@
       </c>
       <c r="F50" s="32"/>
       <c r="G50" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H50" s="8">
         <v>0.79363886306440201</v>
@@ -34534,7 +34539,7 @@
       </c>
       <c r="F51" s="32"/>
       <c r="G51" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H51" s="8">
         <v>0.90556270632206104</v>
@@ -34646,7 +34651,7 @@
       </c>
       <c r="F52" s="32"/>
       <c r="G52" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H52" s="8">
         <v>1.1010858007500099</v>
@@ -34758,7 +34763,7 @@
       </c>
       <c r="F53" s="32"/>
       <c r="G53" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H53" s="8">
         <v>1.02908414421475</v>
@@ -34870,7 +34875,7 @@
       </c>
       <c r="F54" s="32"/>
       <c r="G54" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H54" s="8">
         <v>1.18070895548345</v>
@@ -34982,7 +34987,7 @@
       </c>
       <c r="F55" s="32"/>
       <c r="G55" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H55" s="8">
         <v>1.0646858904615899</v>
@@ -35086,7 +35091,7 @@
       </c>
       <c r="F56" s="32"/>
       <c r="G56" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H56" s="8">
         <v>0.73697624882004897</v>
@@ -35194,7 +35199,7 @@
       </c>
       <c r="F57" s="32"/>
       <c r="G57" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H57" s="8">
         <v>0.97373209388793203</v>
@@ -35298,7 +35303,7 @@
       </c>
       <c r="F58" s="32"/>
       <c r="G58" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H58" s="8">
         <v>0.82348543292182497</v>
@@ -35402,7 +35407,7 @@
       </c>
       <c r="F59" s="32"/>
       <c r="G59" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H59" s="8">
         <v>0.71044739526491196</v>
@@ -35506,7 +35511,7 @@
       </c>
       <c r="F60" s="32"/>
       <c r="G60" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H60" s="8">
         <v>0.88280500150088503</v>
@@ -35610,7 +35615,7 @@
       </c>
       <c r="F61" s="32"/>
       <c r="G61" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H61" s="8">
         <v>0.94992351408624698</v>
@@ -35714,7 +35719,7 @@
       </c>
       <c r="F62" s="32"/>
       <c r="G62" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H62" s="8">
         <v>0.74384723319058799</v>
@@ -35818,7 +35823,7 @@
       </c>
       <c r="F63" s="32"/>
       <c r="G63" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H63" s="8">
         <v>0.79549928087643396</v>
@@ -35922,7 +35927,7 @@
       </c>
       <c r="F64" s="32"/>
       <c r="G64" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H64" s="8">
         <v>0.918336577872919</v>
@@ -36026,7 +36031,7 @@
       </c>
       <c r="F65" s="32"/>
       <c r="G65" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H65" s="8">
         <v>0.74869115235934203</v>
@@ -36130,7 +36135,7 @@
       </c>
       <c r="F66" s="32"/>
       <c r="G66" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H66" s="8">
         <v>0.81870913165802095</v>
@@ -36234,7 +36239,7 @@
       </c>
       <c r="F67" s="32"/>
       <c r="G67" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H67" s="8">
         <v>0.70444259758412298</v>
@@ -36338,7 +36343,7 @@
       </c>
       <c r="F68" s="32"/>
       <c r="G68" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H68" s="8">
         <v>0.69566281573555599</v>
@@ -36442,7 +36447,7 @@
       </c>
       <c r="F69" s="32"/>
       <c r="G69" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H69" s="8">
         <v>0.84215929042431903</v>
@@ -36546,7 +36551,7 @@
       </c>
       <c r="F70" s="32"/>
       <c r="G70" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H70" s="8">
         <v>0.970314653413617</v>
@@ -36650,7 +36655,7 @@
       </c>
       <c r="F71" s="32"/>
       <c r="G71" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H71" s="8">
         <v>0.52166898605770895</v>
@@ -36754,7 +36759,7 @@
       </c>
       <c r="F72" s="32"/>
       <c r="G72" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H72" s="8">
         <v>0.84204408186342505</v>
@@ -36858,7 +36863,7 @@
       </c>
       <c r="F73" s="32"/>
       <c r="G73" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H73" s="8">
         <v>0.89658397455462302</v>
@@ -37214,7 +37219,7 @@
       </c>
       <c r="F78" s="32"/>
       <c r="G78" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H78" s="8">
         <v>0.90728925397264404</v>
@@ -37298,13 +37303,13 @@
     </row>
     <row r="79" spans="1:41">
       <c r="B79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D79" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E79">
         <v>67886.032783868606</v>
@@ -37891,8 +37896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -37909,16 +37914,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="39" t="s">
         <v>118</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>119</v>
       </c>
       <c r="F1" s="40" t="s">
         <v>1</v>
@@ -37926,13 +37931,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" s="41"/>
       <c r="E2" s="41"/>
@@ -37942,13 +37947,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41">
@@ -37960,13 +37965,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="C4" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="47">
         <v>43354</v>
@@ -37981,13 +37986,13 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="41"/>
       <c r="E5" s="41"/>
@@ -38005,7 +38010,7 @@
         <v>ITHUF</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="41"/>
@@ -38015,13 +38020,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="51" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" s="47">
         <v>43391</v>
@@ -38035,13 +38040,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="51" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="47">
         <v>43410</v>
@@ -38056,13 +38061,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" s="41"/>
       <c r="E9" s="41"/>
@@ -38072,13 +38077,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="C10" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="41"/>
       <c r="E10" s="41"/>
@@ -38088,13 +38093,13 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>10</v>
+        <v>418</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="41"/>
       <c r="E11" s="41"/>
@@ -38105,13 +38110,13 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="46" t="s">
-        <v>111</v>
-      </c>
       <c r="C12" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="41"/>
       <c r="E12" s="41"/>
@@ -38121,13 +38126,13 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="41"/>
       <c r="E13" s="41"/>
@@ -38137,13 +38142,13 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
@@ -38153,13 +38158,13 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" s="41"/>
       <c r="E15" s="41"/>
@@ -38169,13 +38174,13 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
@@ -38185,13 +38190,13 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="45" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
@@ -38201,11 +38206,11 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="46"/>
       <c r="C18" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" s="41"/>
       <c r="E18" s="41"/>
@@ -38215,13 +38220,13 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="41"/>
       <c r="E19" s="41"/>
@@ -38231,13 +38236,13 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" s="47">
         <v>43201</v>
@@ -38251,13 +38256,13 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="47">
         <v>43196</v>
@@ -38271,13 +38276,13 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="41"/>
       <c r="E22" s="41"/>
@@ -38287,13 +38292,13 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="46" t="s">
-        <v>74</v>
-      </c>
       <c r="C23" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D23" s="41"/>
       <c r="E23" s="41"/>
@@ -38303,13 +38308,13 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
@@ -38319,13 +38324,13 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="43"/>
       <c r="E25" s="43"/>
@@ -38335,13 +38340,13 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
@@ -38351,13 +38356,13 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
@@ -38367,13 +38372,13 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="46" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="41"/>
       <c r="E28" s="41"/>
@@ -38383,13 +38388,13 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D29" s="41"/>
       <c r="E29" s="41"/>
@@ -38399,13 +38404,13 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="46" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="41"/>
       <c r="E30" s="41"/>
@@ -38415,13 +38420,13 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="41"/>
       <c r="E31" s="41"/>
@@ -38431,13 +38436,13 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="46" t="s">
-        <v>80</v>
-      </c>
       <c r="C32" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="41"/>
       <c r="E32" s="41">
@@ -38449,13 +38454,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="46" t="s">
-        <v>87</v>
-      </c>
       <c r="C33" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D33" s="41"/>
       <c r="E33" s="41"/>
@@ -38465,13 +38470,13 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="46" t="s">
-        <v>85</v>
-      </c>
       <c r="C34" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" s="47">
         <v>43335</v>
@@ -38485,13 +38490,13 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="46" t="s">
-        <v>94</v>
-      </c>
       <c r="C35" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="41"/>
       <c r="E35" s="41"/>
@@ -38501,13 +38506,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="46" t="s">
-        <v>92</v>
-      </c>
       <c r="C36" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D36" s="41"/>
       <c r="E36" s="48">
@@ -38519,13 +38524,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D37" s="41"/>
       <c r="E37" s="41"/>
@@ -38535,12 +38540,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A10">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
positions updated and QQQC excluded
</commit_message>
<xml_diff>
--- a/PositionInfo/full_Port.xlsx
+++ b/PositionInfo/full_Port.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="24000"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="24000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Id" sheetId="33" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="417">
   <si>
     <t>Name</t>
   </si>
@@ -1196,15 +1196,6 @@
   </si>
   <si>
     <t>TEL</t>
-  </si>
-  <si>
-    <t>Global X- NASDAQ CHINA</t>
-  </si>
-  <si>
-    <t>Global X NASDAQ China Technology ETF</t>
-  </si>
-  <si>
-    <t>QQQC</t>
   </si>
   <si>
     <t>2018-09-07</t>
@@ -1701,6 +1692,46 @@
   </cellStyles>
   <dxfs count="103">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="0"/>
@@ -1883,26 +1914,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3032,26 +3043,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
@@ -21290,142 +21281,142 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="RiskTab22" displayName="RiskTab22" ref="A1:N78" totalsRowShown="0" headerRowDxfId="100" dataDxfId="98" headerRowBorderDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="RiskTab22" displayName="RiskTab22" ref="A1:N77" totalsRowShown="0" headerRowDxfId="102" dataDxfId="100" headerRowBorderDxfId="101">
   <tableColumns count="14">
-    <tableColumn id="1" name="Nr." dataDxfId="97" totalsRowDxfId="96"/>
-    <tableColumn id="12" name="Category" totalsRowDxfId="95"/>
-    <tableColumn id="9" name="ShortName" totalsRowDxfId="94"/>
-    <tableColumn id="24" name="Name" dataDxfId="93" totalsRowDxfId="92"/>
-    <tableColumn id="32" name="AlphaVantage" dataDxfId="91" totalsRowDxfId="90"/>
-    <tableColumn id="6" name="AV.length" dataDxfId="89" totalsRowDxfId="88"/>
-    <tableColumn id="10" name="AV.time" dataDxfId="87" totalsRowDxfId="86"/>
-    <tableColumn id="11" name="AV.down" dataDxfId="85" totalsRowDxfId="84"/>
-    <tableColumn id="5" name="barchart" dataDxfId="83" totalsRowDxfId="82"/>
-    <tableColumn id="7" name="barchart.length" dataDxfId="81" totalsRowDxfId="80"/>
-    <tableColumn id="2" name="Bloomberg" dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="8" name="bloomberg.length" dataDxfId="77" totalsRowDxfId="76"/>
-    <tableColumn id="3" name="ISIN" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="4" name="WKN" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="1" name="Nr." dataDxfId="99" totalsRowDxfId="98"/>
+    <tableColumn id="12" name="Category" totalsRowDxfId="97"/>
+    <tableColumn id="9" name="ShortName" totalsRowDxfId="96"/>
+    <tableColumn id="24" name="Name" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="32" name="AlphaVantage" dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="6" name="AV.length" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="10" name="AV.time" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="11" name="AV.down" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="5" name="barchart" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="7" name="barchart.length" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="2" name="Bloomberg" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="8" name="bloomberg.length" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="3" name="ISIN" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="4" name="WKN" dataDxfId="75" totalsRowDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2" displayName="Table2" ref="A1:R78" totalsRowShown="0" headerRowDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2" displayName="Table2" ref="A1:R78" totalsRowShown="0" headerRowDxfId="73">
   <autoFilter ref="A1:R78"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="Nr." dataDxfId="70">
+    <tableColumn id="1" name="Nr." dataDxfId="72">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Nr.]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Category" dataDxfId="69">
+    <tableColumn id="16" name="Category" dataDxfId="71">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Category]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="68">
+    <tableColumn id="2" name="Name" dataDxfId="70">
       <calculatedColumnFormula>RiskTab22[[#This Row],[ShortName]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="AlphaVantage" dataDxfId="67">
+    <tableColumn id="13" name="AlphaVantage" dataDxfId="69">
       <calculatedColumnFormula>RiskTab22[[#This Row],[AlphaVantage]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Volume" dataDxfId="66">
+    <tableColumn id="3" name="Volume" dataDxfId="68">
       <calculatedColumnFormula>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="ClosePrice" dataDxfId="65"/>
-    <tableColumn id="14" name="CloseDate" dataDxfId="64"/>
-    <tableColumn id="5" name="Value" dataDxfId="63"/>
-    <tableColumn id="6" name="SharePortfolio" dataDxfId="62"/>
-    <tableColumn id="7" name="1D.logReturn" dataDxfId="61"/>
-    <tableColumn id="15" name="1D.logRetorn.on.portfolio" dataDxfId="60">
+    <tableColumn id="4" name="ClosePrice" dataDxfId="67"/>
+    <tableColumn id="14" name="CloseDate" dataDxfId="66"/>
+    <tableColumn id="5" name="Value" dataDxfId="65"/>
+    <tableColumn id="6" name="SharePortfolio" dataDxfId="64"/>
+    <tableColumn id="7" name="1D.logReturn" dataDxfId="63"/>
+    <tableColumn id="15" name="1D.logRetorn.on.portfolio" dataDxfId="62">
       <calculatedColumnFormula>Table2[[#This Row],[1D.logReturn]]*Table2[[#This Row],[Value]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="1D.return" dataDxfId="59"/>
-    <tableColumn id="9" name="5D.logReturn" dataDxfId="58"/>
-    <tableColumn id="10" name="23D.logReturn" dataDxfId="57"/>
-    <tableColumn id="11" name="125D.logReturn" dataDxfId="56"/>
-    <tableColumn id="12" name="250D.logReturn" dataDxfId="55"/>
-    <tableColumn id="17" name="curr.1D.logReturn" dataDxfId="54"/>
-    <tableColumn id="18" name="curr.Date" dataDxfId="53"/>
+    <tableColumn id="8" name="1D.return" dataDxfId="61"/>
+    <tableColumn id="9" name="5D.logReturn" dataDxfId="60"/>
+    <tableColumn id="10" name="23D.logReturn" dataDxfId="59"/>
+    <tableColumn id="11" name="125D.logReturn" dataDxfId="58"/>
+    <tableColumn id="12" name="250D.logReturn" dataDxfId="57"/>
+    <tableColumn id="17" name="curr.1D.logReturn" dataDxfId="56"/>
+    <tableColumn id="18" name="curr.Date" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table22" displayName="Table22" ref="A1:AN78" totalsRowShown="0" headerRowDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table22" displayName="Table22" ref="A1:AN78" totalsRowShown="0" headerRowDxfId="54">
   <autoFilter ref="A1:AN78"/>
   <sortState ref="A2:Y82">
     <sortCondition descending="1" ref="J1:J75"/>
   </sortState>
   <tableColumns count="40">
-    <tableColumn id="1" name="Nr." dataDxfId="51">
+    <tableColumn id="1" name="Nr." dataDxfId="53">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Nr.]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" name="Category" dataDxfId="50">
+    <tableColumn id="41" name="Category" dataDxfId="52">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Category]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="49">
+    <tableColumn id="2" name="Name" dataDxfId="51">
       <calculatedColumnFormula>RiskTab22[[#This Row],[ShortName]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="AlphaVantage" dataDxfId="48">
+    <tableColumn id="13" name="AlphaVantage" dataDxfId="50">
       <calculatedColumnFormula>RiskTab22[[#This Row],[AlphaVantage]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Value" dataDxfId="47">
+    <tableColumn id="21" name="Value" dataDxfId="49">
       <calculatedColumnFormula>Table2[[#This Row],[Volume]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="SharePortfolio" dataDxfId="46"/>
-    <tableColumn id="14" name="CloseDate" dataDxfId="45"/>
-    <tableColumn id="3" name="Beta1Y" dataDxfId="44"/>
-    <tableColumn id="18" name="Beta" dataDxfId="43"/>
-    <tableColumn id="19" name="250D.logReturn" dataDxfId="42">
+    <tableColumn id="24" name="SharePortfolio" dataDxfId="48"/>
+    <tableColumn id="14" name="CloseDate" dataDxfId="47"/>
+    <tableColumn id="3" name="Beta1Y" dataDxfId="46"/>
+    <tableColumn id="18" name="Beta" dataDxfId="45"/>
+    <tableColumn id="19" name="250D.logReturn" dataDxfId="44">
       <calculatedColumnFormula>Table2[[#This Row],[250D.logReturn]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="250D.CAPM.Return" dataDxfId="41"/>
-    <tableColumn id="22" name="Jensen.Alpha" dataDxfId="40">
+    <tableColumn id="20" name="250D.CAPM.Return" dataDxfId="43"/>
+    <tableColumn id="22" name="Jensen.Alpha" dataDxfId="42">
       <calculatedColumnFormula>Table22[[#This Row],[250D.logReturn]]-Table22[[#This Row],[std_log_returns_1Y]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="std_log_returns_1Y" dataDxfId="39"/>
-    <tableColumn id="5" name="std_log_returns" dataDxfId="38"/>
-    <tableColumn id="37" name="VolaN1_MSGARCH" dataDxfId="37"/>
-    <tableColumn id="6" name="VaR Normal std1Y" dataDxfId="36"/>
-    <tableColumn id="7" name="VaR Normal" dataDxfId="35"/>
-    <tableColumn id="8" name="VaR HS 1Y" dataDxfId="34"/>
-    <tableColumn id="9" name="individual VaR Bootstrap" dataDxfId="33"/>
-    <tableColumn id="10" name="marginal VaR in €" dataDxfId="32"/>
-    <tableColumn id="11" name="incremental VaR" dataDxfId="31"/>
-    <tableColumn id="23" name="incremental VaR to Port VaR (share Portfolio VaR)" dataDxfId="30"/>
-    <tableColumn id="12" name="incremental VaR per Value" dataDxfId="29"/>
-    <tableColumn id="15" name="share Portfolio VaR / share portfolio" dataDxfId="28"/>
-    <tableColumn id="26" name="VaR bootstrap 05Quantile" dataDxfId="27"/>
-    <tableColumn id="25" name="VaR bootstrap 95Quantile" dataDxfId="26"/>
-    <tableColumn id="34" name="VaR_bootstrap" dataDxfId="25"/>
-    <tableColumn id="39" name="ind_VaR_MSGARCH" dataDxfId="24"/>
-    <tableColumn id="33" name="incVaR bootstrap 05Quantile" dataDxfId="23"/>
-    <tableColumn id="32" name="incVaR bootstrap 95Quantile" dataDxfId="22"/>
-    <tableColumn id="31" name="incVaR bootstrap" dataDxfId="21"/>
-    <tableColumn id="30" name="mVaR bootstrap 05Quantile" dataDxfId="20"/>
-    <tableColumn id="29" name="mVaR bootstrap 95Quantile" dataDxfId="19"/>
-    <tableColumn id="16" name="mVaR bootstrap" dataDxfId="18"/>
-    <tableColumn id="27" name="component_VaR" dataDxfId="17"/>
-    <tableColumn id="38" name="MSGARCH_prob" dataDxfId="16"/>
-    <tableColumn id="40" name="ES_MSGARCH" dataDxfId="15"/>
-    <tableColumn id="17" name="ES bootstrap 05Quantile" dataDxfId="14"/>
-    <tableColumn id="35" name="ES bootstrap 95Quantile" dataDxfId="13"/>
-    <tableColumn id="28" name="ES bootstrap" dataDxfId="12"/>
+    <tableColumn id="4" name="std_log_returns_1Y" dataDxfId="41"/>
+    <tableColumn id="5" name="std_log_returns" dataDxfId="40"/>
+    <tableColumn id="37" name="VolaN1_MSGARCH" dataDxfId="39"/>
+    <tableColumn id="6" name="VaR Normal std1Y" dataDxfId="38"/>
+    <tableColumn id="7" name="VaR Normal" dataDxfId="37"/>
+    <tableColumn id="8" name="VaR HS 1Y" dataDxfId="36"/>
+    <tableColumn id="9" name="individual VaR Bootstrap" dataDxfId="35"/>
+    <tableColumn id="10" name="marginal VaR in €" dataDxfId="34"/>
+    <tableColumn id="11" name="incremental VaR" dataDxfId="33"/>
+    <tableColumn id="23" name="incremental VaR to Port VaR (share Portfolio VaR)" dataDxfId="32"/>
+    <tableColumn id="12" name="incremental VaR per Value" dataDxfId="31"/>
+    <tableColumn id="15" name="share Portfolio VaR / share portfolio" dataDxfId="30"/>
+    <tableColumn id="26" name="VaR bootstrap 05Quantile" dataDxfId="29"/>
+    <tableColumn id="25" name="VaR bootstrap 95Quantile" dataDxfId="28"/>
+    <tableColumn id="34" name="VaR_bootstrap" dataDxfId="27"/>
+    <tableColumn id="39" name="ind_VaR_MSGARCH" dataDxfId="26"/>
+    <tableColumn id="33" name="incVaR bootstrap 05Quantile" dataDxfId="25"/>
+    <tableColumn id="32" name="incVaR bootstrap 95Quantile" dataDxfId="24"/>
+    <tableColumn id="31" name="incVaR bootstrap" dataDxfId="23"/>
+    <tableColumn id="30" name="mVaR bootstrap 05Quantile" dataDxfId="22"/>
+    <tableColumn id="29" name="mVaR bootstrap 95Quantile" dataDxfId="21"/>
+    <tableColumn id="16" name="mVaR bootstrap" dataDxfId="20"/>
+    <tableColumn id="27" name="component_VaR" dataDxfId="19"/>
+    <tableColumn id="38" name="MSGARCH_prob" dataDxfId="18"/>
+    <tableColumn id="40" name="ES_MSGARCH" dataDxfId="17"/>
+    <tableColumn id="17" name="ES bootstrap 05Quantile" dataDxfId="16"/>
+    <tableColumn id="35" name="ES bootstrap 95Quantile" dataDxfId="15"/>
+    <tableColumn id="28" name="ES bootstrap" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="DepPositions" displayName="DepPositions" ref="A1:F37" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="DepPositions" displayName="DepPositions" ref="A1:F37" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
   <autoFilter ref="A1:F37"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Name" dataDxfId="5"/>
-    <tableColumn id="2" name="AlphaVantage" dataDxfId="4"/>
-    <tableColumn id="3" name="Deposite" dataDxfId="3"/>
-    <tableColumn id="7" name="Date" dataDxfId="2"/>
-    <tableColumn id="6" name="Price" dataDxfId="1"/>
-    <tableColumn id="4" name="Volume" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="9"/>
+    <tableColumn id="2" name="AlphaVantage" dataDxfId="8"/>
+    <tableColumn id="3" name="Deposite" dataDxfId="7"/>
+    <tableColumn id="7" name="Date" dataDxfId="6"/>
+    <tableColumn id="6" name="Price" dataDxfId="5"/>
+    <tableColumn id="4" name="Volume" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -21718,13 +21709,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N78"/>
+  <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="A56" sqref="A56:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -21747,7 +21738,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>28</v>
@@ -21791,7 +21782,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C2" t="s">
         <v>192</v>
@@ -21823,7 +21814,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C3" t="s">
         <v>195</v>
@@ -21855,16 +21846,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>402</v>
+      </c>
+      <c r="C4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>403</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="C4" t="s">
-        <v>407</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>406</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>408</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="8"/>
@@ -21881,7 +21872,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C5" t="s">
         <v>198</v>
@@ -21890,7 +21881,7 @@
         <v>199</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F5" s="9">
         <v>443</v>
@@ -21919,7 +21910,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C6" t="s">
         <v>202</v>
@@ -21953,16 +21944,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="8"/>
@@ -21979,7 +21970,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C8" t="s">
         <v>205</v>
@@ -22013,10 +22004,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C9" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>208</v>
@@ -22047,7 +22038,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C10" t="s">
         <v>210</v>
@@ -22085,7 +22076,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C11" t="s">
         <v>215</v>
@@ -22117,16 +22108,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C12" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="8"/>
@@ -22143,7 +22134,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C13" t="s">
         <v>218</v>
@@ -22175,7 +22166,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C14" t="s">
         <v>221</v>
@@ -22184,7 +22175,7 @@
         <v>222</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F14" s="9">
         <v>882</v>
@@ -22207,7 +22198,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C15" t="s">
         <v>223</v>
@@ -22245,7 +22236,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C16" t="s">
         <v>228</v>
@@ -22254,7 +22245,7 @@
         <v>229</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="F16" s="9">
         <v>1054</v>
@@ -22283,7 +22274,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C17" t="s">
         <v>232</v>
@@ -22317,7 +22308,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C18" t="s">
         <v>235</v>
@@ -22351,16 +22342,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C19" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="8"/>
@@ -22377,16 +22368,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C20" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="8"/>
@@ -22403,7 +22394,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C21" t="s">
         <v>238</v>
@@ -22441,7 +22432,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C22" t="s">
         <v>243</v>
@@ -22479,7 +22470,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C23" t="s">
         <v>248</v>
@@ -22519,7 +22510,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C24" t="s">
         <v>254</v>
@@ -22557,10 +22548,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C25" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>259</v>
@@ -22589,7 +22580,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C26" t="s">
         <v>261</v>
@@ -22627,7 +22618,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C27" t="s">
         <v>266</v>
@@ -22659,10 +22650,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C28" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>269</v>
@@ -22691,7 +22682,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C29" t="s">
         <v>271</v>
@@ -22727,7 +22718,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C30" t="s">
         <v>276</v>
@@ -22765,7 +22756,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C31" t="s">
         <v>281</v>
@@ -22803,7 +22794,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C32" t="s">
         <v>286</v>
@@ -22841,7 +22832,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C33" t="s">
         <v>291</v>
@@ -22875,7 +22866,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C34" t="s">
         <v>294</v>
@@ -22913,7 +22904,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C35" t="s">
         <v>299</v>
@@ -22951,7 +22942,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C36" t="s">
         <v>304</v>
@@ -22989,7 +22980,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C37" t="s">
         <v>309</v>
@@ -23027,7 +23018,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C38" t="s">
         <v>314</v>
@@ -23065,7 +23056,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C39" t="s">
         <v>319</v>
@@ -23103,7 +23094,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C40" t="s">
         <v>324</v>
@@ -23137,7 +23128,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C41" t="s">
         <v>327</v>
@@ -23175,7 +23166,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C42" t="s">
         <v>332</v>
@@ -23213,7 +23204,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C43" t="s">
         <v>337</v>
@@ -23251,7 +23242,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C44" t="s">
         <v>342</v>
@@ -23289,7 +23280,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C45" t="s">
         <v>345</v>
@@ -23323,7 +23314,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C46" t="s">
         <v>348</v>
@@ -23357,7 +23348,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C47" t="s">
         <v>351</v>
@@ -23391,7 +23382,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C48" t="s">
         <v>354</v>
@@ -23423,7 +23414,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C49" t="s">
         <v>357</v>
@@ -23455,7 +23446,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C50" t="s">
         <v>360</v>
@@ -23487,7 +23478,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C51" t="s">
         <v>363</v>
@@ -23519,7 +23510,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C52" t="s">
         <v>366</v>
@@ -23551,10 +23542,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C53" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D53" t="s">
         <v>369</v>
@@ -23583,7 +23574,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C54" t="s">
         <v>371</v>
@@ -23615,7 +23606,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C55" t="s">
         <v>374</v>
@@ -23644,25 +23635,25 @@
     </row>
     <row r="56" spans="1:14">
       <c r="A56">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C56" t="s">
-        <v>377</v>
+        <v>119</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>378</v>
+        <v>120</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>379</v>
+        <v>121</v>
       </c>
       <c r="F56" s="9">
-        <v>2178</v>
+        <v>2118</v>
       </c>
       <c r="G56" s="8">
-        <v>1.92336082458496</v>
+        <v>21.457866907119801</v>
       </c>
       <c r="H56" s="1" t="b">
         <v>1</v>
@@ -23671,34 +23662,30 @@
       <c r="J56" s="1"/>
       <c r="K56" s="10"/>
       <c r="L56" s="10"/>
-      <c r="M56" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="N56" s="10" t="s">
-        <v>341</v>
-      </c>
+      <c r="M56" s="10"/>
+      <c r="N56" s="10"/>
     </row>
     <row r="57" spans="1:14">
       <c r="A57">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C57" t="s">
-        <v>119</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
+      </c>
+      <c r="D57" t="s">
+        <v>123</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F57" s="9">
-        <v>2118</v>
+        <v>5654</v>
       </c>
       <c r="G57" s="8">
-        <v>21.457866907119801</v>
+        <v>23.4710981845856</v>
       </c>
       <c r="H57" s="1" t="b">
         <v>1</v>
@@ -23707,68 +23694,68 @@
       <c r="J57" s="1"/>
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
-      <c r="M57" s="10"/>
-      <c r="N57" s="10"/>
+      <c r="M57" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="N57" s="10" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="58" spans="1:14">
       <c r="A58">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C58" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D58" t="s">
-        <v>123</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="F58" s="9">
         <v>5654</v>
       </c>
       <c r="G58" s="8">
-        <v>23.4710981845856</v>
-      </c>
-      <c r="H58" s="1" t="b">
+        <v>24.569455862045299</v>
+      </c>
+      <c r="H58" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
-      <c r="M58" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="N58" s="10" t="s">
-        <v>126</v>
-      </c>
+      <c r="M58" s="10"/>
+      <c r="N58" s="10"/>
     </row>
     <row r="59" spans="1:14">
       <c r="A59">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C59" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D59" t="s">
-        <v>128</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>129</v>
+        <v>131</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="F59" s="9">
         <v>5654</v>
       </c>
       <c r="G59" s="8">
-        <v>24.569455862045299</v>
-      </c>
-      <c r="H59" s="6" t="b">
+        <v>22.1242899894714</v>
+      </c>
+      <c r="H59" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I59" s="1"/>
@@ -23780,25 +23767,25 @@
     </row>
     <row r="60" spans="1:14">
       <c r="A60">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C60" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D60" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F60" s="9">
-        <v>5654</v>
+        <v>5653</v>
       </c>
       <c r="G60" s="8">
-        <v>22.1242899894714</v>
+        <v>23.536000967025799</v>
       </c>
       <c r="H60" s="1" t="b">
         <v>1</v>
@@ -23812,25 +23799,25 @@
     </row>
     <row r="61" spans="1:14">
       <c r="A61">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C61" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D61" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F61" s="9">
-        <v>5653</v>
+        <v>5654</v>
       </c>
       <c r="G61" s="8">
-        <v>23.536000967025799</v>
+        <v>23.488318920135502</v>
       </c>
       <c r="H61" s="1" t="b">
         <v>1</v>
@@ -23844,25 +23831,25 @@
     </row>
     <row r="62" spans="1:14">
       <c r="A62">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C62" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D62" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F62" s="9">
         <v>5654</v>
       </c>
       <c r="G62" s="8">
-        <v>23.488318920135502</v>
+        <v>23.720206022262602</v>
       </c>
       <c r="H62" s="1" t="b">
         <v>1</v>
@@ -23876,25 +23863,25 @@
     </row>
     <row r="63" spans="1:14">
       <c r="A63">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C63" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D63" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F63" s="9">
         <v>5654</v>
       </c>
       <c r="G63" s="8">
-        <v>23.720206022262602</v>
+        <v>23.603425025939899</v>
       </c>
       <c r="H63" s="1" t="b">
         <v>1</v>
@@ -23908,25 +23895,25 @@
     </row>
     <row r="64" spans="1:14">
       <c r="A64">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C64" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D64" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F64" s="9">
-        <v>5654</v>
+        <v>2637</v>
       </c>
       <c r="G64" s="8">
-        <v>23.603425025939899</v>
+        <v>21.069594144821199</v>
       </c>
       <c r="H64" s="1" t="b">
         <v>1</v>
@@ -23938,29 +23925,29 @@
       <c r="M64" s="10"/>
       <c r="N64" s="10"/>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" ht="13" customHeight="1">
       <c r="A65">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C65" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D65" t="s">
-        <v>146</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="F65" s="9">
-        <v>2637</v>
+        <v>5654</v>
       </c>
       <c r="G65" s="8">
-        <v>21.069594144821199</v>
-      </c>
-      <c r="H65" s="1" t="b">
+        <v>23.532724857330301</v>
+      </c>
+      <c r="H65" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I65" s="1"/>
@@ -23970,27 +23957,27 @@
       <c r="M65" s="10"/>
       <c r="N65" s="10"/>
     </row>
-    <row r="66" spans="1:14" ht="13" customHeight="1">
+    <row r="66" spans="1:14">
       <c r="A66">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D66" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F66" s="9">
-        <v>5654</v>
+        <v>2103</v>
       </c>
       <c r="G66" s="8">
-        <v>23.532724857330301</v>
+        <v>21.791109085083001</v>
       </c>
       <c r="H66" s="6" t="b">
         <v>1</v>
@@ -24004,25 +23991,25 @@
     </row>
     <row r="67" spans="1:14">
       <c r="A67">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C67" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D67" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F67" s="9">
-        <v>2103</v>
+        <v>1671</v>
       </c>
       <c r="G67" s="8">
-        <v>21.791109085083001</v>
+        <v>21.236869096755999</v>
       </c>
       <c r="H67" s="6" t="b">
         <v>1</v>
@@ -24036,25 +24023,25 @@
     </row>
     <row r="68" spans="1:14">
       <c r="A68">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D68" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F68" s="9">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="G68" s="8">
-        <v>21.236869096755999</v>
+        <v>23.766425848007199</v>
       </c>
       <c r="H68" s="6" t="b">
         <v>1</v>
@@ -24068,25 +24055,25 @@
     </row>
     <row r="69" spans="1:14">
       <c r="A69">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C69" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D69" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F69" s="9">
-        <v>1670</v>
+        <v>1672</v>
       </c>
       <c r="G69" s="8">
-        <v>23.766425848007199</v>
+        <v>21.495878934860201</v>
       </c>
       <c r="H69" s="6" t="b">
         <v>1</v>
@@ -24100,25 +24087,25 @@
     </row>
     <row r="70" spans="1:14">
       <c r="A70">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C70" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D70" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F70" s="9">
-        <v>1672</v>
+        <v>5654</v>
       </c>
       <c r="G70" s="8">
-        <v>21.495878934860201</v>
+        <v>23.8348948955536</v>
       </c>
       <c r="H70" s="6" t="b">
         <v>1</v>
@@ -24132,25 +24119,25 @@
     </row>
     <row r="71" spans="1:14">
       <c r="A71">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C71" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D71" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F71" s="9">
-        <v>5654</v>
+        <v>2023</v>
       </c>
       <c r="G71" s="8">
-        <v>23.8348948955536</v>
+        <v>21.6658070087433</v>
       </c>
       <c r="H71" s="6" t="b">
         <v>1</v>
@@ -24164,25 +24151,25 @@
     </row>
     <row r="72" spans="1:14">
       <c r="A72">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C72" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D72" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F72" s="9">
-        <v>2023</v>
+        <v>5654</v>
       </c>
       <c r="G72" s="8">
-        <v>21.6658070087433</v>
+        <v>21.9390320777893</v>
       </c>
       <c r="H72" s="6" t="b">
         <v>1</v>
@@ -24196,25 +24183,25 @@
     </row>
     <row r="73" spans="1:14">
       <c r="A73">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C73" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D73" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F73" s="9">
         <v>5654</v>
       </c>
       <c r="G73" s="8">
-        <v>21.9390320777893</v>
+        <v>23.7490749359131</v>
       </c>
       <c r="H73" s="6" t="b">
         <v>1</v>
@@ -24228,25 +24215,25 @@
     </row>
     <row r="74" spans="1:14">
       <c r="A74">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C74" t="s">
-        <v>172</v>
-      </c>
-      <c r="D74" t="s">
-        <v>173</v>
+        <v>175</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F74" s="9">
-        <v>5654</v>
+        <v>4586</v>
       </c>
       <c r="G74" s="8">
-        <v>23.7490749359131</v>
+        <v>23.041922092437702</v>
       </c>
       <c r="H74" s="6" t="b">
         <v>1</v>
@@ -24260,25 +24247,25 @@
     </row>
     <row r="75" spans="1:14">
       <c r="A75">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C75" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F75" s="9">
-        <v>4586</v>
+        <v>3929</v>
       </c>
       <c r="G75" s="8">
-        <v>23.041922092437702</v>
+        <v>22.567579030990601</v>
       </c>
       <c r="H75" s="6" t="b">
         <v>1</v>
@@ -24292,25 +24279,25 @@
     </row>
     <row r="76" spans="1:14">
       <c r="A76">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>396</v>
-      </c>
-      <c r="C76" t="s">
-        <v>178</v>
+        <v>393</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F76" s="9">
-        <v>3929</v>
+        <v>5969</v>
       </c>
       <c r="G76" s="8">
-        <v>22.567579030990601</v>
+        <v>22.260892152786301</v>
       </c>
       <c r="H76" s="6" t="b">
         <v>1</v>
@@ -24324,25 +24311,25 @@
     </row>
     <row r="77" spans="1:14">
       <c r="A77">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>183</v>
+        <v>185</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="F77" s="9">
         <v>5969</v>
       </c>
       <c r="G77" s="8">
-        <v>22.260892152786301</v>
+        <v>23.7166090011597</v>
       </c>
       <c r="H77" s="6" t="b">
         <v>1</v>
@@ -24354,46 +24341,14 @@
       <c r="M77" s="10"/>
       <c r="N77" s="10"/>
     </row>
-    <row r="78" spans="1:14">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78" t="s">
-        <v>395</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F78" s="9">
-        <v>5969</v>
-      </c>
-      <c r="G78" s="8">
-        <v>23.7166090011597</v>
-      </c>
-      <c r="H78" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="10"/>
-      <c r="L78" s="10"/>
-      <c r="M78" s="10"/>
-      <c r="N78" s="10"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="D39:D54 D2:D37">
-    <cfRule type="expression" dxfId="102" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="101" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24438,7 +24393,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L17" sqref="L17"/>
+      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -24466,7 +24421,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
@@ -24511,10 +24466,10 @@
         <v>58</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="R1" s="14" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -25308,7 +25263,7 @@
       </c>
       <c r="E16" s="9">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
-        <v>238</v>
+        <v>818</v>
       </c>
       <c r="F16" s="8">
         <v>0</v>
@@ -27480,19 +27435,19 @@
     <row r="56" spans="1:18">
       <c r="A56" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
-        <v>china tech</v>
+        <v>themetic etf</v>
       </c>
       <c r="C56" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>Global X- NASDAQ CHINA</v>
+        <v>Global X - Copper Miners</v>
       </c>
       <c r="D56" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>QQQC</v>
+        <v>COPX</v>
       </c>
       <c r="E56" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -27533,19 +27488,19 @@
     <row r="57" spans="1:18">
       <c r="A57" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
-        <v>themetic etf</v>
+        <v>country etf</v>
       </c>
       <c r="C57" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>Global X - Copper Miners</v>
+        <v>MSCI Germany</v>
       </c>
       <c r="D57" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>COPX</v>
+        <v>EWG</v>
       </c>
       <c r="E57" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -27584,7 +27539,7 @@
     <row r="58" spans="1:18">
       <c r="A58" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -27592,11 +27547,11 @@
       </c>
       <c r="C58" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Germany</v>
+        <v>MSCI United Kingdom</v>
       </c>
       <c r="D58" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWG</v>
+        <v>EWU</v>
       </c>
       <c r="E58" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -27635,7 +27590,7 @@
     <row r="59" spans="1:18">
       <c r="A59" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -27643,11 +27598,11 @@
       </c>
       <c r="C59" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI United Kingdom</v>
+        <v>MSCI Switzerland</v>
       </c>
       <c r="D59" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWU</v>
+        <v>EWL</v>
       </c>
       <c r="E59" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -27686,7 +27641,7 @@
     <row r="60" spans="1:18">
       <c r="A60" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -27694,11 +27649,11 @@
       </c>
       <c r="C60" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Switzerland</v>
+        <v>MSCI Italy</v>
       </c>
       <c r="D60" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWL</v>
+        <v>EWI</v>
       </c>
       <c r="E60" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -27739,7 +27694,7 @@
     <row r="61" spans="1:18">
       <c r="A61" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -27747,11 +27702,11 @@
       </c>
       <c r="C61" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Italy</v>
+        <v>MSCI Sweden</v>
       </c>
       <c r="D61" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWI</v>
+        <v>EWD</v>
       </c>
       <c r="E61" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -27792,7 +27747,7 @@
     <row r="62" spans="1:18">
       <c r="A62" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -27800,11 +27755,11 @@
       </c>
       <c r="C62" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Sweden</v>
+        <v>MSCI Austria</v>
       </c>
       <c r="D62" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWD</v>
+        <v>EWO</v>
       </c>
       <c r="E62" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -27845,7 +27800,7 @@
     <row r="63" spans="1:18">
       <c r="A63" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -27853,11 +27808,11 @@
       </c>
       <c r="C63" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Austria</v>
+        <v>MSCI Netherlands</v>
       </c>
       <c r="D63" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWO</v>
+        <v>EWN</v>
       </c>
       <c r="E63" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -27898,7 +27853,7 @@
     <row r="64" spans="1:18">
       <c r="A64" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -27906,11 +27861,11 @@
       </c>
       <c r="C64" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Netherlands</v>
+        <v>MSCI Israel</v>
       </c>
       <c r="D64" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWN</v>
+        <v>EIS</v>
       </c>
       <c r="E64" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -27951,7 +27906,7 @@
     <row r="65" spans="1:18">
       <c r="A65" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B65" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -27959,11 +27914,11 @@
       </c>
       <c r="C65" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Israel</v>
+        <v>MSCI Belgium</v>
       </c>
       <c r="D65" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EIS</v>
+        <v>EWK</v>
       </c>
       <c r="E65" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28004,7 +27959,7 @@
     <row r="66" spans="1:18">
       <c r="A66" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B66" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -28012,11 +27967,11 @@
       </c>
       <c r="C66" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Belgium</v>
+        <v>MSCI Ireland</v>
       </c>
       <c r="D66" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWK</v>
+        <v>EIRL</v>
       </c>
       <c r="E66" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28057,7 +28012,7 @@
     <row r="67" spans="1:18">
       <c r="A67" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B67" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -28065,11 +28020,11 @@
       </c>
       <c r="C67" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Ireland</v>
+        <v>MSCI Denmark</v>
       </c>
       <c r="D67" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EIRL</v>
+        <v>EDEN</v>
       </c>
       <c r="E67" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28110,7 +28065,7 @@
     <row r="68" spans="1:18">
       <c r="A68" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B68" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -28118,11 +28073,11 @@
       </c>
       <c r="C68" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Denmark</v>
+        <v>MSCI Finland</v>
       </c>
       <c r="D68" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EDEN</v>
+        <v>EFNL</v>
       </c>
       <c r="E68" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28163,7 +28118,7 @@
     <row r="69" spans="1:18">
       <c r="A69" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B69" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -28171,11 +28126,11 @@
       </c>
       <c r="C69" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Finland</v>
+        <v>MSCI Norway</v>
       </c>
       <c r="D69" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EFNL</v>
+        <v>ENOR</v>
       </c>
       <c r="E69" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28216,7 +28171,7 @@
     <row r="70" spans="1:18">
       <c r="A70" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B70" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -28224,11 +28179,11 @@
       </c>
       <c r="C70" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Norway</v>
+        <v>MSCI Japan</v>
       </c>
       <c r="D70" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>ENOR</v>
+        <v>EWJ</v>
       </c>
       <c r="E70" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28269,7 +28224,7 @@
     <row r="71" spans="1:18">
       <c r="A71" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B71" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -28277,11 +28232,11 @@
       </c>
       <c r="C71" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Japan</v>
+        <v>MSCI New Zealand</v>
       </c>
       <c r="D71" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWJ</v>
+        <v>ENZL</v>
       </c>
       <c r="E71" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28322,7 +28277,7 @@
     <row r="72" spans="1:18">
       <c r="A72" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -28330,11 +28285,11 @@
       </c>
       <c r="C72" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI New Zealand</v>
+        <v>MSCI Hong Kong</v>
       </c>
       <c r="D72" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>ENZL</v>
+        <v>EWH</v>
       </c>
       <c r="E72" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28375,7 +28330,7 @@
     <row r="73" spans="1:18">
       <c r="A73" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -28383,11 +28338,11 @@
       </c>
       <c r="C73" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Hong Kong</v>
+        <v>MSCI Australia</v>
       </c>
       <c r="D73" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWH</v>
+        <v>EWA</v>
       </c>
       <c r="E73" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28428,7 +28383,7 @@
     <row r="74" spans="1:18">
       <c r="A74" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -28436,11 +28391,11 @@
       </c>
       <c r="C74" s="50" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Australia</v>
+        <v>MSCI Taiwan</v>
       </c>
       <c r="D74" s="50" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWA</v>
+        <v>EWT</v>
       </c>
       <c r="E74" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28466,7 +28421,7 @@
     <row r="75" spans="1:18">
       <c r="A75" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B75" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -28474,11 +28429,11 @@
       </c>
       <c r="C75" s="50" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Taiwan</v>
+        <v>MSCI South Africa</v>
       </c>
       <c r="D75" s="50" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWT</v>
+        <v>EZA</v>
       </c>
       <c r="E75" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28504,7 +28459,7 @@
     <row r="76" spans="1:18">
       <c r="A76" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B76" s="53" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -28512,11 +28467,11 @@
       </c>
       <c r="C76" s="50" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI South Africa</v>
+        <v>BorgWarner</v>
       </c>
       <c r="D76" s="50" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EZA</v>
+        <v>BWA</v>
       </c>
       <c r="E76" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28542,19 +28497,19 @@
     <row r="77" spans="1:18">
       <c r="A77" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B77" s="53" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
-        <v>country etf</v>
+        <v>e-car</v>
       </c>
       <c r="C77" s="50" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>BorgWarner</v>
+        <v>Magna International</v>
       </c>
       <c r="D77" s="50" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>BWA</v>
+        <v>MAG</v>
       </c>
       <c r="E77" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28578,21 +28533,21 @@
       <c r="R77" s="16"/>
     </row>
     <row r="78" spans="1:18">
-      <c r="A78" s="6">
+      <c r="A78" s="6" t="e">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>77</v>
-      </c>
-      <c r="B78" s="6" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B78" s="6" t="e">
         <f>RiskTab22[[#This Row],[Category]]</f>
-        <v>e-car</v>
-      </c>
-      <c r="C78" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C78" t="e">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>Magna International</v>
-      </c>
-      <c r="D78" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D78" t="e">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>MAG</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E78" s="9" t="str">
         <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
@@ -28766,7 +28721,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>0</v>
@@ -28841,7 +28796,7 @@
         <v>100</v>
       </c>
       <c r="AA1" s="38" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="AB1" s="38" t="s">
         <v>189</v>
@@ -28865,7 +28820,7 @@
         <v>101</v>
       </c>
       <c r="AI1" s="33" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="AJ1" s="33" t="s">
         <v>188</v>
@@ -28905,7 +28860,7 @@
       </c>
       <c r="F2" s="32"/>
       <c r="G2" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H2" s="8">
         <v>1.12368828206889</v>
@@ -29017,7 +28972,7 @@
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -29131,7 +29086,7 @@
         <v>0.109913346657921</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H4" s="8">
         <v>0.87297167555831501</v>
@@ -29249,7 +29204,7 @@
         <v>8.6921534733935393E-2</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H5" s="8">
         <v>1.0174087456408401</v>
@@ -29367,7 +29322,7 @@
         <v>9.9271773636968097E-2</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H6" s="8">
         <v>1.17693038819965</v>
@@ -29485,7 +29440,7 @@
         <v>4.81626540788887E-2</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H7" s="8">
         <v>1.13709000726567</v>
@@ -29603,7 +29558,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H8" s="8">
         <v>2.5273456299036399</v>
@@ -29719,7 +29674,7 @@
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H9" s="8">
         <v>2.2051373821512898</v>
@@ -29817,7 +29772,7 @@
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H10" s="8">
         <v>1.2467095225395199</v>
@@ -29929,7 +29884,7 @@
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H11" s="8">
         <v>0.98314222638481397</v>
@@ -30043,7 +29998,7 @@
         <v>3.3731613845874302E-2</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H12" s="8">
         <v>1.1799630838866699</v>
@@ -30161,7 +30116,7 @@
         <v>2.7541089974481899E-2</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H13" s="8">
         <v>0.972207317430823</v>
@@ -30279,7 +30234,7 @@
         <v>3.8009113558603501E-2</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H14" s="8">
         <v>0.240757381874383</v>
@@ -30397,7 +30352,7 @@
         <v>3.9334475913855901E-2</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H15" s="8">
         <v>0.825346837594228</v>
@@ -30515,7 +30470,7 @@
         <v>4.9252482904429996E-3</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H16" s="8">
         <v>1.49147150508749</v>
@@ -30633,7 +30588,7 @@
         <v>4.2959017577152703E-3</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H17" s="8">
         <v>1.2185902050452899</v>
@@ -30739,7 +30694,7 @@
         <v>2.7312854596122899E-2</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H18" s="8">
         <v>1.2211083293949601</v>
@@ -30855,7 +30810,7 @@
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H19" s="8">
         <v>1.1443476013836</v>
@@ -30961,7 +30916,7 @@
         <v>3.9956625748862702E-3</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="H20" s="8">
         <v>0.89239236712912395</v>
@@ -31077,7 +31032,7 @@
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H21" s="8">
         <v>0.83046656961950804</v>
@@ -31191,7 +31146,7 @@
         <v>1.7480929652102802E-2</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H22" s="8">
         <v>0.93623450006700304</v>
@@ -31307,7 +31262,7 @@
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H23" s="8">
         <v>1.05759506070163</v>
@@ -31419,7 +31374,7 @@
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H24" s="8">
         <v>0.444834654207934</v>
@@ -31531,7 +31486,7 @@
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H25" s="8">
         <v>0.974841869648163</v>
@@ -31641,7 +31596,7 @@
         <v>2.1392141472862499E-2</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H26" s="8">
         <v>0.94417539143017604</v>
@@ -31759,7 +31714,7 @@
         <v>1.35586124944334E-2</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H27" s="8">
         <v>1.2160232560317801</v>
@@ -31877,7 +31832,7 @@
         <v>6.8514281951130704E-3</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H28" s="8">
         <v>1.46228722343879</v>
@@ -31995,7 +31950,7 @@
         <v>6.5820767185414603E-2</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H29" s="8">
         <v>1.56122957897542</v>
@@ -32113,7 +32068,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H30" s="8">
         <v>0.83441990551737599</v>
@@ -32231,7 +32186,7 @@
         <v>4.0885709528287899E-2</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H31" s="8">
         <v>0.85120831730995705</v>
@@ -32349,7 +32304,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H32" s="8">
         <v>0.84868390104259295</v>
@@ -32467,7 +32422,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H33" s="8">
         <v>0.85067922173435295</v>
@@ -32585,7 +32540,7 @@
         <v>9.75832353937615E-2</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H34" s="8">
         <v>0.74948896351660899</v>
@@ -32703,7 +32658,7 @@
         <v>4.34237495772688E-2</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H35" s="8">
         <v>0.72113070519353495</v>
@@ -32821,7 +32776,7 @@
         <v>4.0040449082824899E-2</v>
       </c>
       <c r="G36" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H36" s="8">
         <v>0.99226736652680503</v>
@@ -32939,7 +32894,7 @@
         <v>2.6203073809354001E-2</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H37" s="8">
         <v>1.04787900155383</v>
@@ -33057,7 +33012,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H38" s="8">
         <v>0.891889568527786</v>
@@ -33175,7 +33130,7 @@
         <v>4.0634239526401397E-2</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H39" s="8">
         <v>0.97164603019500595</v>
@@ -33293,7 +33248,7 @@
         <v>1.44609054328393E-2</v>
       </c>
       <c r="G40" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H40" s="8">
         <v>0.99391592339630197</v>
@@ -33411,7 +33366,7 @@
         <v>2.0394417927453199E-2</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H41" s="8">
         <v>1.11950793481483</v>
@@ -33529,7 +33484,7 @@
         <v>1.5556004587761499E-2</v>
       </c>
       <c r="G42" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H42" s="8">
         <v>0.893742288737711</v>
@@ -33647,7 +33602,7 @@
         <v>1.2299066514425199E-2</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H43" s="8">
         <v>1.14576632807677</v>
@@ -33763,7 +33718,7 @@
       </c>
       <c r="F44" s="32"/>
       <c r="G44" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H44" s="8">
         <v>0.745714291714623</v>
@@ -33867,7 +33822,7 @@
       </c>
       <c r="F45" s="32"/>
       <c r="G45" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H45" s="8">
         <v>0.79996196147574405</v>
@@ -33979,7 +33934,7 @@
       </c>
       <c r="F46" s="32"/>
       <c r="G46" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H46" s="8">
         <v>0.89861458008893902</v>
@@ -34091,7 +34046,7 @@
       </c>
       <c r="F47" s="32"/>
       <c r="G47" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H47" s="8">
         <v>0.65930991203202705</v>
@@ -34203,7 +34158,7 @@
       </c>
       <c r="F48" s="32"/>
       <c r="G48" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H48" s="8">
         <v>0.68469966482162203</v>
@@ -34315,7 +34270,7 @@
       </c>
       <c r="F49" s="32"/>
       <c r="G49" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H49" s="8">
         <v>0.54150330634313804</v>
@@ -34427,7 +34382,7 @@
       </c>
       <c r="F50" s="32"/>
       <c r="G50" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H50" s="8">
         <v>0.79363886306440201</v>
@@ -34539,7 +34494,7 @@
       </c>
       <c r="F51" s="32"/>
       <c r="G51" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H51" s="8">
         <v>0.90556270632206104</v>
@@ -34651,7 +34606,7 @@
       </c>
       <c r="F52" s="32"/>
       <c r="G52" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H52" s="8">
         <v>1.1010858007500099</v>
@@ -34763,7 +34718,7 @@
       </c>
       <c r="F53" s="32"/>
       <c r="G53" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H53" s="8">
         <v>1.02908414421475</v>
@@ -34875,7 +34830,7 @@
       </c>
       <c r="F54" s="32"/>
       <c r="G54" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H54" s="8">
         <v>1.18070895548345</v>
@@ -34987,7 +34942,7 @@
       </c>
       <c r="F55" s="32"/>
       <c r="G55" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H55" s="8">
         <v>1.0646858904615899</v>
@@ -35072,26 +35027,26 @@
     <row r="56" spans="1:40">
       <c r="A56" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
-        <v>china tech</v>
+        <v>themetic etf</v>
       </c>
       <c r="C56" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>Global X- NASDAQ CHINA</v>
+        <v>Global X - Copper Miners</v>
       </c>
       <c r="D56" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>QQQC</v>
+        <v>COPX</v>
       </c>
       <c r="E56" s="23">
         <v>0</v>
       </c>
       <c r="F56" s="32"/>
       <c r="G56" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H56" s="8">
         <v>0.73697624882004897</v>
@@ -35180,26 +35135,26 @@
     <row r="57" spans="1:40">
       <c r="A57" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
-        <v>themetic etf</v>
+        <v>country etf</v>
       </c>
       <c r="C57" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>Global X - Copper Miners</v>
+        <v>MSCI Germany</v>
       </c>
       <c r="D57" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>COPX</v>
+        <v>EWG</v>
       </c>
       <c r="E57" s="23">
         <v>0</v>
       </c>
       <c r="F57" s="32"/>
       <c r="G57" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H57" s="8">
         <v>0.97373209388793203</v>
@@ -35284,7 +35239,7 @@
     <row r="58" spans="1:40">
       <c r="A58" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -35292,18 +35247,18 @@
       </c>
       <c r="C58" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Germany</v>
+        <v>MSCI United Kingdom</v>
       </c>
       <c r="D58" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWG</v>
+        <v>EWU</v>
       </c>
       <c r="E58" s="23">
         <v>0</v>
       </c>
       <c r="F58" s="32"/>
       <c r="G58" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H58" s="8">
         <v>0.82348543292182497</v>
@@ -35388,7 +35343,7 @@
     <row r="59" spans="1:40">
       <c r="A59" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -35396,18 +35351,18 @@
       </c>
       <c r="C59" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI United Kingdom</v>
+        <v>MSCI Switzerland</v>
       </c>
       <c r="D59" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWU</v>
+        <v>EWL</v>
       </c>
       <c r="E59" s="23">
         <v>0</v>
       </c>
       <c r="F59" s="32"/>
       <c r="G59" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H59" s="8">
         <v>0.71044739526491196</v>
@@ -35492,7 +35447,7 @@
     <row r="60" spans="1:40">
       <c r="A60" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -35500,18 +35455,18 @@
       </c>
       <c r="C60" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Switzerland</v>
+        <v>MSCI Italy</v>
       </c>
       <c r="D60" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWL</v>
+        <v>EWI</v>
       </c>
       <c r="E60" s="23">
         <v>0</v>
       </c>
       <c r="F60" s="32"/>
       <c r="G60" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H60" s="8">
         <v>0.88280500150088503</v>
@@ -35596,7 +35551,7 @@
     <row r="61" spans="1:40">
       <c r="A61" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -35604,18 +35559,18 @@
       </c>
       <c r="C61" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Italy</v>
+        <v>MSCI Sweden</v>
       </c>
       <c r="D61" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWI</v>
+        <v>EWD</v>
       </c>
       <c r="E61" s="23">
         <v>0</v>
       </c>
       <c r="F61" s="32"/>
       <c r="G61" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H61" s="8">
         <v>0.94992351408624698</v>
@@ -35700,7 +35655,7 @@
     <row r="62" spans="1:40">
       <c r="A62" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -35708,18 +35663,18 @@
       </c>
       <c r="C62" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Sweden</v>
+        <v>MSCI Austria</v>
       </c>
       <c r="D62" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWD</v>
+        <v>EWO</v>
       </c>
       <c r="E62" s="23">
         <v>0</v>
       </c>
       <c r="F62" s="32"/>
       <c r="G62" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H62" s="8">
         <v>0.74384723319058799</v>
@@ -35804,7 +35759,7 @@
     <row r="63" spans="1:40">
       <c r="A63" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -35812,18 +35767,18 @@
       </c>
       <c r="C63" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Austria</v>
+        <v>MSCI Netherlands</v>
       </c>
       <c r="D63" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWO</v>
+        <v>EWN</v>
       </c>
       <c r="E63" s="23">
         <v>0</v>
       </c>
       <c r="F63" s="32"/>
       <c r="G63" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H63" s="8">
         <v>0.79549928087643396</v>
@@ -35908,7 +35863,7 @@
     <row r="64" spans="1:40">
       <c r="A64" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -35916,18 +35871,18 @@
       </c>
       <c r="C64" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Netherlands</v>
+        <v>MSCI Israel</v>
       </c>
       <c r="D64" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWN</v>
+        <v>EIS</v>
       </c>
       <c r="E64" s="23">
         <v>0</v>
       </c>
       <c r="F64" s="32"/>
       <c r="G64" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H64" s="8">
         <v>0.918336577872919</v>
@@ -36012,7 +35967,7 @@
     <row r="65" spans="1:41">
       <c r="A65" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B65" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -36020,18 +35975,18 @@
       </c>
       <c r="C65" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Israel</v>
+        <v>MSCI Belgium</v>
       </c>
       <c r="D65" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EIS</v>
+        <v>EWK</v>
       </c>
       <c r="E65" s="23">
         <v>0</v>
       </c>
       <c r="F65" s="32"/>
       <c r="G65" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H65" s="8">
         <v>0.74869115235934203</v>
@@ -36116,7 +36071,7 @@
     <row r="66" spans="1:41">
       <c r="A66" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B66" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -36124,18 +36079,18 @@
       </c>
       <c r="C66" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Belgium</v>
+        <v>MSCI Ireland</v>
       </c>
       <c r="D66" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWK</v>
+        <v>EIRL</v>
       </c>
       <c r="E66" s="23">
         <v>0</v>
       </c>
       <c r="F66" s="32"/>
       <c r="G66" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H66" s="8">
         <v>0.81870913165802095</v>
@@ -36220,7 +36175,7 @@
     <row r="67" spans="1:41">
       <c r="A67" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B67" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -36228,18 +36183,18 @@
       </c>
       <c r="C67" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Ireland</v>
+        <v>MSCI Denmark</v>
       </c>
       <c r="D67" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EIRL</v>
+        <v>EDEN</v>
       </c>
       <c r="E67" s="23">
         <v>0</v>
       </c>
       <c r="F67" s="32"/>
       <c r="G67" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H67" s="8">
         <v>0.70444259758412298</v>
@@ -36324,7 +36279,7 @@
     <row r="68" spans="1:41">
       <c r="A68" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B68" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -36332,18 +36287,18 @@
       </c>
       <c r="C68" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Denmark</v>
+        <v>MSCI Finland</v>
       </c>
       <c r="D68" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EDEN</v>
+        <v>EFNL</v>
       </c>
       <c r="E68" s="23">
         <v>0</v>
       </c>
       <c r="F68" s="32"/>
       <c r="G68" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H68" s="8">
         <v>0.69566281573555599</v>
@@ -36428,7 +36383,7 @@
     <row r="69" spans="1:41">
       <c r="A69" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B69" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -36436,18 +36391,18 @@
       </c>
       <c r="C69" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Finland</v>
+        <v>MSCI Norway</v>
       </c>
       <c r="D69" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EFNL</v>
+        <v>ENOR</v>
       </c>
       <c r="E69" s="23">
         <v>0</v>
       </c>
       <c r="F69" s="32"/>
       <c r="G69" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H69" s="8">
         <v>0.84215929042431903</v>
@@ -36532,7 +36487,7 @@
     <row r="70" spans="1:41">
       <c r="A70" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B70" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -36540,18 +36495,18 @@
       </c>
       <c r="C70" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Norway</v>
+        <v>MSCI Japan</v>
       </c>
       <c r="D70" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>ENOR</v>
+        <v>EWJ</v>
       </c>
       <c r="E70" s="23">
         <v>0</v>
       </c>
       <c r="F70" s="32"/>
       <c r="G70" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H70" s="8">
         <v>0.970314653413617</v>
@@ -36636,7 +36591,7 @@
     <row r="71" spans="1:41">
       <c r="A71" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B71" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -36644,18 +36599,18 @@
       </c>
       <c r="C71" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Japan</v>
+        <v>MSCI New Zealand</v>
       </c>
       <c r="D71" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWJ</v>
+        <v>ENZL</v>
       </c>
       <c r="E71" s="23">
         <v>0</v>
       </c>
       <c r="F71" s="32"/>
       <c r="G71" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H71" s="8">
         <v>0.52166898605770895</v>
@@ -36740,7 +36695,7 @@
     <row r="72" spans="1:41">
       <c r="A72" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -36748,18 +36703,18 @@
       </c>
       <c r="C72" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI New Zealand</v>
+        <v>MSCI Hong Kong</v>
       </c>
       <c r="D72" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>ENZL</v>
+        <v>EWH</v>
       </c>
       <c r="E72" s="23">
         <v>0</v>
       </c>
       <c r="F72" s="32"/>
       <c r="G72" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H72" s="8">
         <v>0.84204408186342505</v>
@@ -36844,7 +36799,7 @@
     <row r="73" spans="1:41">
       <c r="A73" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -36852,18 +36807,18 @@
       </c>
       <c r="C73" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Hong Kong</v>
+        <v>MSCI Australia</v>
       </c>
       <c r="D73" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWH</v>
+        <v>EWA</v>
       </c>
       <c r="E73" s="23">
         <v>0</v>
       </c>
       <c r="F73" s="32"/>
       <c r="G73" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H73" s="8">
         <v>0.89658397455462302</v>
@@ -36948,7 +36903,7 @@
     <row r="74" spans="1:41">
       <c r="A74" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -36956,11 +36911,11 @@
       </c>
       <c r="C74" s="50" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Australia</v>
+        <v>MSCI Taiwan</v>
       </c>
       <c r="D74" s="50" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWA</v>
+        <v>EWT</v>
       </c>
       <c r="E74" s="23" t="str">
         <f>Table2[[#This Row],[Volume]]</f>
@@ -37011,7 +36966,7 @@
     <row r="75" spans="1:41">
       <c r="A75" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B75" s="6" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -37019,11 +36974,11 @@
       </c>
       <c r="C75" s="50" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI Taiwan</v>
+        <v>MSCI South Africa</v>
       </c>
       <c r="D75" s="50" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EWT</v>
+        <v>EZA</v>
       </c>
       <c r="E75" s="23" t="str">
         <f>Table2[[#This Row],[Volume]]</f>
@@ -37074,7 +37029,7 @@
     <row r="76" spans="1:41">
       <c r="A76" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B76" s="53" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
@@ -37082,11 +37037,11 @@
       </c>
       <c r="C76" s="50" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>MSCI South Africa</v>
+        <v>BorgWarner</v>
       </c>
       <c r="D76" s="50" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>EZA</v>
+        <v>BWA</v>
       </c>
       <c r="E76" s="23" t="str">
         <f>Table2[[#This Row],[Volume]]</f>
@@ -37137,19 +37092,19 @@
     <row r="77" spans="1:41">
       <c r="A77" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B77" s="53" t="str">
         <f>RiskTab22[[#This Row],[Category]]</f>
-        <v>country etf</v>
+        <v>e-car</v>
       </c>
       <c r="C77" s="50" t="str">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>BorgWarner</v>
+        <v>Magna International</v>
       </c>
       <c r="D77" s="50" t="str">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>BWA</v>
+        <v>MAG</v>
       </c>
       <c r="E77" s="23" t="str">
         <f>Table2[[#This Row],[Volume]]</f>
@@ -37198,28 +37153,28 @@
       <c r="AN77" s="34"/>
     </row>
     <row r="78" spans="1:41">
-      <c r="A78" s="6">
+      <c r="A78" s="6" t="e">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
-        <v>77</v>
-      </c>
-      <c r="B78" s="6" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B78" s="6" t="e">
         <f>RiskTab22[[#This Row],[Category]]</f>
-        <v>e-car</v>
-      </c>
-      <c r="C78" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C78" t="e">
         <f>RiskTab22[[#This Row],[ShortName]]</f>
-        <v>Magna International</v>
-      </c>
-      <c r="D78" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D78" t="e">
         <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
-        <v>MAG</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E78" s="23">
         <v>0</v>
       </c>
       <c r="F78" s="32"/>
       <c r="G78" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H78" s="8">
         <v>0.90728925397264404</v>
@@ -37896,8 +37851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -37934,7 +37889,7 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C2" s="41" t="s">
         <v>76</v>
@@ -38020,10 +37975,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="51" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C7" s="41" t="s">
         <v>76</v>
@@ -38040,10 +37995,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="51" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C8" s="54" t="s">
         <v>76</v>
@@ -38096,7 +38051,7 @@
         <v>45</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C11" s="41" t="s">
         <v>76</v>
@@ -38104,8 +38059,7 @@
       <c r="D11" s="41"/>
       <c r="E11" s="41"/>
       <c r="F11" s="42">
-        <f>173+65</f>
-        <v>238</v>
+        <v>818</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -38540,12 +38494,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A10">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
new webscaping emails AU cannbis included to xlsx
</commit_message>
<xml_diff>
--- a/PositionInfo/full_Port.xlsx
+++ b/PositionInfo/full_Port.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="24000" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="24000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Id" sheetId="33" r:id="rId1"/>
@@ -16,7 +16,6 @@
     <sheet name="Performance" sheetId="26" r:id="rId7"/>
     <sheet name="PerformanceBench" sheetId="29" r:id="rId8"/>
     <sheet name="Summary" sheetId="28" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="40" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="Position">Table2[#All]</definedName>
@@ -65,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="433">
   <si>
     <t>Name</t>
   </si>
@@ -1316,6 +1315,54 @@
   </si>
   <si>
     <t>APHA</t>
+  </si>
+  <si>
+    <t>MLCPF</t>
+  </si>
+  <si>
+    <t>Medipharm Labs</t>
+  </si>
+  <si>
+    <t>Medipharm Labs Corp</t>
+  </si>
+  <si>
+    <t>Cannabis AU</t>
+  </si>
+  <si>
+    <t>Auscann Group Holdings Ltd</t>
+  </si>
+  <si>
+    <t>Auscann</t>
+  </si>
+  <si>
+    <t>ACNNF</t>
+  </si>
+  <si>
+    <t>CNGGF</t>
+  </si>
+  <si>
+    <t>Cann Group</t>
+  </si>
+  <si>
+    <t>Cann Group Ltd</t>
+  </si>
+  <si>
+    <t>MMJ Group Holdings Ltd</t>
+  </si>
+  <si>
+    <t>MMJ Group</t>
+  </si>
+  <si>
+    <t>MMJJF</t>
+  </si>
+  <si>
+    <t>Zelda Therapeutics Ltd</t>
+  </si>
+  <si>
+    <t>Zelda Therapeutics</t>
+  </si>
+  <si>
+    <t>ZLDAF</t>
   </si>
 </sst>
 </file>
@@ -1455,7 +1502,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1505,8 +1552,30 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1638,8 +1707,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1664,6 +1734,17 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1688,9 +1769,60 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="103">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1874,26 +2006,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3023,26 +3135,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
@@ -21281,142 +21373,142 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="RiskTab22" displayName="RiskTab22" ref="A1:N77" totalsRowShown="0" headerRowDxfId="100" dataDxfId="98" headerRowBorderDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="RiskTab22" displayName="RiskTab22" ref="A1:N82" totalsRowShown="0" headerRowDxfId="102" dataDxfId="100" headerRowBorderDxfId="101">
   <tableColumns count="14">
-    <tableColumn id="1" name="Nr." dataDxfId="97" totalsRowDxfId="96"/>
-    <tableColumn id="12" name="Category" totalsRowDxfId="95"/>
-    <tableColumn id="9" name="ShortName" totalsRowDxfId="94"/>
-    <tableColumn id="24" name="Name" dataDxfId="93" totalsRowDxfId="92"/>
-    <tableColumn id="32" name="AlphaVantage" dataDxfId="91" totalsRowDxfId="90"/>
-    <tableColumn id="6" name="AV.length" dataDxfId="89" totalsRowDxfId="88"/>
-    <tableColumn id="10" name="AV.time" dataDxfId="87" totalsRowDxfId="86"/>
-    <tableColumn id="11" name="AV.down" dataDxfId="85" totalsRowDxfId="84"/>
-    <tableColumn id="5" name="barchart" dataDxfId="83" totalsRowDxfId="82"/>
-    <tableColumn id="7" name="barchart.length" dataDxfId="81" totalsRowDxfId="80"/>
-    <tableColumn id="2" name="Bloomberg" dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="8" name="bloomberg.length" dataDxfId="77" totalsRowDxfId="76"/>
-    <tableColumn id="3" name="ISIN" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="4" name="WKN" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="1" name="Nr." dataDxfId="99" totalsRowDxfId="98"/>
+    <tableColumn id="12" name="Category" totalsRowDxfId="97"/>
+    <tableColumn id="9" name="ShortName" totalsRowDxfId="96"/>
+    <tableColumn id="24" name="Name" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="32" name="AlphaVantage" dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="6" name="AV.length" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="10" name="AV.time" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="11" name="AV.down" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="5" name="barchart" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="7" name="barchart.length" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="2" name="Bloomberg" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="8" name="bloomberg.length" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="3" name="ISIN" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="4" name="WKN" dataDxfId="75" totalsRowDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2" displayName="Table2" ref="A1:R77" totalsRowShown="0" headerRowDxfId="71">
-  <autoFilter ref="A1:R77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2" displayName="Table2" ref="A1:R82" totalsRowShown="0" headerRowDxfId="73">
+  <autoFilter ref="A1:R82"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="Nr." dataDxfId="70">
+    <tableColumn id="1" name="Nr." dataDxfId="72">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Nr.]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Category" dataDxfId="69">
+    <tableColumn id="16" name="Category" dataDxfId="71">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Category]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="68">
+    <tableColumn id="2" name="Name" dataDxfId="70">
       <calculatedColumnFormula>RiskTab22[[#This Row],[ShortName]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="AlphaVantage" dataDxfId="67">
+    <tableColumn id="13" name="AlphaVantage" dataDxfId="69">
       <calculatedColumnFormula>RiskTab22[[#This Row],[AlphaVantage]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Volume" dataDxfId="66">
+    <tableColumn id="3" name="Volume" dataDxfId="68">
       <calculatedColumnFormula>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="ClosePrice" dataDxfId="65"/>
-    <tableColumn id="14" name="CloseDate" dataDxfId="64"/>
-    <tableColumn id="5" name="Value" dataDxfId="63"/>
-    <tableColumn id="6" name="SharePortfolio" dataDxfId="62"/>
-    <tableColumn id="7" name="1D.logReturn" dataDxfId="61"/>
-    <tableColumn id="15" name="1D.logRetorn.on.portfolio" dataDxfId="60">
+    <tableColumn id="4" name="ClosePrice" dataDxfId="67"/>
+    <tableColumn id="14" name="CloseDate" dataDxfId="66"/>
+    <tableColumn id="5" name="Value" dataDxfId="65"/>
+    <tableColumn id="6" name="SharePortfolio" dataDxfId="64"/>
+    <tableColumn id="7" name="1D.logReturn" dataDxfId="63"/>
+    <tableColumn id="15" name="1D.logRetorn.on.portfolio" dataDxfId="62">
       <calculatedColumnFormula>Table2[[#This Row],[1D.logReturn]]*Table2[[#This Row],[Value]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="1D.return" dataDxfId="59"/>
-    <tableColumn id="9" name="5D.logReturn" dataDxfId="58"/>
-    <tableColumn id="10" name="23D.logReturn" dataDxfId="57"/>
-    <tableColumn id="11" name="125D.logReturn" dataDxfId="56"/>
-    <tableColumn id="12" name="250D.logReturn" dataDxfId="55"/>
-    <tableColumn id="17" name="curr.1D.logReturn" dataDxfId="54"/>
-    <tableColumn id="18" name="curr.Date" dataDxfId="53"/>
+    <tableColumn id="8" name="1D.return" dataDxfId="61"/>
+    <tableColumn id="9" name="5D.logReturn" dataDxfId="60"/>
+    <tableColumn id="10" name="23D.logReturn" dataDxfId="59"/>
+    <tableColumn id="11" name="125D.logReturn" dataDxfId="58"/>
+    <tableColumn id="12" name="250D.logReturn" dataDxfId="57"/>
+    <tableColumn id="17" name="curr.1D.logReturn" dataDxfId="56"/>
+    <tableColumn id="18" name="curr.Date" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table22" displayName="Table22" ref="A1:AN77" totalsRowShown="0" headerRowDxfId="52">
-  <autoFilter ref="A1:AN77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table22" displayName="Table22" ref="A1:AN82" totalsRowShown="0" headerRowDxfId="54">
+  <autoFilter ref="A1:AN82"/>
   <sortState ref="A2:Y82">
     <sortCondition descending="1" ref="J1:J75"/>
   </sortState>
   <tableColumns count="40">
-    <tableColumn id="1" name="Nr." dataDxfId="51">
+    <tableColumn id="1" name="Nr." dataDxfId="53">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Nr.]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" name="Category" dataDxfId="50">
+    <tableColumn id="41" name="Category" dataDxfId="52">
       <calculatedColumnFormula>RiskTab22[[#This Row],[Category]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="49">
+    <tableColumn id="2" name="Name" dataDxfId="51">
       <calculatedColumnFormula>RiskTab22[[#This Row],[ShortName]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="AlphaVantage" dataDxfId="48">
+    <tableColumn id="13" name="AlphaVantage" dataDxfId="50">
       <calculatedColumnFormula>RiskTab22[[#This Row],[AlphaVantage]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Value" dataDxfId="47">
+    <tableColumn id="21" name="Value" dataDxfId="49">
       <calculatedColumnFormula>Table2[[#This Row],[Volume]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="SharePortfolio" dataDxfId="46"/>
-    <tableColumn id="14" name="CloseDate" dataDxfId="45"/>
-    <tableColumn id="3" name="Beta1Y" dataDxfId="44"/>
-    <tableColumn id="18" name="Beta" dataDxfId="43"/>
-    <tableColumn id="19" name="250D.logReturn" dataDxfId="42">
+    <tableColumn id="24" name="SharePortfolio" dataDxfId="48"/>
+    <tableColumn id="14" name="CloseDate" dataDxfId="47"/>
+    <tableColumn id="3" name="Beta1Y" dataDxfId="46"/>
+    <tableColumn id="18" name="Beta" dataDxfId="45"/>
+    <tableColumn id="19" name="250D.logReturn" dataDxfId="44">
       <calculatedColumnFormula>Table2[[#This Row],[250D.logReturn]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="250D.CAPM.Return" dataDxfId="41"/>
-    <tableColumn id="22" name="Jensen.Alpha" dataDxfId="40">
+    <tableColumn id="20" name="250D.CAPM.Return" dataDxfId="43"/>
+    <tableColumn id="22" name="Jensen.Alpha" dataDxfId="42">
       <calculatedColumnFormula>Table22[[#This Row],[250D.logReturn]]-Table22[[#This Row],[std_log_returns_1Y]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="std_log_returns_1Y" dataDxfId="39"/>
-    <tableColumn id="5" name="std_log_returns" dataDxfId="38"/>
-    <tableColumn id="37" name="VolaN1_MSGARCH" dataDxfId="37"/>
-    <tableColumn id="6" name="VaR Normal std1Y" dataDxfId="36"/>
-    <tableColumn id="7" name="VaR Normal" dataDxfId="35"/>
-    <tableColumn id="8" name="VaR HS 1Y" dataDxfId="34"/>
-    <tableColumn id="9" name="individual VaR Bootstrap" dataDxfId="33"/>
-    <tableColumn id="10" name="marginal VaR in €" dataDxfId="32"/>
-    <tableColumn id="11" name="incremental VaR" dataDxfId="31"/>
-    <tableColumn id="23" name="incremental VaR to Port VaR (share Portfolio VaR)" dataDxfId="30"/>
-    <tableColumn id="12" name="incremental VaR per Value" dataDxfId="29"/>
-    <tableColumn id="15" name="share Portfolio VaR / share portfolio" dataDxfId="28"/>
-    <tableColumn id="26" name="VaR bootstrap 05Quantile" dataDxfId="27"/>
-    <tableColumn id="25" name="VaR bootstrap 95Quantile" dataDxfId="26"/>
-    <tableColumn id="34" name="VaR_bootstrap" dataDxfId="25"/>
-    <tableColumn id="39" name="ind_VaR_MSGARCH" dataDxfId="24"/>
-    <tableColumn id="33" name="incVaR bootstrap 05Quantile" dataDxfId="23"/>
-    <tableColumn id="32" name="incVaR bootstrap 95Quantile" dataDxfId="22"/>
-    <tableColumn id="31" name="incVaR bootstrap" dataDxfId="21"/>
-    <tableColumn id="30" name="mVaR bootstrap 05Quantile" dataDxfId="20"/>
-    <tableColumn id="29" name="mVaR bootstrap 95Quantile" dataDxfId="19"/>
-    <tableColumn id="16" name="mVaR bootstrap" dataDxfId="18"/>
-    <tableColumn id="27" name="component_VaR" dataDxfId="17"/>
-    <tableColumn id="38" name="MSGARCH_prob" dataDxfId="16"/>
-    <tableColumn id="40" name="ES_MSGARCH" dataDxfId="15"/>
-    <tableColumn id="17" name="ES bootstrap 05Quantile" dataDxfId="14"/>
-    <tableColumn id="35" name="ES bootstrap 95Quantile" dataDxfId="13"/>
-    <tableColumn id="28" name="ES bootstrap" dataDxfId="12"/>
+    <tableColumn id="4" name="std_log_returns_1Y" dataDxfId="41"/>
+    <tableColumn id="5" name="std_log_returns" dataDxfId="40"/>
+    <tableColumn id="37" name="VolaN1_MSGARCH" dataDxfId="39"/>
+    <tableColumn id="6" name="VaR Normal std1Y" dataDxfId="38"/>
+    <tableColumn id="7" name="VaR Normal" dataDxfId="37"/>
+    <tableColumn id="8" name="VaR HS 1Y" dataDxfId="36"/>
+    <tableColumn id="9" name="individual VaR Bootstrap" dataDxfId="35"/>
+    <tableColumn id="10" name="marginal VaR in €" dataDxfId="34"/>
+    <tableColumn id="11" name="incremental VaR" dataDxfId="33"/>
+    <tableColumn id="23" name="incremental VaR to Port VaR (share Portfolio VaR)" dataDxfId="32"/>
+    <tableColumn id="12" name="incremental VaR per Value" dataDxfId="31"/>
+    <tableColumn id="15" name="share Portfolio VaR / share portfolio" dataDxfId="30"/>
+    <tableColumn id="26" name="VaR bootstrap 05Quantile" dataDxfId="29"/>
+    <tableColumn id="25" name="VaR bootstrap 95Quantile" dataDxfId="28"/>
+    <tableColumn id="34" name="VaR_bootstrap" dataDxfId="27"/>
+    <tableColumn id="39" name="ind_VaR_MSGARCH" dataDxfId="26"/>
+    <tableColumn id="33" name="incVaR bootstrap 05Quantile" dataDxfId="25"/>
+    <tableColumn id="32" name="incVaR bootstrap 95Quantile" dataDxfId="24"/>
+    <tableColumn id="31" name="incVaR bootstrap" dataDxfId="23"/>
+    <tableColumn id="30" name="mVaR bootstrap 05Quantile" dataDxfId="22"/>
+    <tableColumn id="29" name="mVaR bootstrap 95Quantile" dataDxfId="21"/>
+    <tableColumn id="16" name="mVaR bootstrap" dataDxfId="20"/>
+    <tableColumn id="27" name="component_VaR" dataDxfId="19"/>
+    <tableColumn id="38" name="MSGARCH_prob" dataDxfId="18"/>
+    <tableColumn id="40" name="ES_MSGARCH" dataDxfId="17"/>
+    <tableColumn id="17" name="ES bootstrap 05Quantile" dataDxfId="16"/>
+    <tableColumn id="35" name="ES bootstrap 95Quantile" dataDxfId="15"/>
+    <tableColumn id="28" name="ES bootstrap" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="DepPositions" displayName="DepPositions" ref="A1:F37" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
-  <autoFilter ref="A1:F37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="DepPositions" displayName="DepPositions" ref="A1:F38" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
+  <autoFilter ref="A1:F38"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Name" dataDxfId="5"/>
-    <tableColumn id="2" name="AlphaVantage" dataDxfId="4"/>
-    <tableColumn id="3" name="Deposite" dataDxfId="3"/>
-    <tableColumn id="7" name="Date" dataDxfId="2"/>
-    <tableColumn id="6" name="Price" dataDxfId="1"/>
-    <tableColumn id="4" name="Volume" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="9"/>
+    <tableColumn id="2" name="AlphaVantage" dataDxfId="8"/>
+    <tableColumn id="3" name="Deposite" dataDxfId="7"/>
+    <tableColumn id="7" name="Date" dataDxfId="6"/>
+    <tableColumn id="6" name="Price" dataDxfId="5"/>
+    <tableColumn id="4" name="Volume" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -21709,13 +21801,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N77"/>
+  <dimension ref="A1:N82"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -24341,14 +24433,135 @@
       <c r="M77" s="10"/>
       <c r="N77" s="10"/>
     </row>
+    <row r="78" spans="1:14">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>389</v>
+      </c>
+      <c r="C78" t="s">
+        <v>418</v>
+      </c>
+      <c r="D78" s="55" t="s">
+        <v>419</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="F78" s="9"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="10"/>
+      <c r="L78" s="10"/>
+      <c r="M78" s="10"/>
+      <c r="N78" s="10"/>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>420</v>
+      </c>
+      <c r="C79" t="s">
+        <v>422</v>
+      </c>
+      <c r="D79" t="s">
+        <v>421</v>
+      </c>
+      <c r="E79" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="A80" s="55">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>420</v>
+      </c>
+      <c r="C80" t="s">
+        <v>425</v>
+      </c>
+      <c r="D80" t="s">
+        <v>426</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="F80" s="9"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="10"/>
+      <c r="L80" s="10"/>
+      <c r="M80" s="10"/>
+      <c r="N80" s="10"/>
+    </row>
+    <row r="81" spans="1:14">
+      <c r="A81" s="55">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>420</v>
+      </c>
+      <c r="C81" t="s">
+        <v>431</v>
+      </c>
+      <c r="D81" s="55" t="s">
+        <v>430</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="F81" s="9"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="10"/>
+      <c r="L81" s="10"/>
+      <c r="M81" s="10"/>
+      <c r="N81" s="10"/>
+    </row>
+    <row r="82" spans="1:14">
+      <c r="A82" s="55">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>420</v>
+      </c>
+      <c r="C82" t="s">
+        <v>428</v>
+      </c>
+      <c r="D82" t="s">
+        <v>427</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="F82" s="9"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="10"/>
+      <c r="L82" s="10"/>
+      <c r="M82" s="10"/>
+      <c r="N82" s="10"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D39:D54 D2:D37">
-    <cfRule type="expression" dxfId="102" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="101" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24367,33 +24580,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R94"/>
+  <dimension ref="A1:R99"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A78" sqref="A78:XFD78"/>
+      <selection pane="bottomRight" activeCell="A77" sqref="A77:XFD77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -28533,74 +28728,265 @@
       <c r="R77" s="16"/>
     </row>
     <row r="78" spans="1:18">
-      <c r="B78" t="s">
-        <v>23</v>
-      </c>
-      <c r="C78" t="s">
-        <v>23</v>
-      </c>
-      <c r="D78" t="s">
-        <v>190</v>
-      </c>
-      <c r="G78" s="18">
-        <v>67886.032783868606</v>
-      </c>
+      <c r="A78" s="6">
+        <f>RiskTab22[[#This Row],[Nr.]]</f>
+        <v>78</v>
+      </c>
+      <c r="B78" s="53" t="str">
+        <f>RiskTab22[[#This Row],[Category]]</f>
+        <v>Cannabis CA</v>
+      </c>
+      <c r="C78" s="50" t="str">
+        <f>RiskTab22[[#This Row],[ShortName]]</f>
+        <v>Medipharm Labs</v>
+      </c>
+      <c r="D78" s="50" t="str">
+        <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
+        <v>MLCPF</v>
+      </c>
+      <c r="E78" s="9">
+        <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
+        <v>450</v>
+      </c>
+      <c r="F78" s="8"/>
+      <c r="G78" s="19"/>
       <c r="H78" s="8"/>
-      <c r="I78">
-        <v>-1.15529696622444E-2</v>
-      </c>
+      <c r="I78" s="16"/>
       <c r="J78" s="16"/>
-      <c r="K78" s="16"/>
-      <c r="L78">
-        <v>6.5303597307905706E-2</v>
-      </c>
-      <c r="M78" s="16">
-        <v>0.15956514555913101</v>
-      </c>
-      <c r="N78" s="16">
-        <v>0.31889865259688399</v>
-      </c>
-      <c r="O78" s="16">
-        <v>0.61781896806311198</v>
-      </c>
-      <c r="P78" s="16">
-        <v>0.61781896806311198</v>
-      </c>
+      <c r="K78" s="16">
+        <f>Table2[[#This Row],[1D.logReturn]]*Table2[[#This Row],[Value]]</f>
+        <v>0</v>
+      </c>
+      <c r="L78" s="8"/>
+      <c r="M78" s="16"/>
+      <c r="N78" s="16"/>
+      <c r="O78" s="16"/>
+      <c r="P78" s="16"/>
+      <c r="Q78" s="16"/>
+      <c r="R78" s="16"/>
     </row>
     <row r="79" spans="1:18">
+      <c r="A79" s="6">
+        <f>RiskTab22[[#This Row],[Nr.]]</f>
+        <v>79</v>
+      </c>
+      <c r="B79" s="53" t="str">
+        <f>RiskTab22[[#This Row],[Category]]</f>
+        <v>Cannabis AU</v>
+      </c>
+      <c r="C79" s="50" t="str">
+        <f>RiskTab22[[#This Row],[ShortName]]</f>
+        <v>Auscann</v>
+      </c>
+      <c r="D79" s="50" t="str">
+        <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
+        <v>ACNNF</v>
+      </c>
+      <c r="E79" s="9" t="str">
+        <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
+        <v/>
+      </c>
+      <c r="F79" s="8"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="16"/>
       <c r="J79" s="16"/>
-      <c r="K79" s="16"/>
+      <c r="K79" s="16">
+        <f>Table2[[#This Row],[1D.logReturn]]*Table2[[#This Row],[Value]]</f>
+        <v>0</v>
+      </c>
+      <c r="L79" s="8"/>
+      <c r="M79" s="16"/>
+      <c r="N79" s="16"/>
+      <c r="O79" s="16"/>
+      <c r="P79" s="16"/>
+      <c r="Q79" s="16"/>
+      <c r="R79" s="16"/>
     </row>
     <row r="80" spans="1:18">
-      <c r="H80" s="24"/>
+      <c r="A80" s="6">
+        <f>RiskTab22[[#This Row],[Nr.]]</f>
+        <v>80</v>
+      </c>
+      <c r="B80" s="53" t="str">
+        <f>RiskTab22[[#This Row],[Category]]</f>
+        <v>Cannabis AU</v>
+      </c>
+      <c r="C80" s="50" t="str">
+        <f>RiskTab22[[#This Row],[ShortName]]</f>
+        <v>Cann Group</v>
+      </c>
+      <c r="D80" s="50" t="str">
+        <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
+        <v>CNGGF</v>
+      </c>
+      <c r="E80" s="9" t="str">
+        <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
+        <v/>
+      </c>
+      <c r="F80" s="8"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="16"/>
+      <c r="J80" s="16"/>
+      <c r="K80" s="16">
+        <f>Table2[[#This Row],[1D.logReturn]]*Table2[[#This Row],[Value]]</f>
+        <v>0</v>
+      </c>
+      <c r="L80" s="8"/>
+      <c r="M80" s="16"/>
+      <c r="N80" s="16"/>
+      <c r="O80" s="16"/>
+      <c r="P80" s="16"/>
+      <c r="Q80" s="16"/>
+      <c r="R80" s="16"/>
     </row>
-    <row r="81" spans="8:10">
-      <c r="H81" s="24"/>
+    <row r="81" spans="1:18">
+      <c r="A81" s="6">
+        <f>RiskTab22[[#This Row],[Nr.]]</f>
+        <v>81</v>
+      </c>
+      <c r="B81" s="53" t="str">
+        <f>RiskTab22[[#This Row],[Category]]</f>
+        <v>Cannabis AU</v>
+      </c>
+      <c r="C81" s="50" t="str">
+        <f>RiskTab22[[#This Row],[ShortName]]</f>
+        <v>Zelda Therapeutics</v>
+      </c>
+      <c r="D81" s="50" t="str">
+        <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
+        <v>ZLDAF</v>
+      </c>
+      <c r="E81" s="9" t="str">
+        <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
+        <v/>
+      </c>
+      <c r="F81" s="8"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="8"/>
       <c r="I81" s="16"/>
-      <c r="J81" s="22"/>
+      <c r="J81" s="16"/>
+      <c r="K81" s="16">
+        <f>Table2[[#This Row],[1D.logReturn]]*Table2[[#This Row],[Value]]</f>
+        <v>0</v>
+      </c>
+      <c r="L81" s="8"/>
+      <c r="M81" s="16"/>
+      <c r="N81" s="16"/>
+      <c r="O81" s="16"/>
+      <c r="P81" s="16"/>
+      <c r="Q81" s="16"/>
+      <c r="R81" s="16"/>
     </row>
-    <row r="82" spans="8:10">
-      <c r="H82" s="24"/>
+    <row r="82" spans="1:18">
+      <c r="A82" s="6">
+        <f>RiskTab22[[#This Row],[Nr.]]</f>
+        <v>82</v>
+      </c>
+      <c r="B82" s="53" t="str">
+        <f>RiskTab22[[#This Row],[Category]]</f>
+        <v>Cannabis AU</v>
+      </c>
+      <c r="C82" s="50" t="str">
+        <f>RiskTab22[[#This Row],[ShortName]]</f>
+        <v>MMJ Group</v>
+      </c>
+      <c r="D82" s="50" t="str">
+        <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
+        <v>MMJJF</v>
+      </c>
+      <c r="E82" s="9" t="str">
+        <f>IFERROR(INDEX(DepPositions[Volume],MATCH(Table2[[#This Row],[AlphaVantage]],DepPositions[AlphaVantage],0)),"")</f>
+        <v/>
+      </c>
+      <c r="F82" s="8"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="8"/>
       <c r="I82" s="16"/>
-      <c r="J82" s="22"/>
+      <c r="J82" s="16"/>
+      <c r="K82" s="16">
+        <f>Table2[[#This Row],[1D.logReturn]]*Table2[[#This Row],[Value]]</f>
+        <v>0</v>
+      </c>
+      <c r="L82" s="8"/>
+      <c r="M82" s="16"/>
+      <c r="N82" s="16"/>
+      <c r="O82" s="16"/>
+      <c r="P82" s="16"/>
+      <c r="Q82" s="16"/>
+      <c r="R82" s="16"/>
     </row>
-    <row r="83" spans="8:10">
-      <c r="H83" s="23"/>
-      <c r="I83" s="16"/>
+    <row r="83" spans="1:18">
+      <c r="B83" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" t="s">
+        <v>23</v>
+      </c>
+      <c r="D83" t="s">
+        <v>190</v>
+      </c>
+      <c r="G83" s="18">
+        <v>67886.032783868606</v>
+      </c>
+      <c r="H83" s="8"/>
+      <c r="I83">
+        <v>-1.15529696622444E-2</v>
+      </c>
+      <c r="J83" s="16"/>
+      <c r="K83" s="16"/>
+      <c r="L83">
+        <v>6.5303597307905706E-2</v>
+      </c>
+      <c r="M83" s="16">
+        <v>0.15956514555913101</v>
+      </c>
+      <c r="N83" s="16">
+        <v>0.31889865259688399</v>
+      </c>
+      <c r="O83" s="16">
+        <v>0.61781896806311198</v>
+      </c>
+      <c r="P83" s="16">
+        <v>0.61781896806311198</v>
+      </c>
     </row>
-    <row r="84" spans="8:10">
-      <c r="I84" s="16"/>
-      <c r="J84" s="22"/>
+    <row r="84" spans="1:18">
+      <c r="J84" s="16"/>
+      <c r="K84" s="16"/>
     </row>
-    <row r="85" spans="8:10">
-      <c r="J85" s="22"/>
+    <row r="85" spans="1:18">
+      <c r="H85" s="24"/>
     </row>
-    <row r="94" spans="8:10" ht="43" customHeight="1">
-      <c r="H94" s="21"/>
+    <row r="86" spans="1:18">
+      <c r="H86" s="24"/>
+      <c r="I86" s="16"/>
+      <c r="J86" s="22"/>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="H87" s="24"/>
+      <c r="I87" s="16"/>
+      <c r="J87" s="22"/>
+    </row>
+    <row r="88" spans="1:18">
+      <c r="H88" s="23"/>
+      <c r="I88" s="16"/>
+    </row>
+    <row r="89" spans="1:18">
+      <c r="I89" s="16"/>
+      <c r="J89" s="22"/>
+    </row>
+    <row r="90" spans="1:18">
+      <c r="J90" s="22"/>
+    </row>
+    <row r="98" spans="8:8" ht="43" customHeight="1"/>
+    <row r="99" spans="8:8" ht="43">
+      <c r="H99" s="21"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:K77">
-    <cfRule type="colorScale" priority="278">
+  <conditionalFormatting sqref="J2:K82">
+    <cfRule type="colorScale" priority="306">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -28626,13 +29012,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO80"/>
+  <dimension ref="A1:AO85"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E48" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A78" sqref="A78:XFD78"/>
+      <selection pane="bottomRight" activeCell="A79" sqref="A79:XFD79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -35911,7 +36297,7 @@
       <c r="AM64" s="26"/>
       <c r="AN64" s="34"/>
     </row>
-    <row r="65" spans="1:41">
+    <row r="65" spans="1:40">
       <c r="A65" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>65</v>
@@ -36015,7 +36401,7 @@
       <c r="AM65" s="26"/>
       <c r="AN65" s="34"/>
     </row>
-    <row r="66" spans="1:41">
+    <row r="66" spans="1:40">
       <c r="A66" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>66</v>
@@ -36119,7 +36505,7 @@
       <c r="AM66" s="26"/>
       <c r="AN66" s="34"/>
     </row>
-    <row r="67" spans="1:41">
+    <row r="67" spans="1:40">
       <c r="A67" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>67</v>
@@ -36223,7 +36609,7 @@
       <c r="AM67" s="26"/>
       <c r="AN67" s="34"/>
     </row>
-    <row r="68" spans="1:41">
+    <row r="68" spans="1:40">
       <c r="A68" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>68</v>
@@ -36327,7 +36713,7 @@
       <c r="AM68" s="26"/>
       <c r="AN68" s="34"/>
     </row>
-    <row r="69" spans="1:41">
+    <row r="69" spans="1:40">
       <c r="A69" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>69</v>
@@ -36431,7 +36817,7 @@
       <c r="AM69" s="26"/>
       <c r="AN69" s="34"/>
     </row>
-    <row r="70" spans="1:41">
+    <row r="70" spans="1:40">
       <c r="A70" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>70</v>
@@ -36535,7 +36921,7 @@
       <c r="AM70" s="26"/>
       <c r="AN70" s="34"/>
     </row>
-    <row r="71" spans="1:41">
+    <row r="71" spans="1:40">
       <c r="A71" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>71</v>
@@ -36639,7 +37025,7 @@
       <c r="AM71" s="26"/>
       <c r="AN71" s="34"/>
     </row>
-    <row r="72" spans="1:41">
+    <row r="72" spans="1:40">
       <c r="A72" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>72</v>
@@ -36743,7 +37129,7 @@
       <c r="AM72" s="26"/>
       <c r="AN72" s="34"/>
     </row>
-    <row r="73" spans="1:41">
+    <row r="73" spans="1:40">
       <c r="A73" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>73</v>
@@ -36847,7 +37233,7 @@
       <c r="AM73" s="26"/>
       <c r="AN73" s="34"/>
     </row>
-    <row r="74" spans="1:41">
+    <row r="74" spans="1:40">
       <c r="A74" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>74</v>
@@ -36910,7 +37296,7 @@
       <c r="AM74" s="26"/>
       <c r="AN74" s="34"/>
     </row>
-    <row r="75" spans="1:41">
+    <row r="75" spans="1:40">
       <c r="A75" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>75</v>
@@ -36973,7 +37359,7 @@
       <c r="AM75" s="26"/>
       <c r="AN75" s="34"/>
     </row>
-    <row r="76" spans="1:41">
+    <row r="76" spans="1:40">
       <c r="A76" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>76</v>
@@ -37036,7 +37422,7 @@
       <c r="AM76" s="26"/>
       <c r="AN76" s="34"/>
     </row>
-    <row r="77" spans="1:41">
+    <row r="77" spans="1:40">
       <c r="A77" s="6">
         <f>RiskTab22[[#This Row],[Nr.]]</f>
         <v>77</v>
@@ -37099,80 +37485,395 @@
       <c r="AM77" s="26"/>
       <c r="AN77" s="34"/>
     </row>
-    <row r="78" spans="1:41">
-      <c r="B78" t="s">
+    <row r="78" spans="1:40">
+      <c r="A78" s="6">
+        <f>RiskTab22[[#This Row],[Nr.]]</f>
+        <v>78</v>
+      </c>
+      <c r="B78" s="53" t="str">
+        <f>RiskTab22[[#This Row],[Category]]</f>
+        <v>Cannabis CA</v>
+      </c>
+      <c r="C78" s="50" t="str">
+        <f>RiskTab22[[#This Row],[ShortName]]</f>
+        <v>Medipharm Labs</v>
+      </c>
+      <c r="D78" s="50" t="str">
+        <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
+        <v>MLCPF</v>
+      </c>
+      <c r="E78" s="23">
+        <f>Table2[[#This Row],[Volume]]</f>
+        <v>450</v>
+      </c>
+      <c r="F78" s="32"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="16">
+        <f>Table2[[#This Row],[250D.logReturn]]</f>
+        <v>0</v>
+      </c>
+      <c r="K78" s="16"/>
+      <c r="L78" s="16">
+        <f>Table22[[#This Row],[250D.logReturn]]-Table22[[#This Row],[std_log_returns_1Y]]</f>
+        <v>0</v>
+      </c>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+      <c r="S78" s="26"/>
+      <c r="T78" s="30"/>
+      <c r="U78" s="26"/>
+      <c r="V78" s="16"/>
+      <c r="W78" s="26"/>
+      <c r="X78" s="34"/>
+      <c r="Y78" s="34"/>
+      <c r="Z78" s="34"/>
+      <c r="AA78" s="16"/>
+      <c r="AB78" s="16"/>
+      <c r="AC78" s="16"/>
+      <c r="AD78" s="16"/>
+      <c r="AE78" s="16"/>
+      <c r="AF78" s="36"/>
+      <c r="AG78" s="36"/>
+      <c r="AH78" s="36"/>
+      <c r="AI78" s="36"/>
+      <c r="AJ78" s="36"/>
+      <c r="AK78" s="36"/>
+      <c r="AL78" s="26"/>
+      <c r="AM78" s="26"/>
+      <c r="AN78" s="34"/>
+    </row>
+    <row r="79" spans="1:40">
+      <c r="A79" s="6">
+        <f>RiskTab22[[#This Row],[Nr.]]</f>
+        <v>79</v>
+      </c>
+      <c r="B79" s="53" t="str">
+        <f>RiskTab22[[#This Row],[Category]]</f>
+        <v>Cannabis AU</v>
+      </c>
+      <c r="C79" s="50" t="str">
+        <f>RiskTab22[[#This Row],[ShortName]]</f>
+        <v>Auscann</v>
+      </c>
+      <c r="D79" s="50" t="str">
+        <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
+        <v>ACNNF</v>
+      </c>
+      <c r="E79" s="23" t="str">
+        <f>Table2[[#This Row],[Volume]]</f>
+        <v/>
+      </c>
+      <c r="F79" s="32"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="16">
+        <f>Table2[[#This Row],[250D.logReturn]]</f>
+        <v>0</v>
+      </c>
+      <c r="K79" s="16"/>
+      <c r="L79" s="16">
+        <f>Table22[[#This Row],[250D.logReturn]]-Table22[[#This Row],[std_log_returns_1Y]]</f>
+        <v>0</v>
+      </c>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
+      <c r="S79" s="26"/>
+      <c r="T79" s="30"/>
+      <c r="U79" s="26"/>
+      <c r="V79" s="16"/>
+      <c r="W79" s="26"/>
+      <c r="X79" s="34"/>
+      <c r="Y79" s="34"/>
+      <c r="Z79" s="34"/>
+      <c r="AA79" s="16"/>
+      <c r="AB79" s="16"/>
+      <c r="AC79" s="16"/>
+      <c r="AD79" s="16"/>
+      <c r="AE79" s="16"/>
+      <c r="AF79" s="36"/>
+      <c r="AG79" s="36"/>
+      <c r="AH79" s="36"/>
+      <c r="AI79" s="36"/>
+      <c r="AJ79" s="36"/>
+      <c r="AK79" s="36"/>
+      <c r="AL79" s="26"/>
+      <c r="AM79" s="26"/>
+      <c r="AN79" s="34"/>
+    </row>
+    <row r="80" spans="1:40">
+      <c r="A80" s="6">
+        <f>RiskTab22[[#This Row],[Nr.]]</f>
+        <v>80</v>
+      </c>
+      <c r="B80" s="53" t="str">
+        <f>RiskTab22[[#This Row],[Category]]</f>
+        <v>Cannabis AU</v>
+      </c>
+      <c r="C80" s="50" t="str">
+        <f>RiskTab22[[#This Row],[ShortName]]</f>
+        <v>Cann Group</v>
+      </c>
+      <c r="D80" s="50" t="str">
+        <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
+        <v>CNGGF</v>
+      </c>
+      <c r="E80" s="23" t="str">
+        <f>Table2[[#This Row],[Volume]]</f>
+        <v/>
+      </c>
+      <c r="F80" s="32"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="16">
+        <f>Table2[[#This Row],[250D.logReturn]]</f>
+        <v>0</v>
+      </c>
+      <c r="K80" s="16"/>
+      <c r="L80" s="16">
+        <f>Table22[[#This Row],[250D.logReturn]]-Table22[[#This Row],[std_log_returns_1Y]]</f>
+        <v>0</v>
+      </c>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="26"/>
+      <c r="T80" s="30"/>
+      <c r="U80" s="26"/>
+      <c r="V80" s="16"/>
+      <c r="W80" s="26"/>
+      <c r="X80" s="34"/>
+      <c r="Y80" s="34"/>
+      <c r="Z80" s="34"/>
+      <c r="AA80" s="16"/>
+      <c r="AB80" s="16"/>
+      <c r="AC80" s="16"/>
+      <c r="AD80" s="16"/>
+      <c r="AE80" s="16"/>
+      <c r="AF80" s="36"/>
+      <c r="AG80" s="36"/>
+      <c r="AH80" s="36"/>
+      <c r="AI80" s="36"/>
+      <c r="AJ80" s="36"/>
+      <c r="AK80" s="36"/>
+      <c r="AL80" s="26"/>
+      <c r="AM80" s="26"/>
+      <c r="AN80" s="34"/>
+    </row>
+    <row r="81" spans="1:41">
+      <c r="A81" s="6">
+        <f>RiskTab22[[#This Row],[Nr.]]</f>
+        <v>81</v>
+      </c>
+      <c r="B81" s="53" t="str">
+        <f>RiskTab22[[#This Row],[Category]]</f>
+        <v>Cannabis AU</v>
+      </c>
+      <c r="C81" s="50" t="str">
+        <f>RiskTab22[[#This Row],[ShortName]]</f>
+        <v>Zelda Therapeutics</v>
+      </c>
+      <c r="D81" s="50" t="str">
+        <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
+        <v>ZLDAF</v>
+      </c>
+      <c r="E81" s="23" t="str">
+        <f>Table2[[#This Row],[Volume]]</f>
+        <v/>
+      </c>
+      <c r="F81" s="32"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="8"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="16">
+        <f>Table2[[#This Row],[250D.logReturn]]</f>
+        <v>0</v>
+      </c>
+      <c r="K81" s="16"/>
+      <c r="L81" s="16">
+        <f>Table22[[#This Row],[250D.logReturn]]-Table22[[#This Row],[std_log_returns_1Y]]</f>
+        <v>0</v>
+      </c>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+      <c r="S81" s="26"/>
+      <c r="T81" s="30"/>
+      <c r="U81" s="26"/>
+      <c r="V81" s="16"/>
+      <c r="W81" s="26"/>
+      <c r="X81" s="34"/>
+      <c r="Y81" s="34"/>
+      <c r="Z81" s="34"/>
+      <c r="AA81" s="16"/>
+      <c r="AB81" s="16"/>
+      <c r="AC81" s="16"/>
+      <c r="AD81" s="16"/>
+      <c r="AE81" s="16"/>
+      <c r="AF81" s="36"/>
+      <c r="AG81" s="36"/>
+      <c r="AH81" s="36"/>
+      <c r="AI81" s="36"/>
+      <c r="AJ81" s="36"/>
+      <c r="AK81" s="36"/>
+      <c r="AL81" s="26"/>
+      <c r="AM81" s="26"/>
+      <c r="AN81" s="34"/>
+    </row>
+    <row r="82" spans="1:41">
+      <c r="A82" s="6">
+        <f>RiskTab22[[#This Row],[Nr.]]</f>
+        <v>82</v>
+      </c>
+      <c r="B82" s="53" t="str">
+        <f>RiskTab22[[#This Row],[Category]]</f>
+        <v>Cannabis AU</v>
+      </c>
+      <c r="C82" s="50" t="str">
+        <f>RiskTab22[[#This Row],[ShortName]]</f>
+        <v>MMJ Group</v>
+      </c>
+      <c r="D82" s="50" t="str">
+        <f>RiskTab22[[#This Row],[AlphaVantage]]</f>
+        <v>MMJJF</v>
+      </c>
+      <c r="E82" s="23" t="str">
+        <f>Table2[[#This Row],[Volume]]</f>
+        <v/>
+      </c>
+      <c r="F82" s="32"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="16">
+        <f>Table2[[#This Row],[250D.logReturn]]</f>
+        <v>0</v>
+      </c>
+      <c r="K82" s="16"/>
+      <c r="L82" s="16">
+        <f>Table22[[#This Row],[250D.logReturn]]-Table22[[#This Row],[std_log_returns_1Y]]</f>
+        <v>0</v>
+      </c>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+      <c r="S82" s="26"/>
+      <c r="T82" s="30"/>
+      <c r="U82" s="26"/>
+      <c r="V82" s="16"/>
+      <c r="W82" s="26"/>
+      <c r="X82" s="34"/>
+      <c r="Y82" s="34"/>
+      <c r="Z82" s="34"/>
+      <c r="AA82" s="16"/>
+      <c r="AB82" s="16"/>
+      <c r="AC82" s="16"/>
+      <c r="AD82" s="16"/>
+      <c r="AE82" s="16"/>
+      <c r="AF82" s="36"/>
+      <c r="AG82" s="36"/>
+      <c r="AH82" s="36"/>
+      <c r="AI82" s="36"/>
+      <c r="AJ82" s="36"/>
+      <c r="AK82" s="36"/>
+      <c r="AL82" s="26"/>
+      <c r="AM82" s="26"/>
+      <c r="AN82" s="34"/>
+    </row>
+    <row r="83" spans="1:41">
+      <c r="B83" t="s">
         <v>23</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C83" t="s">
         <v>23</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D83" t="s">
         <v>190</v>
       </c>
-      <c r="E78">
+      <c r="E83">
         <v>67886.032783868606</v>
       </c>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
-      <c r="J78" s="16">
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" s="16">
         <v>0.55110331338949503</v>
       </c>
-      <c r="K78" s="18"/>
-      <c r="L78" s="18"/>
-      <c r="M78" s="18"/>
-      <c r="N78" s="23"/>
-      <c r="O78" s="23"/>
-      <c r="Q78" s="16">
+      <c r="K83" s="18"/>
+      <c r="L83" s="18"/>
+      <c r="M83" s="18"/>
+      <c r="N83" s="23"/>
+      <c r="O83" s="23"/>
+      <c r="Q83" s="16">
         <v>1.3354217318620101E-3</v>
       </c>
-      <c r="R78" s="1">
+      <c r="R83" s="1">
         <v>-5.6336557610431701E-2</v>
       </c>
-      <c r="Y78">
+      <c r="Y83">
         <v>-5.9217116694911302E-2</v>
       </c>
-      <c r="Z78">
+      <c r="Z83">
         <v>-4.4277518659525998E-2</v>
       </c>
-      <c r="AA78" s="35">
+      <c r="AA83" s="35">
         <v>-4.4585538270702801E-2</v>
       </c>
-      <c r="AB78" s="35"/>
-      <c r="AF78" s="37"/>
-      <c r="AG78" s="37"/>
-      <c r="AH78" s="37"/>
-      <c r="AI78" s="37"/>
-      <c r="AJ78" s="37"/>
-      <c r="AK78" s="37"/>
-      <c r="AL78" s="35">
+      <c r="AB83" s="35"/>
+      <c r="AF83" s="37"/>
+      <c r="AG83" s="37"/>
+      <c r="AH83" s="37"/>
+      <c r="AI83" s="37"/>
+      <c r="AJ83" s="37"/>
+      <c r="AK83" s="37"/>
+      <c r="AL83" s="35">
         <v>-6.4514020996561006E-2</v>
       </c>
-      <c r="AM78" s="35">
+      <c r="AM83" s="35">
         <v>-4.9519025494633398E-2</v>
       </c>
-      <c r="AN78" s="35">
+      <c r="AN83" s="35">
         <v>-5.6125117922182097E-2</v>
       </c>
-      <c r="AO78">
+      <c r="AO83">
         <v>-6.2674350059403194E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:41">
-      <c r="AF79" s="37"/>
-      <c r="AG79" s="37"/>
-      <c r="AH79" s="37"/>
-      <c r="AI79" s="37"/>
-      <c r="AJ79" s="37"/>
-      <c r="AK79" s="37"/>
+    <row r="84" spans="1:41">
+      <c r="AF84" s="37"/>
+      <c r="AG84" s="37"/>
+      <c r="AH84" s="37"/>
+      <c r="AI84" s="37"/>
+      <c r="AJ84" s="37"/>
+      <c r="AK84" s="37"/>
     </row>
-    <row r="80" spans="1:41">
-      <c r="AF80" s="37"/>
-      <c r="AG80" s="37"/>
-      <c r="AH80" s="37"/>
-      <c r="AI80" s="37"/>
-      <c r="AJ80" s="37"/>
-      <c r="AK80" s="37"/>
+    <row r="85" spans="1:41">
+      <c r="AF85" s="37"/>
+      <c r="AG85" s="37"/>
+      <c r="AH85" s="37"/>
+      <c r="AI85" s="37"/>
+      <c r="AJ85" s="37"/>
+      <c r="AK85" s="37"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="T1:T1048576">
@@ -37245,7 +37946,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q77">
+  <conditionalFormatting sqref="Q2:Q82">
     <cfRule type="dataBar" priority="286">
       <dataBar>
         <cfvo type="min"/>
@@ -37277,7 +37978,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S77">
+  <conditionalFormatting sqref="S2:S82">
     <cfRule type="colorScale" priority="289">
       <colorScale>
         <cfvo type="min"/>
@@ -37287,7 +37988,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R77">
+  <conditionalFormatting sqref="R2:R82">
     <cfRule type="dataBar" priority="290">
       <dataBar>
         <cfvo type="min"/>
@@ -37309,7 +38010,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P77">
+  <conditionalFormatting sqref="P2:P82">
     <cfRule type="dataBar" priority="292">
       <dataBar>
         <cfvo type="min"/>
@@ -37331,7 +38032,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:O77">
+  <conditionalFormatting sqref="N2:O82">
     <cfRule type="dataBar" priority="294">
       <dataBar>
         <cfvo type="min"/>
@@ -37353,7 +38054,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M77">
+  <conditionalFormatting sqref="M2:M82">
     <cfRule type="dataBar" priority="296">
       <dataBar>
         <cfvo type="min"/>
@@ -37375,7 +38076,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L77">
+  <conditionalFormatting sqref="L2:L82">
     <cfRule type="dataBar" priority="298">
       <dataBar>
         <cfvo type="min"/>
@@ -37399,7 +38100,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S77">
+  <conditionalFormatting sqref="S3:S82">
     <cfRule type="dataBar" priority="300">
       <dataBar>
         <cfvo type="min"/>
@@ -37413,7 +38114,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U77">
+  <conditionalFormatting sqref="U2:U82">
     <cfRule type="dataBar" priority="301">
       <dataBar>
         <cfvo type="min"/>
@@ -37427,7 +38128,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J77">
+  <conditionalFormatting sqref="J2:J82">
     <cfRule type="dataBar" priority="302">
       <dataBar>
         <cfvo type="min"/>
@@ -37441,7 +38142,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V77">
+  <conditionalFormatting sqref="V2:V82">
     <cfRule type="dataBar" priority="303">
       <dataBar>
         <cfvo type="min"/>
@@ -37455,7 +38156,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:AE77">
+  <conditionalFormatting sqref="AE2:AE82">
     <cfRule type="dataBar" priority="304">
       <dataBar>
         <cfvo type="min"/>
@@ -37553,7 +38254,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>Q2:Q77</xm:sqref>
+          <xm:sqref>Q2:Q82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{76A33C2D-0D4E-BD4A-88B2-5CADEC7DA0F6}">
@@ -37566,7 +38267,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>R2:R77</xm:sqref>
+          <xm:sqref>R2:R82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BBA4DEB2-38A5-6C48-B4D9-2A946689E8AB}">
@@ -37579,7 +38280,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>P2:P77</xm:sqref>
+          <xm:sqref>P2:P82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B6FCCB0D-7E44-A845-AFFA-0EC0043D5344}">
@@ -37592,7 +38293,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>N2:O77</xm:sqref>
+          <xm:sqref>N2:O82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{9A63E363-FD2A-CE44-87E0-A683832F68E9}">
@@ -37605,7 +38306,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M2:M77</xm:sqref>
+          <xm:sqref>M2:M82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{25D5B502-6233-FF45-A2DA-2DE77C1B4B6C}">
@@ -37616,7 +38317,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L2:L77</xm:sqref>
+          <xm:sqref>L2:L82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{7A34D4BD-97C9-D441-B06E-88A959E5D9C5}">
@@ -37629,7 +38330,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>S3:S77</xm:sqref>
+          <xm:sqref>S3:S82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{616B73C2-2917-634B-B70F-DA1ECAEB9ED7}">
@@ -37642,7 +38343,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U2:U77</xm:sqref>
+          <xm:sqref>U2:U82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A5020249-3882-6E47-A710-0D4D09B5187B}">
@@ -37653,7 +38354,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J2:J77</xm:sqref>
+          <xm:sqref>J2:J82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{024633CE-4398-F349-B97B-EC623F0C15FF}">
@@ -37666,7 +38367,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>V2:V77</xm:sqref>
+          <xm:sqref>V2:V82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{3FF8BC1E-F04E-3540-B626-ACFDFBFD15E3}">
@@ -37679,7 +38380,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>AE2:AE77</xm:sqref>
+          <xm:sqref>AE2:AE82</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -37692,10 +38393,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A10" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -38338,14 +39039,35 @@
         <v>105</v>
       </c>
     </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="41" t="s">
+        <v>418</v>
+      </c>
+      <c r="B38" s="46" t="s">
+        <v>417</v>
+      </c>
+      <c r="C38" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="41">
+        <v>43515</v>
+      </c>
+      <c r="E38" s="41">
+        <f>902.52/450</f>
+        <v>2.0055999999999998</v>
+      </c>
+      <c r="F38" s="42">
+        <v>450</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A10">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>